<commit_message>
vault backup: 2021-12-17 13:45:39
Affected files:
.obsidian/plugins/recent-files-obsidian/data.json
.obsidian/plugins/rss-reader/data.json
.vault-stats
1附件/权限列表.xlsx
Day Planners/Day Planner-20211210.md
</commit_message>
<xml_diff>
--- a/1附件/权限列表.xlsx
+++ b/1附件/权限列表.xlsx
@@ -5,22 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C4809A0-B502-B648-B622-2115CC5C372F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409FD91F-6416-7442-AA71-7ED50E125230}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="-1600" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mdm权限管理" sheetId="1" r:id="rId1"/>
-    <sheet name="Uniauth权限管理" sheetId="2" r:id="rId2"/>
-    <sheet name="App权限管理" sheetId="3" r:id="rId3"/>
-    <sheet name="运营权限管理" sheetId="4" r:id="rId4"/>
-    <sheet name="运维权限管理" sheetId="5" r:id="rId5"/>
-    <sheet name="安全审核权限管理" sheetId="6" r:id="rId6"/>
+    <sheet name="Mdm权限管理 (2)" sheetId="7" state="hidden" r:id="rId1"/>
+    <sheet name="新角色信息" sheetId="9" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="8" state="hidden" r:id="rId3"/>
+    <sheet name="Mdm权限管理" sheetId="1" r:id="rId4"/>
+    <sheet name="Uniauth权限管理" sheetId="2" r:id="rId5"/>
+    <sheet name="App权限管理" sheetId="3" r:id="rId6"/>
+    <sheet name="运营权限管理" sheetId="4" r:id="rId7"/>
+    <sheet name="运维权限管理" sheetId="5" r:id="rId8"/>
+    <sheet name="安全审核权限管理" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="413">
   <si>
     <t>首页面板</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1199,6 +1202,361 @@
   <si>
     <t>管理员</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户管理</t>
+  </si>
+  <si>
+    <t>组织机构</t>
+  </si>
+  <si>
+    <t>批量锁定设备</t>
+  </si>
+  <si>
+    <t>批量解锁设备</t>
+  </si>
+  <si>
+    <t>更改苹果规则</t>
+  </si>
+  <si>
+    <t>用户列表</t>
+  </si>
+  <si>
+    <t>用户分组</t>
+  </si>
+  <si>
+    <t>统一认证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>安全管控</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>审核系统</t>
+  </si>
+  <si>
+    <t>基础服务</t>
+  </si>
+  <si>
+    <t>首页面板</t>
+  </si>
+  <si>
+    <t>设备管理</t>
+  </si>
+  <si>
+    <t>安全策略</t>
+  </si>
+  <si>
+    <t>安全审计</t>
+  </si>
+  <si>
+    <t>资源管理</t>
+  </si>
+  <si>
+    <t>统计报表</t>
+  </si>
+  <si>
+    <t>日志管理</t>
+  </si>
+  <si>
+    <t>系统管理</t>
+  </si>
+  <si>
+    <t>全部类别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>子类别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读取</t>
+  </si>
+  <si>
+    <t>读取</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>子菜单</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>安卓设备管理</t>
+  </si>
+  <si>
+    <t>提取日志</t>
+  </si>
+  <si>
+    <t>解绑SIM卡</t>
+  </si>
+  <si>
+    <t>注册审核</t>
+  </si>
+  <si>
+    <t>批量通过</t>
+  </si>
+  <si>
+    <t>注册白名单</t>
+  </si>
+  <si>
+    <t>批量导入</t>
+  </si>
+  <si>
+    <t>安卓注册记录</t>
+  </si>
+  <si>
+    <t>锁定设备</t>
+  </si>
+  <si>
+    <t>解锁设备</t>
+  </si>
+  <si>
+    <t>锁定沙箱</t>
+  </si>
+  <si>
+    <t>解锁沙箱</t>
+  </si>
+  <si>
+    <t>发警报音</t>
+  </si>
+  <si>
+    <t>擦除数据</t>
+  </si>
+  <si>
+    <t>恢复数据</t>
+  </si>
+  <si>
+    <t>丢失</t>
+  </si>
+  <si>
+    <t>完全擦除</t>
+  </si>
+  <si>
+    <t>注销设备</t>
+  </si>
+  <si>
+    <t>刷新设备信息</t>
+  </si>
+  <si>
+    <t>定位</t>
+  </si>
+  <si>
+    <t>配置WLAN</t>
+  </si>
+  <si>
+    <t>外出</t>
+  </si>
+  <si>
+    <t>归队</t>
+  </si>
+  <si>
+    <t>重启设备</t>
+  </si>
+  <si>
+    <t>强制关机</t>
+  </si>
+  <si>
+    <t>验证证书</t>
+  </si>
+  <si>
+    <t>远程控制</t>
+  </si>
+  <si>
+    <t>获取实时运行数据</t>
+  </si>
+  <si>
+    <t>导出流量信息</t>
+  </si>
+  <si>
+    <t>删除应用</t>
+  </si>
+  <si>
+    <t>批量拒绝</t>
+  </si>
+  <si>
+    <t>通过</t>
+  </si>
+  <si>
+    <t>拒绝</t>
+  </si>
+  <si>
+    <t>删除</t>
+  </si>
+  <si>
+    <t>批量删除</t>
+  </si>
+  <si>
+    <t>安卓设备策略</t>
+  </si>
+  <si>
+    <t>停用</t>
+  </si>
+  <si>
+    <t>蓝牙白名单</t>
+  </si>
+  <si>
+    <t>批量导入蓝牙白名单</t>
+  </si>
+  <si>
+    <t>批量删除蓝牙白名单</t>
+  </si>
+  <si>
+    <t>添加蓝牙白名单</t>
+  </si>
+  <si>
+    <t>编辑蓝牙白名单</t>
+  </si>
+  <si>
+    <t>删除蓝牙白名单</t>
+  </si>
+  <si>
+    <t>安卓应用安装</t>
+  </si>
+  <si>
+    <t>安卓应用使用</t>
+  </si>
+  <si>
+    <t>安卓上网行为</t>
+  </si>
+  <si>
+    <t>安卓通话记录</t>
+  </si>
+  <si>
+    <t>导出通话记录</t>
+  </si>
+  <si>
+    <t>导出通话录音</t>
+  </si>
+  <si>
+    <t>播放通话录音</t>
+  </si>
+  <si>
+    <t>下载通话录音</t>
+  </si>
+  <si>
+    <t>安卓短信记录</t>
+  </si>
+  <si>
+    <t>安卓彩信记录</t>
+  </si>
+  <si>
+    <t>安卓微信聊天</t>
+  </si>
+  <si>
+    <t>导出会话</t>
+  </si>
+  <si>
+    <t>导出聊天记录</t>
+  </si>
+  <si>
+    <t>安卓QQ聊天</t>
+  </si>
+  <si>
+    <t>安卓敏感词</t>
+  </si>
+  <si>
+    <t>安卓违规状态记录</t>
+  </si>
+  <si>
+    <t>应用分发</t>
+  </si>
+  <si>
+    <t>文档管理</t>
+  </si>
+  <si>
+    <t>取消分发</t>
+  </si>
+  <si>
+    <t>敏感词库</t>
+  </si>
+  <si>
+    <t>用户统计</t>
+  </si>
+  <si>
+    <t>设备统计</t>
+  </si>
+  <si>
+    <t>安全统计</t>
+  </si>
+  <si>
+    <t>应用统计</t>
+  </si>
+  <si>
+    <t>网络统计</t>
+  </si>
+  <si>
+    <t>敏感词统计</t>
+  </si>
+  <si>
+    <t>流量统计</t>
+  </si>
+  <si>
+    <t>管理员操作日志</t>
+  </si>
+  <si>
+    <t>用户登录日志</t>
+  </si>
+  <si>
+    <t>设备日志</t>
+  </si>
+  <si>
+    <t>门禁出入记录</t>
+  </si>
+  <si>
+    <t>电子围栏出入记录</t>
+  </si>
+  <si>
+    <t>系统设置</t>
+  </si>
+  <si>
+    <t>保存注册设置</t>
+  </si>
+  <si>
+    <t>保存功能设置</t>
+  </si>
+  <si>
+    <t>保存SDK设置</t>
+  </si>
+  <si>
+    <t>移动门户设置</t>
+  </si>
+  <si>
+    <t>增加</t>
+  </si>
+  <si>
+    <t>预览</t>
+  </si>
+  <si>
+    <t>保存并推送</t>
+  </si>
+  <si>
+    <t>消息管理</t>
+  </si>
+  <si>
+    <t>安卓意见反馈</t>
+  </si>
+  <si>
+    <t>回复</t>
+  </si>
+  <si>
+    <t>忽略</t>
+  </si>
+  <si>
+    <t>报表下载</t>
+  </si>
+  <si>
+    <t>COPE客户端升级</t>
+  </si>
+  <si>
+    <t>关于系统</t>
+  </si>
+  <si>
+    <t>下载二维码</t>
   </si>
 </sst>
 </file>
@@ -1236,12 +1594,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1250,7 +1623,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1258,6 +1631,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1573,10 +1949,2986 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9952F6B7-2F1C-7444-A3F5-DE47C9B48272}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:R74"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B57" sqref="B57:I74"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="2" customFormat="1">
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="2" customFormat="1">
+      <c r="E11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="2" customFormat="1">
+      <c r="E12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="1" customFormat="1">
+      <c r="C13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="1" customFormat="1">
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="1" customFormat="1"/>
+    <row r="16" spans="1:18">
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="C20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" s="1" customFormat="1">
+      <c r="C21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" s="1" customFormat="1">
+      <c r="C24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" s="1" customFormat="1">
+      <c r="D25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" s="1" customFormat="1">
+      <c r="C26" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" s="1" customFormat="1">
+      <c r="D27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12">
+      <c r="C28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12">
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29" t="s">
+        <v>69</v>
+      </c>
+      <c r="I29" t="s">
+        <v>70</v>
+      </c>
+      <c r="J29" t="s">
+        <v>71</v>
+      </c>
+      <c r="K29" t="s">
+        <v>73</v>
+      </c>
+      <c r="L29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" s="1" customFormat="1">
+      <c r="C31" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12">
+      <c r="C32" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="C33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="C34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>77</v>
+      </c>
+      <c r="G34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="C36" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="C37" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>75</v>
+      </c>
+      <c r="G37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="C38" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="C40" t="s">
+        <v>137</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>83</v>
+      </c>
+      <c r="G40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="C42" t="s">
+        <v>138</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10">
+      <c r="C43" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10">
+      <c r="B44" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" t="s">
+        <v>86</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="C46" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" t="s">
+        <v>60</v>
+      </c>
+      <c r="H47" t="s">
+        <v>59</v>
+      </c>
+      <c r="I47" t="s">
+        <v>8</v>
+      </c>
+      <c r="J47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10">
+      <c r="C48" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9">
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" t="s">
+        <v>57</v>
+      </c>
+      <c r="F49" t="s">
+        <v>59</v>
+      </c>
+      <c r="G49" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" t="s">
+        <v>60</v>
+      </c>
+      <c r="I49" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9">
+      <c r="B50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9">
+      <c r="C51" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>1</v>
+      </c>
+      <c r="F51" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9">
+      <c r="C52" t="s">
+        <v>94</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9">
+      <c r="C53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9">
+      <c r="C54" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9">
+      <c r="C55" t="s">
+        <v>97</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
+        <v>1</v>
+      </c>
+      <c r="F55" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9">
+      <c r="C56" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9">
+      <c r="B57" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" t="s">
+        <v>99</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9">
+      <c r="C58" t="s">
+        <v>100</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9">
+      <c r="C59" t="s">
+        <v>101</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1</v>
+      </c>
+      <c r="E59" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9">
+      <c r="C60" t="s">
+        <v>102</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9">
+      <c r="C61" t="s">
+        <v>103</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9">
+      <c r="B62" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" t="s">
+        <v>105</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9">
+      <c r="D63" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" t="s">
+        <v>106</v>
+      </c>
+      <c r="F63" t="s">
+        <v>107</v>
+      </c>
+      <c r="G63" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9">
+      <c r="C64" t="s">
+        <v>109</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8">
+      <c r="D65" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" t="s">
+        <v>110</v>
+      </c>
+      <c r="F65" t="s">
+        <v>111</v>
+      </c>
+      <c r="G65" t="s">
+        <v>60</v>
+      </c>
+      <c r="H65" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8">
+      <c r="C66" t="s">
+        <v>113</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8" ht="30" customHeight="1">
+      <c r="C67" t="s">
+        <v>140</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8">
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" t="s">
+        <v>114</v>
+      </c>
+      <c r="F68" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="69" spans="3:8" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="C69" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="3:8" s="1" customFormat="1">
+      <c r="D70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8">
+      <c r="C71" t="s">
+        <v>116</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="3:8">
+      <c r="C72" t="s">
+        <v>117</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1</v>
+      </c>
+      <c r="E72" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" s="1" customFormat="1">
+      <c r="C73" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8">
+      <c r="C74" t="s">
+        <v>118</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
+        <v>1</v>
+      </c>
+      <c r="F74" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D0B293-1DEC-F94F-A0DE-99D6257050F6}">
+  <dimension ref="A1:K213"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J100" sqref="J100"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="2"/>
+  <cols>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" outlineLevel="1">
+      <c r="B5" t="s">
+        <v>308</v>
+      </c>
+      <c r="F5" t="s">
+        <v>308</v>
+      </c>
+      <c r="G5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" hidden="1" outlineLevel="2">
+      <c r="G6" t="s">
+        <v>318</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" hidden="1" outlineLevel="2">
+      <c r="G7" t="s">
+        <v>318</v>
+      </c>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" outlineLevel="1" collapsed="1">
+      <c r="B8" t="s">
+        <v>297</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" hidden="1" outlineLevel="2">
+      <c r="G9" t="s">
+        <v>318</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" hidden="1" outlineLevel="2">
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" hidden="1" outlineLevel="2">
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" hidden="1" outlineLevel="2">
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" hidden="1" outlineLevel="2">
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" hidden="1" outlineLevel="2">
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" hidden="1" outlineLevel="2">
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" hidden="1" outlineLevel="2">
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F17" t="s">
+        <v>297</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G18" t="s">
+        <v>318</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F24" t="s">
+        <v>297</v>
+      </c>
+      <c r="G24" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="15" hidden="1" customHeight="1" outlineLevel="2">
+      <c r="G25" t="s">
+        <v>318</v>
+      </c>
+      <c r="H25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="B31" t="s">
+        <v>309</v>
+      </c>
+      <c r="F31" t="s">
+        <v>309</v>
+      </c>
+      <c r="G31" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G32" t="s">
+        <v>318</v>
+      </c>
+      <c r="H32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G34" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="35" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G35" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="36" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G36" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="37" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="39" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="40" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="41" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G41" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="42" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G42" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="43" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G43" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="44" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G44" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="45" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G45" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="46" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G46" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="47" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G47" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="48" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G48" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="49" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G49" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="50" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="51" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G51" t="s">
+        <v>7</v>
+      </c>
+      <c r="H51" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="52" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G52" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="53" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G53" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="54" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G54" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="55" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G55" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="56" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G57" t="s">
+        <v>7</v>
+      </c>
+      <c r="H57" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="58" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G58" t="s">
+        <v>7</v>
+      </c>
+      <c r="H58" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G59" t="s">
+        <v>7</v>
+      </c>
+      <c r="H59" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="60" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G60" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G61" t="s">
+        <v>7</v>
+      </c>
+      <c r="H61" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="62" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G62" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G63" t="s">
+        <v>7</v>
+      </c>
+      <c r="H63" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="64" spans="7:8" hidden="1" outlineLevel="2">
+      <c r="G64" t="s">
+        <v>7</v>
+      </c>
+      <c r="H64" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F65" t="s">
+        <v>309</v>
+      </c>
+      <c r="G65" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="66" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G66" t="s">
+        <v>1</v>
+      </c>
+      <c r="H66" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G67" t="s">
+        <v>7</v>
+      </c>
+      <c r="H67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G68" t="s">
+        <v>7</v>
+      </c>
+      <c r="H68" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="69" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G69" t="s">
+        <v>7</v>
+      </c>
+      <c r="H69" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="70" spans="6:8" ht="1" hidden="1" outlineLevel="2">
+      <c r="G70" t="s">
+        <v>7</v>
+      </c>
+      <c r="H70" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="71" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G71" t="s">
+        <v>7</v>
+      </c>
+      <c r="H71" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="72" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F72" t="s">
+        <v>309</v>
+      </c>
+      <c r="G72" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="73" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G73" t="s">
+        <v>1</v>
+      </c>
+      <c r="H73" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G74" t="s">
+        <v>7</v>
+      </c>
+      <c r="H74" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="75" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G75" t="s">
+        <v>7</v>
+      </c>
+      <c r="H75" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="76" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G76" t="s">
+        <v>7</v>
+      </c>
+      <c r="H76" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G77" t="s">
+        <v>7</v>
+      </c>
+      <c r="H77" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="78" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G78" t="s">
+        <v>7</v>
+      </c>
+      <c r="H78" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="79" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F79" t="s">
+        <v>309</v>
+      </c>
+      <c r="G79" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="80" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G80" t="s">
+        <v>1</v>
+      </c>
+      <c r="H80" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="B81" t="s">
+        <v>310</v>
+      </c>
+      <c r="F81" t="s">
+        <v>310</v>
+      </c>
+      <c r="G81" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G82" t="s">
+        <v>1</v>
+      </c>
+      <c r="H82" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G83" t="s">
+        <v>7</v>
+      </c>
+      <c r="H83" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G84" t="s">
+        <v>7</v>
+      </c>
+      <c r="H84" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G85" t="s">
+        <v>7</v>
+      </c>
+      <c r="H85" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G86" t="s">
+        <v>7</v>
+      </c>
+      <c r="H86" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F87" t="s">
+        <v>310</v>
+      </c>
+      <c r="G87" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G88" t="s">
+        <v>1</v>
+      </c>
+      <c r="H88" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G89" t="s">
+        <v>7</v>
+      </c>
+      <c r="H89" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G90" t="s">
+        <v>7</v>
+      </c>
+      <c r="H90" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G91" t="s">
+        <v>7</v>
+      </c>
+      <c r="H91" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G92" t="s">
+        <v>7</v>
+      </c>
+      <c r="H92" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G93" t="s">
+        <v>7</v>
+      </c>
+      <c r="H93" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G94" t="s">
+        <v>7</v>
+      </c>
+      <c r="H94" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G95" t="s">
+        <v>7</v>
+      </c>
+      <c r="H95" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G96" t="s">
+        <v>7</v>
+      </c>
+      <c r="H96" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="B97" t="s">
+        <v>311</v>
+      </c>
+      <c r="F97" t="s">
+        <v>311</v>
+      </c>
+      <c r="G97" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G98" t="s">
+        <v>1</v>
+      </c>
+      <c r="H98" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G99" t="s">
+        <v>1</v>
+      </c>
+      <c r="H99" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F100" t="s">
+        <v>311</v>
+      </c>
+      <c r="G100" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G101" t="s">
+        <v>1</v>
+      </c>
+      <c r="H101" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G102" t="s">
+        <v>1</v>
+      </c>
+      <c r="H102" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F103" t="s">
+        <v>311</v>
+      </c>
+      <c r="G103" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G104" t="s">
+        <v>1</v>
+      </c>
+      <c r="H104" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G105" t="s">
+        <v>1</v>
+      </c>
+      <c r="H105" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F106" t="s">
+        <v>311</v>
+      </c>
+      <c r="G106" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G107" t="s">
+        <v>1</v>
+      </c>
+      <c r="H107" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G108" t="s">
+        <v>1</v>
+      </c>
+      <c r="H108" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="109" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G109" t="s">
+        <v>1</v>
+      </c>
+      <c r="H109" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G110" t="s">
+        <v>1</v>
+      </c>
+      <c r="H110" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G111" t="s">
+        <v>1</v>
+      </c>
+      <c r="H111" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G112" t="s">
+        <v>1</v>
+      </c>
+      <c r="H112" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="113" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F113" t="s">
+        <v>311</v>
+      </c>
+      <c r="G113" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="114" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G114" t="s">
+        <v>1</v>
+      </c>
+      <c r="H114" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G115" t="s">
+        <v>1</v>
+      </c>
+      <c r="H115" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="116" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F116" t="s">
+        <v>311</v>
+      </c>
+      <c r="G116" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="117" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G117" t="s">
+        <v>1</v>
+      </c>
+      <c r="H117" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G118" t="s">
+        <v>1</v>
+      </c>
+      <c r="H118" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="119" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G119" t="s">
+        <v>1</v>
+      </c>
+      <c r="H119" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F120" t="s">
+        <v>311</v>
+      </c>
+      <c r="G120" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="121" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G121" t="s">
+        <v>1</v>
+      </c>
+      <c r="H121" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G122" t="s">
+        <v>1</v>
+      </c>
+      <c r="H122" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="123" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G123" t="s">
+        <v>1</v>
+      </c>
+      <c r="H123" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="124" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G124" t="s">
+        <v>1</v>
+      </c>
+      <c r="H124" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="125" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G125" t="s">
+        <v>1</v>
+      </c>
+      <c r="H125" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="126" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G126" t="s">
+        <v>1</v>
+      </c>
+      <c r="H126" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F127" t="s">
+        <v>311</v>
+      </c>
+      <c r="G127" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="128" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G128" t="s">
+        <v>1</v>
+      </c>
+      <c r="H128" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G129" t="s">
+        <v>1</v>
+      </c>
+      <c r="H129" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="130" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G130" t="s">
+        <v>1</v>
+      </c>
+      <c r="H130" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="131" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G131" t="s">
+        <v>1</v>
+      </c>
+      <c r="H131" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="132" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G132" t="s">
+        <v>1</v>
+      </c>
+      <c r="H132" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="133" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G133" t="s">
+        <v>1</v>
+      </c>
+      <c r="H133" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F134" t="s">
+        <v>311</v>
+      </c>
+      <c r="G134" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="135" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G135" t="s">
+        <v>1</v>
+      </c>
+      <c r="H135" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G136" t="s">
+        <v>1</v>
+      </c>
+      <c r="H136" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="137" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F137" t="s">
+        <v>311</v>
+      </c>
+      <c r="G137" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="138" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G138" t="s">
+        <v>1</v>
+      </c>
+      <c r="H138" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G139" t="s">
+        <v>1</v>
+      </c>
+      <c r="H139" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="140" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="B140" t="s">
+        <v>312</v>
+      </c>
+      <c r="F140" t="s">
+        <v>312</v>
+      </c>
+      <c r="G140" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="141" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G141" t="s">
+        <v>1</v>
+      </c>
+      <c r="H141" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G142" t="s">
+        <v>7</v>
+      </c>
+      <c r="H142" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="143" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F143" t="s">
+        <v>312</v>
+      </c>
+      <c r="G143" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="144" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G144" t="s">
+        <v>1</v>
+      </c>
+      <c r="H144" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G145" t="s">
+        <v>7</v>
+      </c>
+      <c r="H145" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="146" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G146" t="s">
+        <v>7</v>
+      </c>
+      <c r="H146" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G147" t="s">
+        <v>7</v>
+      </c>
+      <c r="H147" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="148" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G148" t="s">
+        <v>7</v>
+      </c>
+      <c r="H148" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="149" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G149" t="s">
+        <v>7</v>
+      </c>
+      <c r="H149" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="150" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G150" t="s">
+        <v>7</v>
+      </c>
+      <c r="H150" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="151" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F151" t="s">
+        <v>312</v>
+      </c>
+      <c r="G151" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="152" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G152" t="s">
+        <v>1</v>
+      </c>
+      <c r="H152" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="153" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G153" t="s">
+        <v>7</v>
+      </c>
+      <c r="H153" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="154" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G154" t="s">
+        <v>7</v>
+      </c>
+      <c r="H154" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="155" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G155" t="s">
+        <v>7</v>
+      </c>
+      <c r="H155" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="156" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="B156" t="s">
+        <v>313</v>
+      </c>
+      <c r="F156" t="s">
+        <v>313</v>
+      </c>
+      <c r="G156" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="157" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G157" t="s">
+        <v>1</v>
+      </c>
+      <c r="H157" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G158" t="s">
+        <v>1</v>
+      </c>
+      <c r="H158" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="159" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F159" t="s">
+        <v>313</v>
+      </c>
+      <c r="G159" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="160" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G160" t="s">
+        <v>1</v>
+      </c>
+      <c r="H160" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G161" t="s">
+        <v>1</v>
+      </c>
+      <c r="H161" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="162" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F162" t="s">
+        <v>313</v>
+      </c>
+      <c r="G162" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="163" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G163" t="s">
+        <v>1</v>
+      </c>
+      <c r="H163" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G164" t="s">
+        <v>1</v>
+      </c>
+      <c r="H164" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="165" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F165" t="s">
+        <v>313</v>
+      </c>
+      <c r="G165" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="166" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G166" t="s">
+        <v>1</v>
+      </c>
+      <c r="H166" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G167" t="s">
+        <v>1</v>
+      </c>
+      <c r="H167" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="168" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F168" t="s">
+        <v>313</v>
+      </c>
+      <c r="G168" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="169" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G169" t="s">
+        <v>1</v>
+      </c>
+      <c r="H169" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G170" t="s">
+        <v>1</v>
+      </c>
+      <c r="H170" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="171" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F171" t="s">
+        <v>313</v>
+      </c>
+      <c r="G171" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="172" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G172" t="s">
+        <v>1</v>
+      </c>
+      <c r="H172" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G173" t="s">
+        <v>1</v>
+      </c>
+      <c r="H173" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="174" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F174" t="s">
+        <v>313</v>
+      </c>
+      <c r="G174" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="175" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G175" t="s">
+        <v>1</v>
+      </c>
+      <c r="H175" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G176" t="s">
+        <v>1</v>
+      </c>
+      <c r="H176" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="177" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="B177" t="s">
+        <v>314</v>
+      </c>
+      <c r="F177" t="s">
+        <v>314</v>
+      </c>
+      <c r="G177" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="178" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G178" t="s">
+        <v>1</v>
+      </c>
+      <c r="H178" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F179" t="s">
+        <v>314</v>
+      </c>
+      <c r="G179" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="180" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G180" t="s">
+        <v>1</v>
+      </c>
+      <c r="H180" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F181" t="s">
+        <v>314</v>
+      </c>
+      <c r="G181" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="182" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G182" t="s">
+        <v>1</v>
+      </c>
+      <c r="H182" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F183" t="s">
+        <v>314</v>
+      </c>
+      <c r="G183" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="184" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G184" t="s">
+        <v>1</v>
+      </c>
+      <c r="H184" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F185" t="s">
+        <v>314</v>
+      </c>
+      <c r="G185" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="186" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G186" t="s">
+        <v>1</v>
+      </c>
+      <c r="H186" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="B187" t="s">
+        <v>315</v>
+      </c>
+      <c r="F187" t="s">
+        <v>315</v>
+      </c>
+      <c r="G187" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="188" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G188" t="s">
+        <v>1</v>
+      </c>
+      <c r="H188" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G189" t="s">
+        <v>7</v>
+      </c>
+      <c r="H189" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="190" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G190" t="s">
+        <v>7</v>
+      </c>
+      <c r="H190" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="191" spans="2:8" hidden="1" outlineLevel="2">
+      <c r="G191" t="s">
+        <v>7</v>
+      </c>
+      <c r="H191" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="192" spans="2:8" outlineLevel="1" collapsed="1">
+      <c r="F192" t="s">
+        <v>315</v>
+      </c>
+      <c r="G192" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="193" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G193" t="s">
+        <v>1</v>
+      </c>
+      <c r="H193" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G194" t="s">
+        <v>7</v>
+      </c>
+      <c r="H194" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="195" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G195" t="s">
+        <v>7</v>
+      </c>
+      <c r="H195" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="196" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G196" t="s">
+        <v>7</v>
+      </c>
+      <c r="H196" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="197" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G197" t="s">
+        <v>7</v>
+      </c>
+      <c r="H197" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="198" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F198" t="s">
+        <v>315</v>
+      </c>
+      <c r="G198" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="199" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G199" t="s">
+        <v>1</v>
+      </c>
+      <c r="H199" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F200" t="s">
+        <v>315</v>
+      </c>
+      <c r="G200" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="201" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G201" t="s">
+        <v>1</v>
+      </c>
+      <c r="H201" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G202" t="s">
+        <v>7</v>
+      </c>
+      <c r="H202" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="203" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G203" t="s">
+        <v>7</v>
+      </c>
+      <c r="H203" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="204" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F204" t="s">
+        <v>315</v>
+      </c>
+      <c r="G204" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="205" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G205" t="s">
+        <v>1</v>
+      </c>
+      <c r="H205" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F206" t="s">
+        <v>315</v>
+      </c>
+      <c r="G206" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="207" spans="6:8" hidden="1" outlineLevel="2">
+      <c r="G207" t="s">
+        <v>1</v>
+      </c>
+      <c r="H207" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="6:8" outlineLevel="1" collapsed="1">
+      <c r="F208" t="s">
+        <v>315</v>
+      </c>
+      <c r="G208" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" hidden="1" outlineLevel="2">
+      <c r="G209" t="s">
+        <v>1</v>
+      </c>
+      <c r="H209" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" hidden="1" outlineLevel="2">
+      <c r="G210" t="s">
+        <v>1</v>
+      </c>
+      <c r="H210" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" outlineLevel="1" collapsed="1"/>
+    <row r="212" spans="1:8">
+      <c r="A212" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8">
+      <c r="A213" t="s">
+        <v>307</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A55561D-0015-464D-BFB1-1E3382BADF08}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" outlineLevel="1">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" outlineLevel="1">
+      <c r="C4">
+        <v>111</v>
+      </c>
+      <c r="D4">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" outlineLevel="1">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>299</v>
+      </c>
+      <c r="H5" t="s">
+        <v>300</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="B6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" hidden="1" outlineLevel="1">
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" hidden="1" outlineLevel="1">
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" collapsed="1">
+      <c r="B9" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" hidden="1" outlineLevel="1">
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" collapsed="1"/>
+  </sheetData>
+  <dataConsolidate/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754B3636-7394-6344-94B9-FC95971C758A}">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>
@@ -2670,11 +6022,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85160F0E-AAA4-2440-88EE-EDE07CD3F226}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
@@ -3264,7 +6616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC44C7D-B5C9-8244-8110-B919A147507E}">
   <dimension ref="A1:I22"/>
   <sheetViews>
@@ -3594,7 +6946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B3B789-6212-894F-BA86-A23B372BEE33}">
   <dimension ref="A1:G22"/>
   <sheetViews>
@@ -3890,7 +7242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F9AB08-A3B8-514B-AD13-E0375A045A1B}">
   <dimension ref="A1:G36"/>
   <sheetViews>
@@ -4338,7 +7690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89C31BD-9216-6A49-8C90-0ADAF2498DB4}">
   <dimension ref="A1:D14"/>
   <sheetViews>

</xml_diff>

<commit_message>
vault backup: 2021-12-31 15:26:00
Affected files:
1附件/~$权限列表.xlsx
1附件/权限列表.xlsx
</commit_message>
<xml_diff>
--- a/1附件/权限列表.xlsx
+++ b/1附件/权限列表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409FD91F-6416-7442-AA71-7ED50E125230}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0A7033-0759-C944-962D-95D012C0C541}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-1600" windowWidth="35840" windowHeight="22400" activeTab="1" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
+    <workbookView xWindow="880" yWindow="0" windowWidth="18760" windowHeight="21600" activeTab="3" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Mdm权限管理 (2)" sheetId="7" state="hidden" r:id="rId1"/>
@@ -3058,7 +3058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D0B293-1DEC-F94F-A0DE-99D6257050F6}">
   <dimension ref="A1:K213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J100" sqref="J100"/>
     </sheetView>
@@ -3644,7 +3644,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="70" spans="6:8" ht="1" hidden="1" outlineLevel="2">
+    <row r="70" spans="6:8" hidden="1" outlineLevel="2">
       <c r="G70" t="s">
         <v>7</v>
       </c>
@@ -4926,10 +4926,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754B3636-7394-6344-94B9-FC95971C758A}">
-  <dimension ref="A1:Q73"/>
+  <dimension ref="A2:Q74"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="G102" sqref="G102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4943,517 +4943,503 @@
     <col min="17" max="17" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
       <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
-      <c r="B4" t="s">
+    <row r="5" spans="1:17">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
       <c r="C5" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G6" t="s">
         <v>17</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
-      <c r="B6" t="s">
+    <row r="7" spans="1:17">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
       <c r="C7" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
         <v>17</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
-      <c r="A8" t="s">
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>121</v>
       </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" s="2" customFormat="1">
-      <c r="C9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="2" customFormat="1">
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="Q10" s="2" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" s="2" customFormat="1">
-      <c r="D10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="2" customFormat="1">
       <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="2" customFormat="1">
+      <c r="D12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="1" customFormat="1">
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:17" s="1" customFormat="1">
+      <c r="B13" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" s="1" customFormat="1">
       <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" s="1" customFormat="1"/>
-    <row r="15" spans="1:17">
-      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" s="1" customFormat="1">
+      <c r="C14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" s="1" customFormat="1"/>
+    <row r="16" spans="1:17">
+      <c r="B16" t="s">
         <v>51</v>
       </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
       <c r="C16" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
         <v>52</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>53</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>54</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
-      <c r="B17" t="s">
+    <row r="18" spans="1:11">
+      <c r="B18" t="s">
         <v>56</v>
       </c>
-      <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
       <c r="C18" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
         <v>57</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>59</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>8</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>60</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
-      <c r="B19" t="s">
+    <row r="20" spans="1:11">
+      <c r="B20" t="s">
         <v>124</v>
       </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="1" customFormat="1">
-      <c r="B20" s="1" t="s">
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="1" customFormat="1">
+      <c r="B21" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" t="s">
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
         <v>61</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>126</v>
       </c>
-      <c r="C21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
       <c r="C22" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
         <v>63</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>58</v>
       </c>
-      <c r="F22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="1" customFormat="1">
-      <c r="B23" s="1" t="s">
+    <row r="24" spans="1:11" s="1" customFormat="1">
+      <c r="B24" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="1" customFormat="1">
       <c r="C24" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="1" customFormat="1">
+      <c r="C25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="1" t="s">
+      <c r="F25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="1" customFormat="1">
-      <c r="B25" s="1" t="s">
+    <row r="26" spans="1:11" s="1" customFormat="1">
+      <c r="B26" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="1" customFormat="1">
       <c r="C26" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="1" customFormat="1">
+      <c r="C27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
-      <c r="B27" t="s">
+    <row r="28" spans="1:11">
+      <c r="B28" t="s">
         <v>65</v>
       </c>
-      <c r="C27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
       <c r="C28" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
         <v>66</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>67</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>68</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>69</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H29" t="s">
         <v>70</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I29" t="s">
         <v>71</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J29" t="s">
         <v>73</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
-      <c r="A29" t="s">
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
         <v>74</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>129</v>
       </c>
-      <c r="C29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="1" customFormat="1">
-      <c r="B30" s="1" t="s">
+    <row r="31" spans="1:11" s="1" customFormat="1">
+      <c r="B31" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="C31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="B31" t="s">
-        <v>131</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="B32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
@@ -5467,49 +5453,49 @@
     </row>
     <row r="33" spans="1:9">
       <c r="B33" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="B34" t="s">
         <v>133</v>
       </c>
-      <c r="C33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
         <v>77</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F34" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
+    <row r="35" spans="1:9">
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
         <v>79</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="B35" t="s">
-        <v>134</v>
-      </c>
-      <c r="C35" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" t="s">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="B36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -5520,83 +5506,83 @@
       <c r="E36" t="s">
         <v>75</v>
       </c>
-      <c r="F36" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="37" spans="1:9">
       <c r="B37" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="B38" t="s">
         <v>136</v>
       </c>
-      <c r="C37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
         <v>83</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F38" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
-      <c r="C38" t="s">
+    <row r="39" spans="1:9">
+      <c r="C39" t="s">
         <v>8</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>82</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
-      <c r="B39" t="s">
+    <row r="40" spans="1:9">
+      <c r="B40" t="s">
         <v>137</v>
       </c>
-      <c r="C39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
         <v>83</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
-      <c r="C40" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" t="s">
+    <row r="41" spans="1:9">
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
         <v>81</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="B41" t="s">
-        <v>138</v>
-      </c>
-      <c r="C41" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="B42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
@@ -5609,126 +5595,126 @@
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
         <v>85</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>86</v>
       </c>
-      <c r="C43" t="s">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
       <c r="C44" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
-      <c r="B45" t="s">
+    <row r="46" spans="1:9">
+      <c r="B46" t="s">
         <v>87</v>
       </c>
-      <c r="C45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D45" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
       <c r="C46" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
         <v>62</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E47" t="s">
         <v>4</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F47" t="s">
         <v>60</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G47" t="s">
         <v>59</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H47" t="s">
         <v>8</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I47" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
-      <c r="B47" t="s">
+    <row r="48" spans="1:9">
+      <c r="B48" t="s">
         <v>89</v>
       </c>
-      <c r="C47" t="s">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
       <c r="C48" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D48" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
         <v>57</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>59</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F49" t="s">
         <v>8</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G49" t="s">
         <v>60</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H49" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
-      <c r="A49" t="s">
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
         <v>90</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>91</v>
       </c>
-      <c r="C49" t="s">
-        <v>1</v>
-      </c>
-      <c r="D49" t="s">
-        <v>1</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="C50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
-      <c r="B50" t="s">
+    <row r="51" spans="1:8">
+      <c r="B51" t="s">
         <v>93</v>
-      </c>
-      <c r="C50" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" t="s">
-        <v>1</v>
-      </c>
-      <c r="E50" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="B51" t="s">
-        <v>94</v>
       </c>
       <c r="C51" t="s">
         <v>1</v>
@@ -5740,9 +5726,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:8">
       <c r="B52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C52" t="s">
         <v>1</v>
@@ -5754,9 +5740,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:8">
       <c r="B53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C53" t="s">
         <v>1</v>
@@ -5768,9 +5754,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:8">
       <c r="B54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C54" t="s">
         <v>1</v>
@@ -5782,9 +5768,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:8">
       <c r="B55" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C55" t="s">
         <v>1</v>
@@ -5796,222 +5782,236 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
-      <c r="A56" t="s">
+    <row r="56" spans="1:8">
+      <c r="B56" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
         <v>98</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>99</v>
       </c>
-      <c r="C56" t="s">
-        <v>1</v>
-      </c>
-      <c r="D56" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="B57" t="s">
+      <c r="C57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="B58" t="s">
         <v>100</v>
       </c>
-      <c r="C57" t="s">
-        <v>1</v>
-      </c>
-      <c r="D57" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="B58" t="s">
+      <c r="C58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="B59" t="s">
         <v>101</v>
       </c>
-      <c r="C58" t="s">
-        <v>1</v>
-      </c>
-      <c r="D58" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="B60" t="s">
         <v>102</v>
       </c>
-      <c r="C59" t="s">
-        <v>1</v>
-      </c>
-      <c r="D59" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="B60" t="s">
+      <c r="C60" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="B61" t="s">
         <v>103</v>
       </c>
-      <c r="C60" t="s">
-        <v>1</v>
-      </c>
-      <c r="D60" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" t="s">
+      <c r="C61" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
         <v>104</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>105</v>
       </c>
-      <c r="C61" t="s">
-        <v>1</v>
-      </c>
-      <c r="D61" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
       <c r="C62" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D62" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
         <v>106</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E63" t="s">
         <v>107</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F63" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
-      <c r="B63" t="s">
+    <row r="64" spans="1:8">
+      <c r="B64" t="s">
         <v>109</v>
       </c>
-      <c r="C63" t="s">
-        <v>1</v>
-      </c>
-      <c r="D63" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
       <c r="C64" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7">
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" t="s">
         <v>110</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E65" t="s">
         <v>111</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F65" t="s">
         <v>60</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G65" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="2:5">
-      <c r="B65" t="s">
+    <row r="66" spans="2:7">
+      <c r="B66" t="s">
         <v>113</v>
       </c>
-      <c r="C65" t="s">
-        <v>1</v>
-      </c>
-      <c r="D65" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" ht="30" customHeight="1">
-      <c r="B66" t="s">
+      <c r="C66" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="30" customHeight="1">
+      <c r="B67" t="s">
         <v>140</v>
       </c>
-      <c r="C66" t="s">
-        <v>1</v>
-      </c>
-      <c r="D66" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5">
       <c r="C67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7">
+      <c r="C68" t="s">
         <v>8</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" t="s">
         <v>114</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E68" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="68" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="B68" s="1" t="s">
+    <row r="69" spans="2:7" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="B69" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" s="1" customFormat="1">
       <c r="C69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" s="1" customFormat="1">
+      <c r="C70" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D70" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E70" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="2:5">
-      <c r="B70" t="s">
+    <row r="71" spans="2:7">
+      <c r="B71" t="s">
         <v>116</v>
       </c>
-      <c r="C70" t="s">
-        <v>1</v>
-      </c>
-      <c r="D70" t="s">
-        <v>1</v>
-      </c>
-      <c r="E70" t="s">
+      <c r="C71" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="2:5">
-      <c r="B71" t="s">
+    <row r="72" spans="2:7">
+      <c r="B72" t="s">
         <v>117</v>
       </c>
-      <c r="C71" t="s">
-        <v>1</v>
-      </c>
-      <c r="D71" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" s="1" customFormat="1">
-      <c r="B72" s="1" t="s">
+      <c r="C72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" s="1" customFormat="1">
+      <c r="B73" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5">
-      <c r="B73" t="s">
+      <c r="C73" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7">
+      <c r="B74" t="s">
         <v>118</v>
       </c>
-      <c r="C73" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" t="s">
-        <v>1</v>
-      </c>
-      <c r="E73" t="s">
+      <c r="C74" t="s">
+        <v>1</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
         <v>119</v>
       </c>
     </row>

</xml_diff>

<commit_message>
vault backup: 2022-01-04 14:58:32
Affected files:
.obsidian/plugins/recent-files-obsidian/data.json
.obsidian/plugins/rss-reader/data.json
.obsidian/workspace
1附件/权限列表.xlsx
</commit_message>
<xml_diff>
--- a/1附件/权限列表.xlsx
+++ b/1附件/权限列表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0A7033-0759-C944-962D-95D012C0C541}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8661F934-5093-3841-83B2-5839A7BDB574}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="0" windowWidth="18760" windowHeight="21600" activeTab="3" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
+    <workbookView xWindow="940" yWindow="0" windowWidth="18760" windowHeight="21600" activeTab="3" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Mdm权限管理 (2)" sheetId="7" state="hidden" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="417">
   <si>
     <t>首页面板</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1557,6 +1557,22 @@
   </si>
   <si>
     <t>下载二维码</t>
+  </si>
+  <si>
+    <t>category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>menu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4926,10 +4942,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754B3636-7394-6344-94B9-FC95971C758A}">
-  <dimension ref="A2:Q74"/>
+  <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4943,6 +4959,20 @@
     <col min="17" max="17" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D1" t="s">
+        <v>416</v>
+      </c>
+    </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
vault backup: 2022-01-05 10:38:02
Affected files:
.obsidian/plugins/recent-files-obsidian/data.json
.obsidian/workspace
.obsidian/workspaces.json
1附件/~$权限列表.xlsx
1附件/权限列表.xlsx
</commit_message>
<xml_diff>
--- a/1附件/权限列表.xlsx
+++ b/1附件/权限列表.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8661F934-5093-3841-83B2-5839A7BDB574}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587F8429-6BC9-354A-B86E-388CD8315A02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="0" windowWidth="18760" windowHeight="21600" activeTab="3" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
+    <workbookView xWindow="940" yWindow="0" windowWidth="37460" windowHeight="21600" activeTab="4" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Mdm权限管理 (2)" sheetId="7" state="hidden" r:id="rId1"/>
     <sheet name="新角色信息" sheetId="9" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="8" state="hidden" r:id="rId3"/>
-    <sheet name="Mdm权限管理" sheetId="1" r:id="rId4"/>
-    <sheet name="Uniauth权限管理" sheetId="2" r:id="rId5"/>
-    <sheet name="App权限管理" sheetId="3" r:id="rId6"/>
-    <sheet name="运营权限管理" sheetId="4" r:id="rId7"/>
-    <sheet name="运维权限管理" sheetId="5" r:id="rId8"/>
-    <sheet name="安全审核权限管理" sheetId="6" r:id="rId9"/>
+    <sheet name="Mdm权限管理-bak" sheetId="10" r:id="rId4"/>
+    <sheet name="Mdm权限管理" sheetId="1" r:id="rId5"/>
+    <sheet name="Uniauth权限管理" sheetId="2" r:id="rId6"/>
+    <sheet name="App权限管理" sheetId="3" r:id="rId7"/>
+    <sheet name="运营权限管理" sheetId="4" r:id="rId8"/>
+    <sheet name="运维权限管理" sheetId="5" r:id="rId9"/>
+    <sheet name="安全审核权限管理" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="417">
   <si>
     <t>首页面板</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3070,6 +3071,171 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89C31BD-9216-6A49-8C90-0ADAF2498DB4}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" t="s">
+        <v>231</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D0B293-1DEC-F94F-A0DE-99D6257050F6}">
   <dimension ref="A1:K213"/>
@@ -4941,11 +5107,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754B3636-7394-6344-94B9-FC95971C758A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DDD172-913C-9849-BA64-D36E9C652016}">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6053,6 +6219,103 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754B3636-7394-6344-94B9-FC95971C758A}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85160F0E-AAA4-2440-88EE-EDE07CD3F226}">
   <dimension ref="A1:N39"/>
   <sheetViews>
@@ -6646,7 +6909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC44C7D-B5C9-8244-8110-B919A147507E}">
   <dimension ref="A1:I22"/>
   <sheetViews>
@@ -6976,7 +7239,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B3B789-6212-894F-BA86-A23B372BEE33}">
   <dimension ref="A1:G22"/>
   <sheetViews>
@@ -7272,7 +7535,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F9AB08-A3B8-514B-AD13-E0375A045A1B}">
   <dimension ref="A1:G36"/>
   <sheetViews>
@@ -7718,169 +7981,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89C31BD-9216-6A49-8C90-0ADAF2498DB4}">
-  <dimension ref="A1:D14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="B3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="B7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" t="s">
-        <v>227</v>
-      </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="B11" t="s">
-        <v>226</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B13" t="s">
-        <v>231</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>104</v>
-      </c>
-      <c r="B14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2022-01-05 11:45:07
Affected files:
.obsidian/plugins/recent-files-obsidian/data.json
.obsidian/plugins/rss-reader/data.json
.obsidian/workspace
1附件/权限列表.xlsx
</commit_message>
<xml_diff>
--- a/1附件/权限列表.xlsx
+++ b/1附件/权限列表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587F8429-6BC9-354A-B86E-388CD8315A02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFE2B8A-EC2A-864C-83AD-E2CBFB8C93F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="0" windowWidth="37460" windowHeight="21600" activeTab="4" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
+    <workbookView xWindow="940" yWindow="0" windowWidth="37460" windowHeight="21600" activeTab="5" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Mdm权限管理 (2)" sheetId="7" state="hidden" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="Sheet2" sheetId="8" state="hidden" r:id="rId3"/>
     <sheet name="Mdm权限管理-bak" sheetId="10" r:id="rId4"/>
     <sheet name="Mdm权限管理" sheetId="1" r:id="rId5"/>
-    <sheet name="Uniauth权限管理" sheetId="2" r:id="rId6"/>
-    <sheet name="App权限管理" sheetId="3" r:id="rId7"/>
-    <sheet name="运营权限管理" sheetId="4" r:id="rId8"/>
-    <sheet name="运维权限管理" sheetId="5" r:id="rId9"/>
-    <sheet name="安全审核权限管理" sheetId="6" r:id="rId10"/>
+    <sheet name="Sheet3" sheetId="11" r:id="rId6"/>
+    <sheet name="Uniauth权限管理" sheetId="2" r:id="rId7"/>
+    <sheet name="App权限管理" sheetId="3" r:id="rId8"/>
+    <sheet name="运营权限管理" sheetId="4" r:id="rId9"/>
+    <sheet name="运维权限管理" sheetId="5" r:id="rId10"/>
+    <sheet name="安全审核权限管理" sheetId="6" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2128" uniqueCount="421">
   <si>
     <t>首页面板</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1574,13 +1575,105 @@
   <si>
     <t>code</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">INSERT INTO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t xml:space="preserve">`fine_auth_perm_relation` </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t xml:space="preserve">VALUES </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFA9B7C6"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>(</t>
+    </r>
+  </si>
+  <si>
+    <t>);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>'2'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>'funcId'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>'2', 'funcId',</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t/>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1595,6 +1688,21 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFCC7832"/>
+      <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="JetBrains Mono"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1640,7 +1748,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1651,6 +1759,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3072,6 +3183,454 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F9AB08-A3B8-514B-AD13-E0375A045A1B}">
+  <dimension ref="A1:G36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" t="s">
+        <v>267</v>
+      </c>
+      <c r="F3" t="s">
+        <v>268</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" t="s">
+        <v>267</v>
+      </c>
+      <c r="F5" t="s">
+        <v>268</v>
+      </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" t="s">
+        <v>271</v>
+      </c>
+      <c r="F7" t="s">
+        <v>272</v>
+      </c>
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" t="s">
+        <v>273</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>274</v>
+      </c>
+      <c r="B10" t="s">
+        <v>274</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>275</v>
+      </c>
+      <c r="B12" t="s">
+        <v>275</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>276</v>
+      </c>
+      <c r="B14" t="s">
+        <v>276</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" t="s">
+        <v>277</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" t="s">
+        <v>268</v>
+      </c>
+      <c r="F16" t="s">
+        <v>267</v>
+      </c>
+      <c r="G16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" t="s">
+        <v>278</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" t="s">
+        <v>281</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" t="s">
+        <v>282</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>284</v>
+      </c>
+      <c r="E26" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" t="s">
+        <v>283</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>284</v>
+      </c>
+      <c r="E28" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" t="s">
+        <v>286</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>284</v>
+      </c>
+      <c r="E30" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" t="s">
+        <v>287</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>114</v>
+      </c>
+      <c r="E32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" t="s">
+        <v>288</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" t="s">
+        <v>289</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89C31BD-9216-6A49-8C90-0ADAF2498DB4}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -6222,7 +6781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754B3636-7394-6344-94B9-FC95971C758A}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -6316,6 +6875,3287 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A421E20D-3F20-FF4A-A250-792992ED1A42}">
+  <dimension ref="A1:E181"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C1" t="str">
+        <f>B1&amp;""&amp;A1&amp;D1&amp;A1&amp;E1</f>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (0, '2', 'funcId',0);</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="E1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C65" si="0">B2&amp;""&amp;A2&amp;D2&amp;A2&amp;E2</f>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (1, '2', 'funcId',1);</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="E2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (2, '2', 'funcId',2);</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E3" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (3, '2', 'funcId',3);</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E4" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (4, '2', 'funcId',4);</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (5, '2', 'funcId',5);</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E6" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (6, '2', 'funcId',6);</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E7" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (7, '2', 'funcId',7);</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E8" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (8, '2', 'funcId',8);</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E9" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (9, '2', 'funcId',9);</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E10" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (10, '2', 'funcId',10);</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E11" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (11, '2', 'funcId',11);</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E12" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (12, '2', 'funcId',12);</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E13" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (13, '2', 'funcId',13);</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (14, '2', 'funcId',14);</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E15" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (15, '2', 'funcId',15);</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E16" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (16, '2', 'funcId',16);</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E17" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (17, '2', 'funcId',17);</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E18" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (18, '2', 'funcId',18);</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E19" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (19, '2', 'funcId',19);</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E20" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (20, '2', 'funcId',20);</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E21" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (21, '2', 'funcId',21);</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E22" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (22, '2', 'funcId',22);</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E23" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (23, '2', 'funcId',23);</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E24" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (24, '2', 'funcId',24);</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E25" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (25, '2', 'funcId',25);</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E26" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (26, '2', 'funcId',26);</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E27" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (27, '2', 'funcId',27);</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E28" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (28, '2', 'funcId',28);</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E29" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (29, '2', 'funcId',29);</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E30" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (30, '2', 'funcId',30);</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E31" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4">
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (31, '2', 'funcId',31);</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E32" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (32, '2', 'funcId',32);</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E33" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (33, '2', 'funcId',33);</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E34" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (34, '2', 'funcId',34);</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E35" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4">
+        <v>35</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (35, '2', 'funcId',35);</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E36" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (36, '2', 'funcId',36);</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E37" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (37, '2', 'funcId',37);</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E38" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (38, '2', 'funcId',38);</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E39" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="4">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (39, '2', 'funcId',39);</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E40" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="4">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (40, '2', 'funcId',40);</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E41" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="4">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (41, '2', 'funcId',41);</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E42" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="4">
+        <v>42</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (42, '2', 'funcId',42);</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E43" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="4">
+        <v>43</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (43, '2', 'funcId',43);</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E44" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="4">
+        <v>44</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (44, '2', 'funcId',44);</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E45" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="4">
+        <v>45</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (45, '2', 'funcId',45);</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E46" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="4">
+        <v>46</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (46, '2', 'funcId',46);</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E47" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="4">
+        <v>47</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (47, '2', 'funcId',47);</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E48" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="4">
+        <v>48</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (48, '2', 'funcId',48);</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E49" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="4">
+        <v>49</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (49, '2', 'funcId',49);</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E50" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="4">
+        <v>50</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (50, '2', 'funcId',50);</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E51" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="4">
+        <v>51</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (51, '2', 'funcId',51);</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E52" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="4">
+        <v>52</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (52, '2', 'funcId',52);</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E53" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="4">
+        <v>53</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (53, '2', 'funcId',53);</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E54" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="4">
+        <v>54</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (54, '2', 'funcId',54);</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E55" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="4">
+        <v>55</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (55, '2', 'funcId',55);</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E56" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="4">
+        <v>56</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (56, '2', 'funcId',56);</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E57" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="4">
+        <v>57</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (57, '2', 'funcId',57);</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E58" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="4">
+        <v>58</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (58, '2', 'funcId',58);</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E59" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="4">
+        <v>59</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (59, '2', 'funcId',59);</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E60" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="4">
+        <v>60</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (60, '2', 'funcId',60);</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E61" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="4">
+        <v>61</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (61, '2', 'funcId',61);</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E62" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="4">
+        <v>62</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (62, '2', 'funcId',62);</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E63" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="4">
+        <v>63</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (63, '2', 'funcId',63);</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E64" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="4">
+        <v>64</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (64, '2', 'funcId',64);</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E65" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="4">
+        <v>65</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" ref="C66:C129" si="1">B66&amp;""&amp;A66&amp;D66&amp;A66&amp;E66</f>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (65, '2', 'funcId',65);</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E66" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="4">
+        <v>66</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (66, '2', 'funcId',66);</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E67" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="4">
+        <v>67</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (67, '2', 'funcId',67);</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E68" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="4">
+        <v>68</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (68, '2', 'funcId',68);</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E69" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="4">
+        <v>69</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (69, '2', 'funcId',69);</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E70" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="4">
+        <v>70</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (70, '2', 'funcId',70);</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E71" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="4">
+        <v>71</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (71, '2', 'funcId',71);</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E72" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="4">
+        <v>72</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (72, '2', 'funcId',72);</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E73" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="4">
+        <v>73</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (73, '2', 'funcId',73);</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E74" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="4">
+        <v>74</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (74, '2', 'funcId',74);</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E75" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="4">
+        <v>75</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (75, '2', 'funcId',75);</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E76" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="4">
+        <v>76</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (76, '2', 'funcId',76);</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E77" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="4">
+        <v>77</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (77, '2', 'funcId',77);</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E78" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="4">
+        <v>78</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (78, '2', 'funcId',78);</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E79" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="4">
+        <v>79</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (79, '2', 'funcId',79);</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E80" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="4">
+        <v>80</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (80, '2', 'funcId',80);</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E81" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="4">
+        <v>81</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (81, '2', 'funcId',81);</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E82" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="4">
+        <v>82</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (82, '2', 'funcId',82);</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E83" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="4">
+        <v>83</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (83, '2', 'funcId',83);</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E84" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="4">
+        <v>84</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (84, '2', 'funcId',84);</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E85" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="4">
+        <v>85</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (85, '2', 'funcId',85);</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E86" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="4">
+        <v>86</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (86, '2', 'funcId',86);</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E87" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="4">
+        <v>87</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (87, '2', 'funcId',87);</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E88" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="4">
+        <v>88</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (88, '2', 'funcId',88);</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E89" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="4">
+        <v>89</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (89, '2', 'funcId',89);</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E90" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="4">
+        <v>90</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (90, '2', 'funcId',90);</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E91" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="4">
+        <v>91</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (91, '2', 'funcId',91);</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E92" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="4">
+        <v>92</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (92, '2', 'funcId',92);</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E93" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="4">
+        <v>93</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (93, '2', 'funcId',93);</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E94" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="4">
+        <v>94</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (94, '2', 'funcId',94);</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E95" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="4">
+        <v>95</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (95, '2', 'funcId',95);</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E96" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="4">
+        <v>96</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (96, '2', 'funcId',96);</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E97" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="4">
+        <v>97</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (97, '2', 'funcId',97);</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E98" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="4">
+        <v>98</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (98, '2', 'funcId',98);</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E99" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="4">
+        <v>99</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (99, '2', 'funcId',99);</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E100" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="4">
+        <v>100</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (100, '2', 'funcId',100);</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E101" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="4">
+        <v>101</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (101, '2', 'funcId',101);</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E102" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="4">
+        <v>102</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (102, '2', 'funcId',102);</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E103" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" s="4">
+        <v>103</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (103, '2', 'funcId',103);</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E104" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="4">
+        <v>104</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (104, '2', 'funcId',104);</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E105" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="4">
+        <v>105</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C106" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (105, '2', 'funcId',105);</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E106" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="4">
+        <v>106</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C107" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (106, '2', 'funcId',106);</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E107" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="4">
+        <v>107</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C108" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (107, '2', 'funcId',107);</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E108" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="4">
+        <v>108</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C109" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (108, '2', 'funcId',108);</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E109" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="4">
+        <v>109</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C110" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (109, '2', 'funcId',109);</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E110" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="4">
+        <v>110</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C111" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (110, '2', 'funcId',110);</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E111" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" s="4">
+        <v>111</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C112" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (111, '2', 'funcId',111);</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E112" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="4">
+        <v>112</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C113" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (112, '2', 'funcId',112);</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E113" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="4">
+        <v>113</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C114" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (113, '2', 'funcId',113);</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E114" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="4">
+        <v>114</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C115" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (114, '2', 'funcId',114);</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E115" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="4">
+        <v>115</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C116" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (115, '2', 'funcId',115);</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E116" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="4">
+        <v>116</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C117" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (116, '2', 'funcId',116);</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E117" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="4">
+        <v>117</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C118" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (117, '2', 'funcId',117);</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E118" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="4">
+        <v>118</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C119" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (118, '2', 'funcId',118);</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E119" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="4">
+        <v>119</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C120" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (119, '2', 'funcId',119);</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E120" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="4">
+        <v>120</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C121" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (120, '2', 'funcId',120);</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E121" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" s="4">
+        <v>121</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C122" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (121, '2', 'funcId',121);</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E122" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="4">
+        <v>122</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C123" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (122, '2', 'funcId',122);</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E123" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="4">
+        <v>123</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C124" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (123, '2', 'funcId',123);</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E124" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" s="4">
+        <v>124</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C125" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (124, '2', 'funcId',124);</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E125" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="4">
+        <v>125</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C126" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (125, '2', 'funcId',125);</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E126" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="4">
+        <v>126</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C127" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (126, '2', 'funcId',126);</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E127" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="4">
+        <v>127</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C128" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (127, '2', 'funcId',127);</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E128" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" s="4">
+        <v>128</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C129" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (128, '2', 'funcId',128);</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E129" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" s="4">
+        <v>129</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C130" t="str">
+        <f t="shared" ref="C130:C181" si="2">B130&amp;""&amp;A130&amp;D130&amp;A130&amp;E130</f>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (129, '2', 'funcId',129);</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E130" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" s="4">
+        <v>130</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C131" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (130, '2', 'funcId',130);</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E131" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" s="4">
+        <v>131</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C132" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (131, '2', 'funcId',131);</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E132" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" s="4">
+        <v>132</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C133" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (132, '2', 'funcId',132);</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E133" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" s="4">
+        <v>133</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C134" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (133, '2', 'funcId',133);</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E134" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" s="4">
+        <v>134</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C135" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (134, '2', 'funcId',134);</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E135" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" s="4">
+        <v>135</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C136" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (135, '2', 'funcId',135);</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E136" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" s="4">
+        <v>136</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C137" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (136, '2', 'funcId',136);</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E137" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" s="4">
+        <v>137</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C138" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (137, '2', 'funcId',137);</v>
+      </c>
+      <c r="D138" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E138" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" s="4">
+        <v>138</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C139" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (138, '2', 'funcId',138);</v>
+      </c>
+      <c r="D139" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E139" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" s="4">
+        <v>139</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C140" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (139, '2', 'funcId',139);</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E140" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" s="4">
+        <v>140</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C141" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (140, '2', 'funcId',140);</v>
+      </c>
+      <c r="D141" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E141" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" s="4">
+        <v>141</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C142" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (141, '2', 'funcId',141);</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E142" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" s="4">
+        <v>142</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C143" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (142, '2', 'funcId',142);</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E143" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" s="4">
+        <v>143</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C144" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (143, '2', 'funcId',143);</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E144" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" s="4">
+        <v>144</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C145" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (144, '2', 'funcId',144);</v>
+      </c>
+      <c r="D145" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E145" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="4">
+        <v>145</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C146" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (145, '2', 'funcId',145);</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E146" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" s="4">
+        <v>146</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C147" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (146, '2', 'funcId',146);</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E147" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="4">
+        <v>147</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C148" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (147, '2', 'funcId',147);</v>
+      </c>
+      <c r="D148" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E148" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" s="4">
+        <v>148</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C149" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (148, '2', 'funcId',148);</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E149" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" s="4">
+        <v>149</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C150" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (149, '2', 'funcId',149);</v>
+      </c>
+      <c r="D150" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E150" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" s="4">
+        <v>150</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C151" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (150, '2', 'funcId',150);</v>
+      </c>
+      <c r="D151" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E151" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" s="4">
+        <v>151</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C152" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (151, '2', 'funcId',151);</v>
+      </c>
+      <c r="D152" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E152" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" s="4">
+        <v>152</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C153" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (152, '2', 'funcId',152);</v>
+      </c>
+      <c r="D153" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E153" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" s="4">
+        <v>153</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C154" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (153, '2', 'funcId',153);</v>
+      </c>
+      <c r="D154" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E154" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" s="4">
+        <v>154</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C155" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (154, '2', 'funcId',154);</v>
+      </c>
+      <c r="D155" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E155" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" s="4">
+        <v>155</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C156" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (155, '2', 'funcId',155);</v>
+      </c>
+      <c r="D156" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E156" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" s="4">
+        <v>156</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C157" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (156, '2', 'funcId',156);</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E157" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" s="4">
+        <v>157</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C158" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (157, '2', 'funcId',157);</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E158" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" s="4">
+        <v>158</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C159" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (158, '2', 'funcId',158);</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E159" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" s="4">
+        <v>159</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C160" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (159, '2', 'funcId',159);</v>
+      </c>
+      <c r="D160" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E160" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" s="4">
+        <v>160</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C161" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (160, '2', 'funcId',160);</v>
+      </c>
+      <c r="D161" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E161" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" s="4">
+        <v>161</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C162" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (161, '2', 'funcId',161);</v>
+      </c>
+      <c r="D162" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E162" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" s="4">
+        <v>162</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C163" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (162, '2', 'funcId',162);</v>
+      </c>
+      <c r="D163" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E163" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" s="4">
+        <v>163</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C164" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (163, '2', 'funcId',163);</v>
+      </c>
+      <c r="D164" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E164" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" s="4">
+        <v>164</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C165" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (164, '2', 'funcId',164);</v>
+      </c>
+      <c r="D165" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E165" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" s="4">
+        <v>165</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C166" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (165, '2', 'funcId',165);</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E166" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" s="4">
+        <v>166</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C167" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (166, '2', 'funcId',166);</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E167" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" s="4">
+        <v>167</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C168" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (167, '2', 'funcId',167);</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E168" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" s="4">
+        <v>168</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C169" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (168, '2', 'funcId',168);</v>
+      </c>
+      <c r="D169" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E169" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" s="4">
+        <v>169</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C170" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (169, '2', 'funcId',169);</v>
+      </c>
+      <c r="D170" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E170" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" s="4">
+        <v>170</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C171" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (170, '2', 'funcId',170);</v>
+      </c>
+      <c r="D171" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E171" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" s="4">
+        <v>171</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C172" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (171, '2', 'funcId',171);</v>
+      </c>
+      <c r="D172" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E172" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" s="4">
+        <v>172</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C173" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (172, '2', 'funcId',172);</v>
+      </c>
+      <c r="D173" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E173" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" s="4">
+        <v>173</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C174" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (173, '2', 'funcId',173);</v>
+      </c>
+      <c r="D174" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E174" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" s="4">
+        <v>174</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C175" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (174, '2', 'funcId',174);</v>
+      </c>
+      <c r="D175" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E175" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" s="4">
+        <v>175</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C176" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (175, '2', 'funcId',175);</v>
+      </c>
+      <c r="D176" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E176" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" s="4">
+        <v>176</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C177" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (176, '2', 'funcId',176);</v>
+      </c>
+      <c r="D177" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E177" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" s="4">
+        <v>177</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C178" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (177, '2', 'funcId',177);</v>
+      </c>
+      <c r="D178" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E178" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" s="4">
+        <v>178</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C179" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (178, '2', 'funcId',178);</v>
+      </c>
+      <c r="D179" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E179" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" s="4">
+        <v>179</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C180" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (179, '2', 'funcId',179);</v>
+      </c>
+      <c r="D180" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E180" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" s="4">
+        <v>180</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C181" t="str">
+        <f t="shared" si="2"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (180, '2', 'funcId',180);</v>
+      </c>
+      <c r="D181" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E181" t="s">
+        <v>418</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85160F0E-AAA4-2440-88EE-EDE07CD3F226}">
   <dimension ref="A1:N39"/>
   <sheetViews>
@@ -6909,7 +10749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC44C7D-B5C9-8244-8110-B919A147507E}">
   <dimension ref="A1:I22"/>
   <sheetViews>
@@ -7239,7 +11079,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B3B789-6212-894F-BA86-A23B372BEE33}">
   <dimension ref="A1:G22"/>
   <sheetViews>
@@ -7533,452 +11373,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F9AB08-A3B8-514B-AD13-E0375A045A1B}">
-  <dimension ref="A1:G36"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>265</v>
-      </c>
-      <c r="B2" t="s">
-        <v>266</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E3" t="s">
-        <v>267</v>
-      </c>
-      <c r="F3" t="s">
-        <v>268</v>
-      </c>
-      <c r="G3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="B4" t="s">
-        <v>269</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" t="s">
-        <v>267</v>
-      </c>
-      <c r="F5" t="s">
-        <v>268</v>
-      </c>
-      <c r="G5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="B6" t="s">
-        <v>270</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" t="s">
-        <v>271</v>
-      </c>
-      <c r="F7" t="s">
-        <v>272</v>
-      </c>
-      <c r="G7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" t="s">
-        <v>273</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>274</v>
-      </c>
-      <c r="B10" t="s">
-        <v>274</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>275</v>
-      </c>
-      <c r="B12" t="s">
-        <v>275</v>
-      </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>276</v>
-      </c>
-      <c r="B14" t="s">
-        <v>276</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" t="s">
-        <v>277</v>
-      </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>110</v>
-      </c>
-      <c r="E16" t="s">
-        <v>268</v>
-      </c>
-      <c r="F16" t="s">
-        <v>267</v>
-      </c>
-      <c r="G16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" t="s">
-        <v>278</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" t="s">
-        <v>281</v>
-      </c>
-      <c r="C21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" t="s">
-        <v>282</v>
-      </c>
-      <c r="C24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5">
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" t="s">
-        <v>284</v>
-      </c>
-      <c r="E26" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5">
-      <c r="B27" t="s">
-        <v>283</v>
-      </c>
-      <c r="C27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="C28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" t="s">
-        <v>284</v>
-      </c>
-      <c r="E28" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="B29" t="s">
-        <v>286</v>
-      </c>
-      <c r="C29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="C30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" t="s">
-        <v>284</v>
-      </c>
-      <c r="E30" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5">
-      <c r="B31" t="s">
-        <v>287</v>
-      </c>
-      <c r="C31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5">
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" t="s">
-        <v>114</v>
-      </c>
-      <c r="E32" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5">
-      <c r="B33" t="s">
-        <v>288</v>
-      </c>
-      <c r="C33" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="C34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" t="s">
-        <v>114</v>
-      </c>
-      <c r="E34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="B35" t="s">
-        <v>289</v>
-      </c>
-      <c r="C35" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="C36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" t="s">
-        <v>114</v>
-      </c>
-      <c r="E36" t="s">
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2022-01-05 15:49:15
Affected files:
.obsidian/plugins/rss-reader/data.json
.vault-stats
14TODO/TODO.md
1附件/~$权限列表.xlsx
1附件/权限列表.xlsx
</commit_message>
<xml_diff>
--- a/1附件/权限列表.xlsx
+++ b/1附件/权限列表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A49E8A-F44A-9D47-8808-9FD18428E547}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804979DF-302D-5A49-8A33-DED74AEB3452}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="0" windowWidth="37460" windowHeight="21600" activeTab="5" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sheet2" sheetId="8" state="hidden" r:id="rId3"/>
     <sheet name="Mdm权限管理-bak" sheetId="10" r:id="rId4"/>
     <sheet name="Mdm权限管理" sheetId="1" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="11" r:id="rId6"/>
+    <sheet name="Mdm数据库脚本" sheetId="11" r:id="rId6"/>
     <sheet name="Uniauth权限管理" sheetId="2" r:id="rId7"/>
     <sheet name="App权限管理" sheetId="3" r:id="rId8"/>
     <sheet name="运营权限管理" sheetId="4" r:id="rId9"/>
@@ -6878,8 +6878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A421E20D-3F20-FF4A-A250-792992ED1A42}">
   <dimension ref="A1:E181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="L84" sqref="L84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
vault backup: 2022-01-05 16:49:15
Affected files:
.obsidian/plugins/rss-reader/data.json
1附件/~$权限列表.xlsx
1附件/权限列表.xlsx
</commit_message>
<xml_diff>
--- a/1附件/权限列表.xlsx
+++ b/1附件/权限列表.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804979DF-302D-5A49-8A33-DED74AEB3452}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC529B8-ED3E-3D4C-A565-92D892E3AA14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="0" windowWidth="37460" windowHeight="21600" activeTab="5" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
+    <workbookView xWindow="940" yWindow="0" windowWidth="37460" windowHeight="21600" activeTab="4" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Mdm权限管理 (2)" sheetId="7" state="hidden" r:id="rId1"/>
     <sheet name="新角色信息" sheetId="9" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="8" state="hidden" r:id="rId3"/>
-    <sheet name="Mdm权限管理-bak" sheetId="10" r:id="rId4"/>
-    <sheet name="Mdm权限管理" sheetId="1" r:id="rId5"/>
+    <sheet name="Mdm权限管理" sheetId="10" r:id="rId4"/>
+    <sheet name="数据字典首页面板_x000a_首页面板_x000a_查看_x000a_用户管理_x000a_组织机构_x000a_查看_x000a_编" sheetId="12" r:id="rId5"/>
     <sheet name="Mdm数据库脚本" sheetId="11" r:id="rId6"/>
     <sheet name="Uniauth权限管理" sheetId="2" r:id="rId7"/>
     <sheet name="App权限管理" sheetId="3" r:id="rId8"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2128" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2221" uniqueCount="485">
   <si>
     <t>首页面板</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1667,6 +1667,198 @@
       </rPr>
       <t/>
     </r>
+  </si>
+  <si>
+    <t>苹果设备管理</t>
+  </si>
+  <si>
+    <t>苹果注册记录</t>
+  </si>
+  <si>
+    <t>苹果设备策略</t>
+  </si>
+  <si>
+    <t>苹果规则</t>
+  </si>
+  <si>
+    <t>苹果应用安装</t>
+  </si>
+  <si>
+    <t>苹果意见反馈</t>
+  </si>
+  <si>
+    <t>苹果客户端升级</t>
+  </si>
+  <si>
+    <t>user_management</t>
+  </si>
+  <si>
+    <t>the_security_policy</t>
+  </si>
+  <si>
+    <t>the_front_panel</t>
+  </si>
+  <si>
+    <t>system_management</t>
+  </si>
+  <si>
+    <t>statistical_reports</t>
+  </si>
+  <si>
+    <t>security_audit</t>
+  </si>
+  <si>
+    <t>resource_management</t>
+  </si>
+  <si>
+    <t>log_management</t>
+  </si>
+  <si>
+    <t>equipment_management</t>
+  </si>
+  <si>
+    <t>user_statistics</t>
+  </si>
+  <si>
+    <t>user_login_log</t>
+  </si>
+  <si>
+    <t>traffic_statistics</t>
+  </si>
+  <si>
+    <t>the_user_group</t>
+  </si>
+  <si>
+    <t>the_organization</t>
+  </si>
+  <si>
+    <t>the_message_management</t>
+  </si>
+  <si>
+    <t>the_app_install</t>
+  </si>
+  <si>
+    <t>the_android_phone_records</t>
+  </si>
+  <si>
+    <t>the_android_device_management</t>
+  </si>
+  <si>
+    <t>the_administrator_operation_log</t>
+  </si>
+  <si>
+    <t>system_settings</t>
+  </si>
+  <si>
+    <t>sensitive_word_statistics</t>
+  </si>
+  <si>
+    <t>sensitive_word_library</t>
+  </si>
+  <si>
+    <t>safety_statistics</t>
+  </si>
+  <si>
+    <t>report_to_download</t>
+  </si>
+  <si>
+    <t>registration_audit</t>
+  </si>
+  <si>
+    <t>registered_white_list</t>
+  </si>
+  <si>
+    <t>network_statistics</t>
+  </si>
+  <si>
+    <t>mobile_portal_settings</t>
+  </si>
+  <si>
+    <t>list_of_users</t>
+  </si>
+  <si>
+    <t>equipment_statistics</t>
+  </si>
+  <si>
+    <t>equipment_log</t>
+  </si>
+  <si>
+    <t>entrance_guard_access_records</t>
+  </si>
+  <si>
+    <t>electronic_fence_in_record</t>
+  </si>
+  <si>
+    <t>document_management</t>
+  </si>
+  <si>
+    <t>cope_the_client_upgrade</t>
+  </si>
+  <si>
+    <t>bluetooth_white_list</t>
+  </si>
+  <si>
+    <t>application_of_statistical</t>
+  </si>
+  <si>
+    <t>application_of_distributed</t>
+  </si>
+  <si>
+    <t>apples_rules</t>
+  </si>
+  <si>
+    <t>apples_feedback</t>
+  </si>
+  <si>
+    <t>apple_registration_record</t>
+  </si>
+  <si>
+    <t>apple_equipment_management</t>
+  </si>
+  <si>
+    <t>apple_devices_strategy</t>
+  </si>
+  <si>
+    <t>apple_client_upgrade</t>
+  </si>
+  <si>
+    <t>android_wx_letter_to_chat</t>
+  </si>
+  <si>
+    <t>android_words</t>
+  </si>
+  <si>
+    <t>android_text_record</t>
+  </si>
+  <si>
+    <t>android_registration_record</t>
+  </si>
+  <si>
+    <t>android_qq_chat</t>
+  </si>
+  <si>
+    <t>android_mms_record</t>
+  </si>
+  <si>
+    <t>android_internet_behavior</t>
+  </si>
+  <si>
+    <t>android_in_violation_of_state_records</t>
+  </si>
+  <si>
+    <t>android_feedback</t>
+  </si>
+  <si>
+    <t>android_devices_strategy</t>
+  </si>
+  <si>
+    <t>android_applications_use</t>
+  </si>
+  <si>
+    <t>android_applications_to_install</t>
+  </si>
+  <si>
+    <t>about_a_system</t>
   </si>
 </sst>
 </file>
@@ -5670,7 +5862,7 @@
   <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6778,96 +6970,917 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754B3636-7394-6344-94B9-FC95971C758A}">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DFAFE7B-50A9-ED46-A4A9-43F085DA759E}">
+  <dimension ref="A1:I185"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="138.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B1" t="s">
-        <v>414</v>
-      </c>
-      <c r="C1" t="s">
-        <v>415</v>
-      </c>
-      <c r="D1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>310</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>311</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>120</v>
-      </c>
+        <v>433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B4" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>378</v>
+      </c>
+      <c r="B5" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>374</v>
+      </c>
+      <c r="B6" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>373</v>
+      </c>
+      <c r="B7" t="s">
+        <v>474</v>
+      </c>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B8" t="s">
+        <v>473</v>
+      </c>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>367</v>
+      </c>
+      <c r="B9" t="s">
+        <v>478</v>
+      </c>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>357</v>
+      </c>
+      <c r="B10" t="s">
+        <v>481</v>
+      </c>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>322</v>
+      </c>
+      <c r="B11" t="s">
+        <v>445</v>
+      </c>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>368</v>
+      </c>
+      <c r="B12" t="s">
+        <v>444</v>
+      </c>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>375</v>
+      </c>
+      <c r="B13" t="s">
+        <v>472</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>380</v>
+      </c>
+      <c r="B14" t="s">
+        <v>479</v>
+      </c>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>406</v>
+      </c>
+      <c r="B15" t="s">
+        <v>480</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>365</v>
+      </c>
+      <c r="B16" t="s">
+        <v>483</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>366</v>
+      </c>
+      <c r="B17" t="s">
+        <v>482</v>
+      </c>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>329</v>
+      </c>
+      <c r="B18" t="s">
+        <v>475</v>
+      </c>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>409</v>
+      </c>
+      <c r="B19" t="s">
+        <v>451</v>
+      </c>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>396</v>
+      </c>
+      <c r="B20" t="s">
+        <v>459</v>
+      </c>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>411</v>
+      </c>
+      <c r="B21" t="s">
+        <v>484</v>
+      </c>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>392</v>
+      </c>
+      <c r="B22" t="s">
+        <v>446</v>
+      </c>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>359</v>
+      </c>
+      <c r="B23" t="s">
+        <v>463</v>
+      </c>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>391</v>
+      </c>
+      <c r="B24" t="s">
+        <v>439</v>
+      </c>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>395</v>
+      </c>
+      <c r="B25" t="s">
+        <v>460</v>
+      </c>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>384</v>
+      </c>
+      <c r="B26" t="s">
+        <v>449</v>
+      </c>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>390</v>
+      </c>
+      <c r="B27" t="s">
+        <v>448</v>
+      </c>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>424</v>
+      </c>
+      <c r="B28" t="s">
+        <v>466</v>
+      </c>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>427</v>
+      </c>
+      <c r="B29" t="s">
+        <v>471</v>
+      </c>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>423</v>
+      </c>
+      <c r="B30" t="s">
+        <v>470</v>
+      </c>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>421</v>
+      </c>
+      <c r="B31" t="s">
+        <v>469</v>
+      </c>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>426</v>
+      </c>
+      <c r="B32" t="s">
+        <v>467</v>
+      </c>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>425</v>
+      </c>
+      <c r="B33" t="s">
+        <v>443</v>
+      </c>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>422</v>
+      </c>
+      <c r="B34" t="s">
+        <v>468</v>
+      </c>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>314</v>
+      </c>
+      <c r="B35" t="s">
+        <v>435</v>
+      </c>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>309</v>
+      </c>
+      <c r="B36" t="s">
+        <v>436</v>
+      </c>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>394</v>
+      </c>
+      <c r="B37" t="s">
+        <v>458</v>
+      </c>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>386</v>
+      </c>
+      <c r="B38" t="s">
+        <v>457</v>
+      </c>
+      <c r="I38" s="4"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>308</v>
+      </c>
+      <c r="B39" t="s">
+        <v>430</v>
+      </c>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
+        <v>313</v>
+      </c>
+      <c r="B40" t="s">
+        <v>432</v>
+      </c>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>389</v>
+      </c>
+      <c r="B41" t="s">
+        <v>454</v>
+      </c>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>382</v>
+      </c>
+      <c r="B42" t="s">
+        <v>461</v>
+      </c>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>315</v>
+      </c>
+      <c r="B43" t="s">
+        <v>431</v>
+      </c>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>397</v>
+      </c>
+      <c r="B44" t="s">
+        <v>447</v>
+      </c>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>405</v>
+      </c>
+      <c r="B45" t="s">
+        <v>442</v>
+      </c>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>401</v>
+      </c>
+      <c r="B46" t="s">
+        <v>455</v>
+      </c>
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>381</v>
+      </c>
+      <c r="B47" t="s">
+        <v>465</v>
+      </c>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>388</v>
+      </c>
+      <c r="B48" t="s">
+        <v>464</v>
+      </c>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" t="s">
+        <v>393</v>
+      </c>
+      <c r="B49" t="s">
+        <v>438</v>
+      </c>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" t="s">
+        <v>303</v>
+      </c>
+      <c r="B50" t="s">
+        <v>440</v>
+      </c>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" t="s">
+        <v>297</v>
+      </c>
+      <c r="B51" t="s">
+        <v>428</v>
+      </c>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>302</v>
+      </c>
+      <c r="B52" t="s">
+        <v>456</v>
+      </c>
+      <c r="I52" s="4"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
+        <v>385</v>
+      </c>
+      <c r="B53" t="s">
+        <v>437</v>
+      </c>
+      <c r="I53" s="4"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="s">
+        <v>327</v>
+      </c>
+      <c r="B54" t="s">
+        <v>453</v>
+      </c>
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
+        <v>325</v>
+      </c>
+      <c r="B55" t="s">
+        <v>452</v>
+      </c>
+      <c r="I55" s="4"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>312</v>
+      </c>
+      <c r="B56" t="s">
+        <v>434</v>
+      </c>
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>298</v>
+      </c>
+      <c r="B57" t="s">
+        <v>441</v>
+      </c>
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="I61" s="4"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="I63" s="4"/>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="I64" s="4"/>
+    </row>
+    <row r="65" spans="9:9">
+      <c r="I65" s="4"/>
+    </row>
+    <row r="66" spans="9:9">
+      <c r="I66" s="4"/>
+    </row>
+    <row r="67" spans="9:9">
+      <c r="I67" s="4"/>
+    </row>
+    <row r="68" spans="9:9">
+      <c r="I68" s="4"/>
+    </row>
+    <row r="69" spans="9:9">
+      <c r="I69" s="4"/>
+    </row>
+    <row r="70" spans="9:9">
+      <c r="I70" s="4"/>
+    </row>
+    <row r="71" spans="9:9">
+      <c r="I71" s="4"/>
+    </row>
+    <row r="72" spans="9:9">
+      <c r="I72" s="4"/>
+    </row>
+    <row r="73" spans="9:9">
+      <c r="I73" s="4"/>
+    </row>
+    <row r="74" spans="9:9">
+      <c r="I74" s="4"/>
+    </row>
+    <row r="75" spans="9:9">
+      <c r="I75" s="4"/>
+    </row>
+    <row r="76" spans="9:9">
+      <c r="I76" s="4"/>
+    </row>
+    <row r="77" spans="9:9">
+      <c r="I77" s="4"/>
+    </row>
+    <row r="78" spans="9:9">
+      <c r="I78" s="4"/>
+    </row>
+    <row r="79" spans="9:9">
+      <c r="I79" s="4"/>
+    </row>
+    <row r="80" spans="9:9">
+      <c r="I80" s="4"/>
+    </row>
+    <row r="81" spans="9:9">
+      <c r="I81" s="4"/>
+    </row>
+    <row r="82" spans="9:9">
+      <c r="I82" s="4"/>
+    </row>
+    <row r="83" spans="9:9">
+      <c r="I83" s="4"/>
+    </row>
+    <row r="84" spans="9:9">
+      <c r="I84" s="4"/>
+    </row>
+    <row r="85" spans="9:9">
+      <c r="I85" s="4"/>
+    </row>
+    <row r="86" spans="9:9">
+      <c r="I86" s="4"/>
+    </row>
+    <row r="87" spans="9:9">
+      <c r="I87" s="4"/>
+    </row>
+    <row r="88" spans="9:9">
+      <c r="I88" s="4"/>
+    </row>
+    <row r="89" spans="9:9">
+      <c r="I89" s="4"/>
+    </row>
+    <row r="90" spans="9:9">
+      <c r="I90" s="4"/>
+    </row>
+    <row r="91" spans="9:9">
+      <c r="I91" s="4"/>
+    </row>
+    <row r="92" spans="9:9">
+      <c r="I92" s="4"/>
+    </row>
+    <row r="93" spans="9:9">
+      <c r="I93" s="4"/>
+    </row>
+    <row r="94" spans="9:9">
+      <c r="I94" s="4"/>
+    </row>
+    <row r="95" spans="9:9">
+      <c r="I95" s="4"/>
+    </row>
+    <row r="96" spans="9:9">
+      <c r="I96" s="4"/>
+    </row>
+    <row r="97" spans="9:9">
+      <c r="I97" s="4"/>
+    </row>
+    <row r="98" spans="9:9">
+      <c r="I98" s="4"/>
+    </row>
+    <row r="99" spans="9:9">
+      <c r="I99" s="4"/>
+    </row>
+    <row r="100" spans="9:9">
+      <c r="I100" s="4"/>
+    </row>
+    <row r="101" spans="9:9">
+      <c r="I101" s="4"/>
+    </row>
+    <row r="102" spans="9:9">
+      <c r="I102" s="4"/>
+    </row>
+    <row r="103" spans="9:9">
+      <c r="I103" s="4"/>
+    </row>
+    <row r="104" spans="9:9">
+      <c r="I104" s="4"/>
+    </row>
+    <row r="105" spans="9:9">
+      <c r="I105" s="4"/>
+    </row>
+    <row r="106" spans="9:9">
+      <c r="I106" s="4"/>
+    </row>
+    <row r="107" spans="9:9">
+      <c r="I107" s="4"/>
+    </row>
+    <row r="108" spans="9:9">
+      <c r="I108" s="4"/>
+    </row>
+    <row r="109" spans="9:9">
+      <c r="I109" s="4"/>
+    </row>
+    <row r="110" spans="9:9">
+      <c r="I110" s="4"/>
+    </row>
+    <row r="111" spans="9:9">
+      <c r="I111" s="4"/>
+    </row>
+    <row r="112" spans="9:9">
+      <c r="I112" s="4"/>
+    </row>
+    <row r="113" spans="9:9">
+      <c r="I113" s="4"/>
+    </row>
+    <row r="114" spans="9:9">
+      <c r="I114" s="4"/>
+    </row>
+    <row r="115" spans="9:9">
+      <c r="I115" s="4"/>
+    </row>
+    <row r="116" spans="9:9">
+      <c r="I116" s="4"/>
+    </row>
+    <row r="117" spans="9:9">
+      <c r="I117" s="4"/>
+    </row>
+    <row r="118" spans="9:9">
+      <c r="I118" s="4"/>
+    </row>
+    <row r="119" spans="9:9">
+      <c r="I119" s="4"/>
+    </row>
+    <row r="120" spans="9:9">
+      <c r="I120" s="4"/>
+    </row>
+    <row r="121" spans="9:9">
+      <c r="I121" s="4"/>
+    </row>
+    <row r="122" spans="9:9">
+      <c r="I122" s="4"/>
+    </row>
+    <row r="123" spans="9:9">
+      <c r="I123" s="4"/>
+    </row>
+    <row r="124" spans="9:9">
+      <c r="I124" s="4"/>
+    </row>
+    <row r="125" spans="9:9">
+      <c r="I125" s="4"/>
+    </row>
+    <row r="126" spans="9:9">
+      <c r="I126" s="4"/>
+    </row>
+    <row r="127" spans="9:9">
+      <c r="I127" s="4"/>
+    </row>
+    <row r="128" spans="9:9">
+      <c r="I128" s="4"/>
+    </row>
+    <row r="129" spans="9:9">
+      <c r="I129" s="4"/>
+    </row>
+    <row r="130" spans="9:9">
+      <c r="I130" s="4"/>
+    </row>
+    <row r="131" spans="9:9">
+      <c r="I131" s="4"/>
+    </row>
+    <row r="132" spans="9:9">
+      <c r="I132" s="4"/>
+    </row>
+    <row r="133" spans="9:9">
+      <c r="I133" s="4"/>
+    </row>
+    <row r="134" spans="9:9">
+      <c r="I134" s="4"/>
+    </row>
+    <row r="135" spans="9:9">
+      <c r="I135" s="4"/>
+    </row>
+    <row r="136" spans="9:9">
+      <c r="I136" s="4"/>
+    </row>
+    <row r="137" spans="9:9">
+      <c r="I137" s="4"/>
+    </row>
+    <row r="138" spans="9:9">
+      <c r="I138" s="4"/>
+    </row>
+    <row r="139" spans="9:9">
+      <c r="I139" s="4"/>
+    </row>
+    <row r="140" spans="9:9">
+      <c r="I140" s="4"/>
+    </row>
+    <row r="141" spans="9:9">
+      <c r="I141" s="4"/>
+    </row>
+    <row r="142" spans="9:9">
+      <c r="I142" s="4"/>
+    </row>
+    <row r="143" spans="9:9">
+      <c r="I143" s="4"/>
+    </row>
+    <row r="144" spans="9:9">
+      <c r="I144" s="4"/>
+    </row>
+    <row r="145" spans="9:9">
+      <c r="I145" s="4"/>
+    </row>
+    <row r="146" spans="9:9">
+      <c r="I146" s="4"/>
+    </row>
+    <row r="147" spans="9:9">
+      <c r="I147" s="4"/>
+    </row>
+    <row r="148" spans="9:9">
+      <c r="I148" s="4"/>
+    </row>
+    <row r="149" spans="9:9">
+      <c r="I149" s="4"/>
+    </row>
+    <row r="150" spans="9:9">
+      <c r="I150" s="4"/>
+    </row>
+    <row r="151" spans="9:9">
+      <c r="I151" s="4"/>
+    </row>
+    <row r="152" spans="9:9">
+      <c r="I152" s="4"/>
+    </row>
+    <row r="153" spans="9:9">
+      <c r="I153" s="4"/>
+    </row>
+    <row r="154" spans="9:9">
+      <c r="I154" s="4"/>
+    </row>
+    <row r="155" spans="9:9">
+      <c r="I155" s="4"/>
+    </row>
+    <row r="156" spans="9:9">
+      <c r="I156" s="4"/>
+    </row>
+    <row r="157" spans="9:9">
+      <c r="I157" s="4"/>
+    </row>
+    <row r="158" spans="9:9">
+      <c r="I158" s="4"/>
+    </row>
+    <row r="159" spans="9:9">
+      <c r="I159" s="4"/>
+    </row>
+    <row r="160" spans="9:9">
+      <c r="I160" s="4"/>
+    </row>
+    <row r="161" spans="9:9">
+      <c r="I161" s="4"/>
+    </row>
+    <row r="162" spans="9:9">
+      <c r="I162" s="4"/>
+    </row>
+    <row r="163" spans="9:9">
+      <c r="I163" s="4"/>
+    </row>
+    <row r="164" spans="9:9">
+      <c r="I164" s="4"/>
+    </row>
+    <row r="165" spans="9:9">
+      <c r="I165" s="4"/>
+    </row>
+    <row r="166" spans="9:9">
+      <c r="I166" s="4"/>
+    </row>
+    <row r="167" spans="9:9">
+      <c r="I167" s="4"/>
+    </row>
+    <row r="168" spans="9:9">
+      <c r="I168" s="4"/>
+    </row>
+    <row r="169" spans="9:9">
+      <c r="I169" s="4"/>
+    </row>
+    <row r="170" spans="9:9">
+      <c r="I170" s="4"/>
+    </row>
+    <row r="171" spans="9:9">
+      <c r="I171" s="4"/>
+    </row>
+    <row r="172" spans="9:9">
+      <c r="I172" s="4"/>
+    </row>
+    <row r="173" spans="9:9">
+      <c r="I173" s="4"/>
+    </row>
+    <row r="174" spans="9:9">
+      <c r="I174" s="4"/>
+    </row>
+    <row r="175" spans="9:9">
+      <c r="I175" s="4"/>
+    </row>
+    <row r="176" spans="9:9">
+      <c r="I176" s="4"/>
+    </row>
+    <row r="177" spans="9:9">
+      <c r="I177" s="4"/>
+    </row>
+    <row r="178" spans="9:9">
+      <c r="I178" s="4"/>
+    </row>
+    <row r="179" spans="9:9">
+      <c r="I179" s="4"/>
+    </row>
+    <row r="180" spans="9:9">
+      <c r="I180" s="4"/>
+    </row>
+    <row r="181" spans="9:9">
+      <c r="I181" s="4"/>
+    </row>
+    <row r="182" spans="9:9">
+      <c r="I182" s="4"/>
+    </row>
+    <row r="183" spans="9:9">
+      <c r="I183" s="4"/>
+    </row>
+    <row r="184" spans="9:9">
+      <c r="I184" s="4"/>
+    </row>
+    <row r="185" spans="9:9">
+      <c r="I185" s="4"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A126">
+    <sortCondition ref="A1:A126"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6878,7 +7891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A421E20D-3F20-FF4A-A250-792992ED1A42}">
   <dimension ref="A1:E181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="L84" sqref="L84"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
vault backup: 2022-01-06 00:13:33
Affected files:
1附件/权限列表.xlsx
</commit_message>
<xml_diff>
--- a/1附件/权限列表.xlsx
+++ b/1附件/权限列表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09228BB-50A1-6149-8635-4B69A5B36EE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA09C532-ABE2-D64B-9B56-6FEAE5C6B150}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="0" windowWidth="37460" windowHeight="21600" activeTab="9" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
+    <workbookView xWindow="940" yWindow="0" windowWidth="37460" windowHeight="21600" activeTab="11" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Mdm权限管理 (2)" sheetId="7" state="hidden" r:id="rId1"/>
@@ -23,9 +23,11 @@
     <sheet name="Uniauth数据字典" sheetId="13" r:id="rId8"/>
     <sheet name="Uniauth数据库脚本" sheetId="14" r:id="rId9"/>
     <sheet name="App权限管理" sheetId="3" r:id="rId10"/>
-    <sheet name="运营权限管理" sheetId="4" r:id="rId11"/>
-    <sheet name="运维权限管理" sheetId="5" r:id="rId12"/>
-    <sheet name="安全审核权限管理" sheetId="6" r:id="rId13"/>
+    <sheet name="App数据字典" sheetId="15" r:id="rId11"/>
+    <sheet name="App数据库脚本" sheetId="16" r:id="rId12"/>
+    <sheet name="运营权限管理" sheetId="4" r:id="rId13"/>
+    <sheet name="运维权限管理" sheetId="5" r:id="rId14"/>
+    <sheet name="安全审核权限管理" sheetId="6" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2914" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3151" uniqueCount="690">
   <si>
     <t>首页面板</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2291,6 +2293,299 @@
         <rFont val="JetBrains Mono"/>
       </rPr>
       <t>'1', 'funcId',</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>控制台</t>
+  </si>
+  <si>
+    <t>应用管理</t>
+  </si>
+  <si>
+    <t>创建应用</t>
+  </si>
+  <si>
+    <t>下架应用</t>
+  </si>
+  <si>
+    <t>升级应用</t>
+  </si>
+  <si>
+    <t>编辑安全策略</t>
+  </si>
+  <si>
+    <t>编辑发布策略</t>
+  </si>
+  <si>
+    <t>删除应用评价</t>
+  </si>
+  <si>
+    <t>上架应用</t>
+  </si>
+  <si>
+    <t>编辑应用</t>
+  </si>
+  <si>
+    <t>应用审核</t>
+  </si>
+  <si>
+    <t>撤回</t>
+  </si>
+  <si>
+    <t>提醒</t>
+  </si>
+  <si>
+    <t>申请</t>
+  </si>
+  <si>
+    <t>应用集市</t>
+  </si>
+  <si>
+    <t>上架</t>
+  </si>
+  <si>
+    <t>升级</t>
+  </si>
+  <si>
+    <t>部署统计</t>
+  </si>
+  <si>
+    <t>运行统计</t>
+  </si>
+  <si>
+    <t>活跃用户</t>
+  </si>
+  <si>
+    <t>安卓沙箱策略</t>
+  </si>
+  <si>
+    <t>添加策略</t>
+  </si>
+  <si>
+    <t>删除策略</t>
+  </si>
+  <si>
+    <t>编辑策略</t>
+  </si>
+  <si>
+    <t>推荐管理</t>
+  </si>
+  <si>
+    <t>添加推荐</t>
+  </si>
+  <si>
+    <t>修改推荐</t>
+  </si>
+  <si>
+    <t>系统日志</t>
+  </si>
+  <si>
+    <t>类别管理</t>
+  </si>
+  <si>
+    <t>添加类别</t>
+  </si>
+  <si>
+    <t>编辑类别</t>
+  </si>
+  <si>
+    <t>冻结类别</t>
+  </si>
+  <si>
+    <t>激活类别</t>
+  </si>
+  <si>
+    <t>标签管理</t>
+  </si>
+  <si>
+    <t>冻结</t>
+  </si>
+  <si>
+    <t>激活</t>
+  </si>
+  <si>
+    <t>编辑默认签名</t>
+  </si>
+  <si>
+    <t>remind</t>
+  </si>
+  <si>
+    <t>shelves</t>
+  </si>
+  <si>
+    <t>upgrade</t>
+  </si>
+  <si>
+    <t>download</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>freeze</t>
+  </si>
+  <si>
+    <t>Application_management</t>
+  </si>
+  <si>
+    <t>Create_app</t>
+  </si>
+  <si>
+    <t>The_shelves_application</t>
+  </si>
+  <si>
+    <t>Upgrade_application</t>
+  </si>
+  <si>
+    <t>Editing_a_Security_Policy</t>
+  </si>
+  <si>
+    <t>Edit_publish_strategy</t>
+  </si>
+  <si>
+    <t>Deleting_an_Application_Evaluation</t>
+  </si>
+  <si>
+    <t>On_the_application</t>
+  </si>
+  <si>
+    <t>Editor_application</t>
+  </si>
+  <si>
+    <t>Delete_the_application</t>
+  </si>
+  <si>
+    <t>Application_review</t>
+  </si>
+  <si>
+    <t>To_withdraw</t>
+  </si>
+  <si>
+    <t>To_apply_for</t>
+  </si>
+  <si>
+    <t>Application_of_the_market</t>
+  </si>
+  <si>
+    <t>Statistical_reports</t>
+  </si>
+  <si>
+    <t>The_deployment_of_statistical</t>
+  </si>
+  <si>
+    <t>Run_the_statistical</t>
+  </si>
+  <si>
+    <t>Active_users</t>
+  </si>
+  <si>
+    <t>Android_sandbox_strategy</t>
+  </si>
+  <si>
+    <t>Add_a_policy</t>
+  </si>
+  <si>
+    <t>Deletion_policy</t>
+  </si>
+  <si>
+    <t>Edit_policies</t>
+  </si>
+  <si>
+    <t>The_recommended_management</t>
+  </si>
+  <si>
+    <t>Add_the_recommended</t>
+  </si>
+  <si>
+    <t>Modify_the_recommended</t>
+  </si>
+  <si>
+    <t>The_system_log</t>
+  </si>
+  <si>
+    <t>Category_management</t>
+  </si>
+  <si>
+    <t>Add_category</t>
+  </si>
+  <si>
+    <t>Edit_category</t>
+  </si>
+  <si>
+    <t>Frozen_category</t>
+  </si>
+  <si>
+    <t>Activate_the_category</t>
+  </si>
+  <si>
+    <t>Label_management</t>
+  </si>
+  <si>
+    <t>The_activation</t>
+  </si>
+  <si>
+    <t>Editing_the_Default_Signature</t>
+  </si>
+  <si>
+    <t>The_console</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>'4'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>'funcId'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>'4', 'funcId',</t>
     </r>
     <r>
       <rPr>
@@ -3819,7 +4114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC44C7D-B5C9-8244-8110-B919A147507E}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -4160,6 +4455,2706 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25078354-96F9-7844-A29A-36E43FC30F16}">
+  <dimension ref="A1:F48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="96" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" t="s">
+        <v>602</v>
+      </c>
+      <c r="D1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="str">
+        <f>D2</f>
+        <v>read</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>595</v>
+      </c>
+      <c r="D2" t="str">
+        <f>LOWER(C2)</f>
+        <v>read</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"right."&amp;D2&amp;"="&amp;B2</f>
+        <v>right.read=查看</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"right."&amp;D2&amp;"="&amp;D2</f>
+        <v>right.read=read</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A48" si="0">D3</f>
+        <v>application_management</v>
+      </c>
+      <c r="B3" t="s">
+        <v>611</v>
+      </c>
+      <c r="C3" t="s">
+        <v>653</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D48" si="1">LOWER(C3)</f>
+        <v>application_management</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E48" si="2">"right."&amp;D3&amp;"="&amp;B3</f>
+        <v>right.application_management=应用管理</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F48" si="3">"right."&amp;D3&amp;"="&amp;D3</f>
+        <v>right.application_management=application_management</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>write</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>601</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>write</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="2"/>
+        <v>right.write=编辑</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="3"/>
+        <v>right.write=write</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>create_app</v>
+      </c>
+      <c r="B5" t="s">
+        <v>612</v>
+      </c>
+      <c r="C5" t="s">
+        <v>654</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>create_app</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="2"/>
+        <v>right.create_app=创建应用</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="3"/>
+        <v>right.create_app=create_app</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>the_shelves_application</v>
+      </c>
+      <c r="B6" t="s">
+        <v>613</v>
+      </c>
+      <c r="C6" t="s">
+        <v>655</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>the_shelves_application</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_shelves_application=下架应用</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="3"/>
+        <v>right.the_shelves_application=the_shelves_application</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>upgrade_application</v>
+      </c>
+      <c r="B7" t="s">
+        <v>614</v>
+      </c>
+      <c r="C7" t="s">
+        <v>656</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>upgrade_application</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="2"/>
+        <v>right.upgrade_application=升级应用</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="3"/>
+        <v>right.upgrade_application=upgrade_application</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>editing_a_security_policy</v>
+      </c>
+      <c r="B8" t="s">
+        <v>615</v>
+      </c>
+      <c r="C8" t="s">
+        <v>657</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>editing_a_security_policy</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="2"/>
+        <v>right.editing_a_security_policy=编辑安全策略</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="3"/>
+        <v>right.editing_a_security_policy=editing_a_security_policy</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>edit_publish_strategy</v>
+      </c>
+      <c r="B9" t="s">
+        <v>616</v>
+      </c>
+      <c r="C9" t="s">
+        <v>658</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>edit_publish_strategy</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="2"/>
+        <v>right.edit_publish_strategy=编辑发布策略</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="3"/>
+        <v>right.edit_publish_strategy=edit_publish_strategy</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>deleting_an_application_evaluation</v>
+      </c>
+      <c r="B10" t="s">
+        <v>617</v>
+      </c>
+      <c r="C10" t="s">
+        <v>659</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>deleting_an_application_evaluation</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="2"/>
+        <v>right.deleting_an_application_evaluation=删除应用评价</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="3"/>
+        <v>right.deleting_an_application_evaluation=deleting_an_application_evaluation</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>on_the_application</v>
+      </c>
+      <c r="B11" t="s">
+        <v>618</v>
+      </c>
+      <c r="C11" t="s">
+        <v>660</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>on_the_application</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="2"/>
+        <v>right.on_the_application=上架应用</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="3"/>
+        <v>right.on_the_application=on_the_application</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>editor_application</v>
+      </c>
+      <c r="B12" t="s">
+        <v>619</v>
+      </c>
+      <c r="C12" t="s">
+        <v>661</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>editor_application</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v>right.editor_application=编辑应用</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="3"/>
+        <v>right.editor_application=editor_application</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>delete_the_application</v>
+      </c>
+      <c r="B13" t="s">
+        <v>346</v>
+      </c>
+      <c r="C13" t="s">
+        <v>662</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>delete_the_application</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v>right.delete_the_application=删除应用</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="3"/>
+        <v>right.delete_the_application=delete_the_application</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>application_review</v>
+      </c>
+      <c r="B14" t="s">
+        <v>620</v>
+      </c>
+      <c r="C14" t="s">
+        <v>663</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>application_review</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
+        <v>right.application_review=应用审核</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="3"/>
+        <v>right.application_review=application_review</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>to_withdraw</v>
+      </c>
+      <c r="B15" t="s">
+        <v>621</v>
+      </c>
+      <c r="C15" t="s">
+        <v>664</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>to_withdraw</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="2"/>
+        <v>right.to_withdraw=撤回</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="3"/>
+        <v>right.to_withdraw=to_withdraw</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>remind</v>
+      </c>
+      <c r="B16" t="s">
+        <v>622</v>
+      </c>
+      <c r="C16" t="s">
+        <v>647</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>remind</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="2"/>
+        <v>right.remind=提醒</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="3"/>
+        <v>right.remind=remind</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>to_apply_for</v>
+      </c>
+      <c r="B17" t="s">
+        <v>623</v>
+      </c>
+      <c r="C17" t="s">
+        <v>665</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>to_apply_for</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="2"/>
+        <v>right.to_apply_for=申请</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="3"/>
+        <v>right.to_apply_for=to_apply_for</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>delete</v>
+      </c>
+      <c r="B18" t="s">
+        <v>350</v>
+      </c>
+      <c r="C18" t="s">
+        <v>536</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>delete</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
+        <v>right.delete=删除</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="3"/>
+        <v>right.delete=delete</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>application_of_the_market</v>
+      </c>
+      <c r="B19" t="s">
+        <v>624</v>
+      </c>
+      <c r="C19" t="s">
+        <v>666</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>application_of_the_market</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
+        <v>right.application_of_the_market=应用集市</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="3"/>
+        <v>right.application_of_the_market=application_of_the_market</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>shelves</v>
+      </c>
+      <c r="B20" t="s">
+        <v>625</v>
+      </c>
+      <c r="C20" t="s">
+        <v>648</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>shelves</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
+        <v>right.shelves=上架</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="3"/>
+        <v>right.shelves=shelves</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>upgrade</v>
+      </c>
+      <c r="B21" t="s">
+        <v>626</v>
+      </c>
+      <c r="C21" t="s">
+        <v>649</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>upgrade</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v>right.upgrade=升级</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="3"/>
+        <v>right.upgrade=upgrade</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>download</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>650</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>download</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="2"/>
+        <v>right.download=下载</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="3"/>
+        <v>right.download=download</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>statistical_reports</v>
+      </c>
+      <c r="B23" t="s">
+        <v>308</v>
+      </c>
+      <c r="C23" t="s">
+        <v>667</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>statistical_reports</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="2"/>
+        <v>right.statistical_reports=统计报表</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="3"/>
+        <v>right.statistical_reports=statistical_reports</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>the_deployment_of_statistical</v>
+      </c>
+      <c r="B24" t="s">
+        <v>627</v>
+      </c>
+      <c r="C24" t="s">
+        <v>668</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>the_deployment_of_statistical</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_deployment_of_statistical=部署统计</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="3"/>
+        <v>right.the_deployment_of_statistical=the_deployment_of_statistical</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>export</v>
+      </c>
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
+        <v>541</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>export</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="2"/>
+        <v>right.export=导出</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="3"/>
+        <v>right.export=export</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>run_the_statistical</v>
+      </c>
+      <c r="B26" t="s">
+        <v>628</v>
+      </c>
+      <c r="C26" t="s">
+        <v>669</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>run_the_statistical</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="2"/>
+        <v>right.run_the_statistical=运行统计</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="3"/>
+        <v>right.run_the_statistical=run_the_statistical</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v>active_users</v>
+      </c>
+      <c r="B27" t="s">
+        <v>629</v>
+      </c>
+      <c r="C27" t="s">
+        <v>670</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>active_users</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="2"/>
+        <v>right.active_users=活跃用户</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="3"/>
+        <v>right.active_users=active_users</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v>android_sandbox_strategy</v>
+      </c>
+      <c r="B28" t="s">
+        <v>630</v>
+      </c>
+      <c r="C28" t="s">
+        <v>671</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>android_sandbox_strategy</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="2"/>
+        <v>right.android_sandbox_strategy=安卓沙箱策略</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="3"/>
+        <v>right.android_sandbox_strategy=android_sandbox_strategy</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
+        <v>add_a_policy</v>
+      </c>
+      <c r="B29" t="s">
+        <v>631</v>
+      </c>
+      <c r="C29" t="s">
+        <v>672</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>add_a_policy</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="2"/>
+        <v>right.add_a_policy=添加策略</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="3"/>
+        <v>right.add_a_policy=add_a_policy</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="str">
+        <f t="shared" si="0"/>
+        <v>deletion_policy</v>
+      </c>
+      <c r="B30" t="s">
+        <v>632</v>
+      </c>
+      <c r="C30" t="s">
+        <v>673</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>deletion_policy</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="2"/>
+        <v>right.deletion_policy=删除策略</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="3"/>
+        <v>right.deletion_policy=deletion_policy</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="str">
+        <f t="shared" si="0"/>
+        <v>edit_policies</v>
+      </c>
+      <c r="B31" t="s">
+        <v>633</v>
+      </c>
+      <c r="C31" t="s">
+        <v>674</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>edit_policies</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="2"/>
+        <v>right.edit_policies=编辑策略</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="3"/>
+        <v>right.edit_policies=edit_policies</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="str">
+        <f t="shared" si="0"/>
+        <v>system_management</v>
+      </c>
+      <c r="B32" t="s">
+        <v>310</v>
+      </c>
+      <c r="C32" t="s">
+        <v>575</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>system_management</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="2"/>
+        <v>right.system_management=系统管理</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="3"/>
+        <v>right.system_management=system_management</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="str">
+        <f t="shared" si="0"/>
+        <v>the_recommended_management</v>
+      </c>
+      <c r="B33" t="s">
+        <v>634</v>
+      </c>
+      <c r="C33" t="s">
+        <v>675</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>the_recommended_management</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_recommended_management=推荐管理</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="3"/>
+        <v>right.the_recommended_management=the_recommended_management</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="str">
+        <f t="shared" si="0"/>
+        <v>add_the_recommended</v>
+      </c>
+      <c r="B34" t="s">
+        <v>635</v>
+      </c>
+      <c r="C34" t="s">
+        <v>676</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v>add_the_recommended</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="2"/>
+        <v>right.add_the_recommended=添加推荐</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="3"/>
+        <v>right.add_the_recommended=add_the_recommended</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="str">
+        <f t="shared" si="0"/>
+        <v>modify_the_recommended</v>
+      </c>
+      <c r="B35" t="s">
+        <v>636</v>
+      </c>
+      <c r="C35" t="s">
+        <v>677</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v>modify_the_recommended</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="2"/>
+        <v>right.modify_the_recommended=修改推荐</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="3"/>
+        <v>right.modify_the_recommended=modify_the_recommended</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="str">
+        <f t="shared" si="0"/>
+        <v>the_system_log</v>
+      </c>
+      <c r="B36" t="s">
+        <v>637</v>
+      </c>
+      <c r="C36" t="s">
+        <v>678</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v>the_system_log</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_system_log=系统日志</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="3"/>
+        <v>right.the_system_log=the_system_log</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="str">
+        <f t="shared" si="0"/>
+        <v>category_management</v>
+      </c>
+      <c r="B37" t="s">
+        <v>638</v>
+      </c>
+      <c r="C37" t="s">
+        <v>679</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v>category_management</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="2"/>
+        <v>right.category_management=类别管理</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="3"/>
+        <v>right.category_management=category_management</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="str">
+        <f t="shared" si="0"/>
+        <v>add_category</v>
+      </c>
+      <c r="B38" t="s">
+        <v>639</v>
+      </c>
+      <c r="C38" t="s">
+        <v>680</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v>add_category</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="2"/>
+        <v>right.add_category=添加类别</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="3"/>
+        <v>right.add_category=add_category</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="str">
+        <f t="shared" si="0"/>
+        <v>edit_category</v>
+      </c>
+      <c r="B39" t="s">
+        <v>640</v>
+      </c>
+      <c r="C39" t="s">
+        <v>681</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="1"/>
+        <v>edit_category</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="2"/>
+        <v>right.edit_category=编辑类别</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="3"/>
+        <v>right.edit_category=edit_category</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="str">
+        <f t="shared" si="0"/>
+        <v>frozen_category</v>
+      </c>
+      <c r="B40" t="s">
+        <v>641</v>
+      </c>
+      <c r="C40" t="s">
+        <v>682</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="1"/>
+        <v>frozen_category</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="2"/>
+        <v>right.frozen_category=冻结类别</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="3"/>
+        <v>right.frozen_category=frozen_category</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="str">
+        <f t="shared" si="0"/>
+        <v>activate_the_category</v>
+      </c>
+      <c r="B41" t="s">
+        <v>642</v>
+      </c>
+      <c r="C41" t="s">
+        <v>683</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="1"/>
+        <v>activate_the_category</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="2"/>
+        <v>right.activate_the_category=激活类别</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="3"/>
+        <v>right.activate_the_category=activate_the_category</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="str">
+        <f t="shared" si="0"/>
+        <v>label_management</v>
+      </c>
+      <c r="B42" t="s">
+        <v>643</v>
+      </c>
+      <c r="C42" t="s">
+        <v>684</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v>label_management</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="2"/>
+        <v>right.label_management=标签管理</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="3"/>
+        <v>right.label_management=label_management</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="str">
+        <f t="shared" si="0"/>
+        <v>add</v>
+      </c>
+      <c r="B43" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" t="s">
+        <v>651</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v>add</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="2"/>
+        <v>right.add=添加</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="3"/>
+        <v>right.add=add</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="str">
+        <f t="shared" si="0"/>
+        <v>freeze</v>
+      </c>
+      <c r="B44" t="s">
+        <v>644</v>
+      </c>
+      <c r="C44" t="s">
+        <v>652</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v>freeze</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="2"/>
+        <v>right.freeze=冻结</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="3"/>
+        <v>right.freeze=freeze</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="str">
+        <f t="shared" si="0"/>
+        <v>the_activation</v>
+      </c>
+      <c r="B45" t="s">
+        <v>645</v>
+      </c>
+      <c r="C45" t="s">
+        <v>685</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="1"/>
+        <v>the_activation</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_activation=激活</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="3"/>
+        <v>right.the_activation=the_activation</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="str">
+        <f t="shared" si="0"/>
+        <v>system_settings</v>
+      </c>
+      <c r="B46" t="s">
+        <v>392</v>
+      </c>
+      <c r="C46" t="s">
+        <v>576</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="1"/>
+        <v>system_settings</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="2"/>
+        <v>right.system_settings=系统设置</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="3"/>
+        <v>right.system_settings=system_settings</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="str">
+        <f t="shared" si="0"/>
+        <v>editing_the_default_signature</v>
+      </c>
+      <c r="B47" t="s">
+        <v>646</v>
+      </c>
+      <c r="C47" t="s">
+        <v>686</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="1"/>
+        <v>editing_the_default_signature</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="2"/>
+        <v>right.editing_the_default_signature=编辑默认签名</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="3"/>
+        <v>right.editing_the_default_signature=editing_the_default_signature</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="str">
+        <f t="shared" si="0"/>
+        <v>the_console</v>
+      </c>
+      <c r="B48" t="s">
+        <v>610</v>
+      </c>
+      <c r="C48" t="s">
+        <v>687</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="1"/>
+        <v>the_console</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_console=控制台</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="3"/>
+        <v>right.the_console=the_console</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729CB04B-3595-F94F-8768-A7FA5DE90163}">
+  <dimension ref="A1:E181"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4">
+        <v>362</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C1" t="str">
+        <f>B1&amp;""&amp;A1&amp;D1&amp;A1&amp;E1</f>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (362, '4', 'funcId',362);</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>688</v>
+      </c>
+      <c r="E1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4">
+        <v>363</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C65" si="0">B2&amp;""&amp;A2&amp;D2&amp;A2&amp;E2</f>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (363, '4', 'funcId',363);</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>688</v>
+      </c>
+      <c r="E2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4">
+        <v>364</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (364, '4', 'funcId',364);</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4">
+        <v>365</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (365, '4', 'funcId',365);</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E4" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4">
+        <v>366</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (366, '4', 'funcId',366);</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4">
+        <v>367</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (367, '4', 'funcId',367);</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4">
+        <v>368</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (368, '4', 'funcId',368);</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E7" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4">
+        <v>369</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (369, '4', 'funcId',369);</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E8" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4">
+        <v>370</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (370, '4', 'funcId',370);</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E9" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4">
+        <v>371</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (371, '4', 'funcId',371);</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E10" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4">
+        <v>372</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (372, '4', 'funcId',372);</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E11" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4">
+        <v>373</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (373, '4', 'funcId',373);</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E12" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4">
+        <v>374</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (374, '4', 'funcId',374);</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E13" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4">
+        <v>375</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (375, '4', 'funcId',375);</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E14" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4">
+        <v>376</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (376, '4', 'funcId',376);</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E15" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4">
+        <v>377</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (377, '4', 'funcId',377);</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E16" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4">
+        <v>378</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (378, '4', 'funcId',378);</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E17" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4">
+        <v>379</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (379, '4', 'funcId',379);</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E18" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4">
+        <v>380</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (380, '4', 'funcId',380);</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E19" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4">
+        <v>381</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (381, '4', 'funcId',381);</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E20" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4">
+        <v>382</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (382, '4', 'funcId',382);</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E21" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4">
+        <v>383</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (383, '4', 'funcId',383);</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E22" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4">
+        <v>384</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (384, '4', 'funcId',384);</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E23" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4">
+        <v>385</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (385, '4', 'funcId',385);</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E24" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4">
+        <v>386</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (386, '4', 'funcId',386);</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E25" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="4">
+        <v>387</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (387, '4', 'funcId',387);</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E26" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4">
+        <v>388</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (388, '4', 'funcId',388);</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E27" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4">
+        <v>389</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (389, '4', 'funcId',389);</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E28" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="4">
+        <v>390</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (390, '4', 'funcId',390);</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E29" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="4">
+        <v>391</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (391, '4', 'funcId',391);</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E30" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4">
+        <v>392</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (392, '4', 'funcId',392);</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E31" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4">
+        <v>393</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (393, '4', 'funcId',393);</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E32" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4">
+        <v>394</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (394, '4', 'funcId',394);</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E33" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4">
+        <v>395</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (395, '4', 'funcId',395);</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E34" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="4">
+        <v>396</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (396, '4', 'funcId',396);</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E35" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4">
+        <v>397</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (397, '4', 'funcId',397);</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E36" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4">
+        <v>398</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (398, '4', 'funcId',398);</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E37" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4">
+        <v>399</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (399, '4', 'funcId',399);</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E38" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="4">
+        <v>400</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (400, '4', 'funcId',400);</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E39" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="4">
+        <v>401</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (401, '4', 'funcId',401);</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E40" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="4">
+        <v>402</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (402, '4', 'funcId',402);</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E41" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="4">
+        <v>403</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (403, '4', 'funcId',403);</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E42" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="4">
+        <v>404</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (404, '4', 'funcId',404);</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E43" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="4">
+        <v>405</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (405, '4', 'funcId',405);</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E44" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="4">
+        <v>406</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (406, '4', 'funcId',406);</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E45" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="4">
+        <v>407</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (407, '4', 'funcId',407);</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E46" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="4">
+        <v>408</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (408, '4', 'funcId',408);</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>689</v>
+      </c>
+      <c r="E47" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="D55" s="4"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="D56" s="4"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="D58" s="4"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="D59" s="4"/>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="D60" s="4"/>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="D61" s="4"/>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="D62" s="4"/>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="D63" s="4"/>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="D64" s="4"/>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="D65" s="4"/>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="D66" s="4"/>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="D67" s="4"/>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="D68" s="4"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="D69" s="4"/>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="D70" s="4"/>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="D71" s="4"/>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="D72" s="4"/>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="D73" s="4"/>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="D74" s="4"/>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="D75" s="4"/>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="D76" s="4"/>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="D77" s="4"/>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="D78" s="4"/>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="D79" s="4"/>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="D80" s="4"/>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+      <c r="D81" s="4"/>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="D82" s="4"/>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="D83" s="4"/>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
+      <c r="D84" s="4"/>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
+      <c r="D85" s="4"/>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="D86" s="4"/>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="D87" s="4"/>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="D88" s="4"/>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="D89" s="4"/>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="D90" s="4"/>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="D91" s="4"/>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="D92" s="4"/>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="D93" s="4"/>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="D94" s="4"/>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="D95" s="4"/>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="D96" s="4"/>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="D97" s="4"/>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="D98" s="4"/>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="D99" s="4"/>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="D100" s="4"/>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="D101" s="4"/>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="D102" s="4"/>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="D103" s="4"/>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="D104" s="4"/>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="D105" s="4"/>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4"/>
+      <c r="D106" s="4"/>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="D107" s="4"/>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="D108" s="4"/>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="D109" s="4"/>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="D110" s="4"/>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="D111" s="4"/>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="D112" s="4"/>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+      <c r="D113" s="4"/>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="4"/>
+      <c r="B114" s="4"/>
+      <c r="D114" s="4"/>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="4"/>
+      <c r="B115" s="4"/>
+      <c r="D115" s="4"/>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="4"/>
+      <c r="B116" s="4"/>
+      <c r="D116" s="4"/>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="4"/>
+      <c r="B117" s="4"/>
+      <c r="D117" s="4"/>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="D118" s="4"/>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+      <c r="D119" s="4"/>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="D120" s="4"/>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+      <c r="D121" s="4"/>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="4"/>
+      <c r="B122" s="4"/>
+      <c r="D122" s="4"/>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="4"/>
+      <c r="B123" s="4"/>
+      <c r="D123" s="4"/>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="4"/>
+      <c r="B124" s="4"/>
+      <c r="D124" s="4"/>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="4"/>
+      <c r="B125" s="4"/>
+      <c r="D125" s="4"/>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="4"/>
+      <c r="B126" s="4"/>
+      <c r="D126" s="4"/>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="4"/>
+      <c r="B127" s="4"/>
+      <c r="D127" s="4"/>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="4"/>
+      <c r="B128" s="4"/>
+      <c r="D128" s="4"/>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="4"/>
+      <c r="B129" s="4"/>
+      <c r="D129" s="4"/>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="4"/>
+      <c r="B130" s="4"/>
+      <c r="D130" s="4"/>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="4"/>
+      <c r="B131" s="4"/>
+      <c r="D131" s="4"/>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="4"/>
+      <c r="B132" s="4"/>
+      <c r="D132" s="4"/>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="4"/>
+      <c r="B133" s="4"/>
+      <c r="D133" s="4"/>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="4"/>
+      <c r="B134" s="4"/>
+      <c r="D134" s="4"/>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="4"/>
+      <c r="B135" s="4"/>
+      <c r="D135" s="4"/>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="4"/>
+      <c r="B136" s="4"/>
+      <c r="D136" s="4"/>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="4"/>
+      <c r="B137" s="4"/>
+      <c r="D137" s="4"/>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="4"/>
+      <c r="B138" s="4"/>
+      <c r="D138" s="4"/>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="4"/>
+      <c r="B139" s="4"/>
+      <c r="D139" s="4"/>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="4"/>
+      <c r="B140" s="4"/>
+      <c r="D140" s="4"/>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="4"/>
+      <c r="B141" s="4"/>
+      <c r="D141" s="4"/>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="4"/>
+      <c r="B142" s="4"/>
+      <c r="D142" s="4"/>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="4"/>
+      <c r="B143" s="4"/>
+      <c r="D143" s="4"/>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="4"/>
+      <c r="B144" s="4"/>
+      <c r="D144" s="4"/>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="4"/>
+      <c r="B145" s="4"/>
+      <c r="D145" s="4"/>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="4"/>
+      <c r="B146" s="4"/>
+      <c r="D146" s="4"/>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="4"/>
+      <c r="B147" s="4"/>
+      <c r="D147" s="4"/>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="4"/>
+      <c r="B148" s="4"/>
+      <c r="D148" s="4"/>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="4"/>
+      <c r="B149" s="4"/>
+      <c r="D149" s="4"/>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="4"/>
+      <c r="B150" s="4"/>
+      <c r="D150" s="4"/>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="4"/>
+      <c r="B151" s="4"/>
+      <c r="D151" s="4"/>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="4"/>
+      <c r="B152" s="4"/>
+      <c r="D152" s="4"/>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="4"/>
+      <c r="B153" s="4"/>
+      <c r="D153" s="4"/>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="4"/>
+      <c r="B154" s="4"/>
+      <c r="D154" s="4"/>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="4"/>
+      <c r="B155" s="4"/>
+      <c r="D155" s="4"/>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="4"/>
+      <c r="B156" s="4"/>
+      <c r="D156" s="4"/>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="4"/>
+      <c r="B157" s="4"/>
+      <c r="D157" s="4"/>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="4"/>
+      <c r="B158" s="4"/>
+      <c r="D158" s="4"/>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="4"/>
+      <c r="B159" s="4"/>
+      <c r="D159" s="4"/>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="4"/>
+      <c r="B160" s="4"/>
+      <c r="D160" s="4"/>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="4"/>
+      <c r="B161" s="4"/>
+      <c r="D161" s="4"/>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="4"/>
+      <c r="B162" s="4"/>
+      <c r="D162" s="4"/>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="4"/>
+      <c r="B163" s="4"/>
+      <c r="D163" s="4"/>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" s="4"/>
+      <c r="B164" s="4"/>
+      <c r="D164" s="4"/>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="4"/>
+      <c r="B165" s="4"/>
+      <c r="D165" s="4"/>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="4"/>
+      <c r="B166" s="4"/>
+      <c r="D166" s="4"/>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="4"/>
+      <c r="B167" s="4"/>
+      <c r="D167" s="4"/>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" s="4"/>
+      <c r="B168" s="4"/>
+      <c r="D168" s="4"/>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" s="4"/>
+      <c r="B169" s="4"/>
+      <c r="D169" s="4"/>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" s="4"/>
+      <c r="B170" s="4"/>
+      <c r="D170" s="4"/>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" s="4"/>
+      <c r="B171" s="4"/>
+      <c r="D171" s="4"/>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" s="4"/>
+      <c r="B172" s="4"/>
+      <c r="D172" s="4"/>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" s="4"/>
+      <c r="B173" s="4"/>
+      <c r="D173" s="4"/>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" s="4"/>
+      <c r="B174" s="4"/>
+      <c r="D174" s="4"/>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" s="4"/>
+      <c r="B175" s="4"/>
+      <c r="D175" s="4"/>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="4"/>
+      <c r="B176" s="4"/>
+      <c r="D176" s="4"/>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" s="4"/>
+      <c r="B177" s="4"/>
+      <c r="D177" s="4"/>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" s="4"/>
+      <c r="B178" s="4"/>
+      <c r="D178" s="4"/>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" s="4"/>
+      <c r="B179" s="4"/>
+      <c r="D179" s="4"/>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" s="4"/>
+      <c r="B180" s="4"/>
+      <c r="D180" s="4"/>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" s="4"/>
+      <c r="B181" s="4"/>
+      <c r="D181" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B3B789-6212-894F-BA86-A23B372BEE33}">
   <dimension ref="A1:G22"/>
   <sheetViews>
@@ -4455,7 +7450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F9AB08-A3B8-514B-AD13-E0375A045A1B}">
   <dimension ref="A1:G36"/>
   <sheetViews>
@@ -4903,7 +7898,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89C31BD-9216-6A49-8C90-0ADAF2498DB4}">
   <dimension ref="A1:D14"/>
   <sheetViews>

</xml_diff>

<commit_message>
vault backup: 2022-01-07 10:33:39
Affected files:
14TODO/TODO.md
1附件/权限列表.xlsx
</commit_message>
<xml_diff>
--- a/1附件/权限列表.xlsx
+++ b/1附件/权限列表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA09C532-ABE2-D64B-9B56-6FEAE5C6B150}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0800894-4EA3-BF4E-97BB-30FEAD957A2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="0" windowWidth="37460" windowHeight="21600" activeTab="11" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
+    <workbookView xWindow="900" yWindow="0" windowWidth="37500" windowHeight="21600" activeTab="15" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Mdm权限管理 (2)" sheetId="7" state="hidden" r:id="rId1"/>
@@ -26,8 +26,10 @@
     <sheet name="App数据字典" sheetId="15" r:id="rId11"/>
     <sheet name="App数据库脚本" sheetId="16" r:id="rId12"/>
     <sheet name="运营权限管理" sheetId="4" r:id="rId13"/>
-    <sheet name="运维权限管理" sheetId="5" r:id="rId14"/>
-    <sheet name="安全审核权限管理" sheetId="6" r:id="rId15"/>
+    <sheet name="运营数据字典" sheetId="18" r:id="rId14"/>
+    <sheet name="运维权限管理" sheetId="5" r:id="rId15"/>
+    <sheet name="运维数据字典" sheetId="19" r:id="rId16"/>
+    <sheet name="安全审核权限管理" sheetId="6" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3151" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3317" uniqueCount="799">
   <si>
     <t>首页面板</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2595,6 +2597,333 @@
       </rPr>
       <t/>
     </r>
+  </si>
+  <si>
+    <t>平台概况</t>
+  </si>
+  <si>
+    <t>平台资源</t>
+  </si>
+  <si>
+    <t>平台运营</t>
+  </si>
+  <si>
+    <t>租户管理</t>
+  </si>
+  <si>
+    <t>普通租户管理</t>
+  </si>
+  <si>
+    <t>创建租户</t>
+  </si>
+  <si>
+    <t>停用租户</t>
+  </si>
+  <si>
+    <t>编辑租户</t>
+  </si>
+  <si>
+    <t>注销租户</t>
+  </si>
+  <si>
+    <t>导出用户列表</t>
+  </si>
+  <si>
+    <t>同步日志</t>
+  </si>
+  <si>
+    <t>导出租户失败记录</t>
+  </si>
+  <si>
+    <t>导出用户失败记录</t>
+  </si>
+  <si>
+    <t>服务管理</t>
+  </si>
+  <si>
+    <t>服务列表</t>
+  </si>
+  <si>
+    <t>添加服务</t>
+  </si>
+  <si>
+    <t>删除服务</t>
+  </si>
+  <si>
+    <t>编辑服务</t>
+  </si>
+  <si>
+    <t>编辑授权提醒设置</t>
+  </si>
+  <si>
+    <t>编辑资源使用限制</t>
+  </si>
+  <si>
+    <t>平台授权信息</t>
+  </si>
+  <si>
+    <t>双因素认证设置</t>
+  </si>
+  <si>
+    <t>编辑短信认证总开关</t>
+  </si>
+  <si>
+    <t>批量设置双因素认证</t>
+  </si>
+  <si>
+    <t>设置双因素认证</t>
+  </si>
+  <si>
+    <t>Application/SDK</t>
+  </si>
+  <si>
+    <t>Platform_overview</t>
+  </si>
+  <si>
+    <t>To_view</t>
+  </si>
+  <si>
+    <t>Platform_resources</t>
+  </si>
+  <si>
+    <t>Platform_operation</t>
+  </si>
+  <si>
+    <t>Tenant_management</t>
+  </si>
+  <si>
+    <t>Common_Tenant_Management</t>
+  </si>
+  <si>
+    <t>The_editor</t>
+  </si>
+  <si>
+    <t>Create_a_tenant</t>
+  </si>
+  <si>
+    <t>Stop_using_the_tenant</t>
+  </si>
+  <si>
+    <t>Edit_the_tenant</t>
+  </si>
+  <si>
+    <t>The_cancellation_of_the_tenant</t>
+  </si>
+  <si>
+    <t>Cb_Tenant_Management</t>
+  </si>
+  <si>
+    <t>Exporting_a_User_List</t>
+  </si>
+  <si>
+    <t>User_management</t>
+  </si>
+  <si>
+    <t>Synchronous_log</t>
+  </si>
+  <si>
+    <t>Failed_to_export_vstore_records</t>
+  </si>
+  <si>
+    <t>Failed_to_export_user_logs</t>
+  </si>
+  <si>
+    <t>Service_management</t>
+  </si>
+  <si>
+    <t>Service_list</t>
+  </si>
+  <si>
+    <t>Add_the_service</t>
+  </si>
+  <si>
+    <t>Remove_the_service</t>
+  </si>
+  <si>
+    <t>Editing_service</t>
+  </si>
+  <si>
+    <t>Edit_authorization_alert_Settings</t>
+  </si>
+  <si>
+    <t>Edit_resource_usage_restrictions</t>
+  </si>
+  <si>
+    <t>Platform_Authorization_Information</t>
+  </si>
+  <si>
+    <t>Two-factor_authentication_setting</t>
+  </si>
+  <si>
+    <t>Edit_the_main_switch_of_SMS_authentication</t>
+  </si>
+  <si>
+    <t>Configure_two-factor_authentication_in_batches</t>
+  </si>
+  <si>
+    <t>Configure_two-factor_authentication</t>
+  </si>
+  <si>
+    <t>监控管理</t>
+  </si>
+  <si>
+    <t>服务器</t>
+  </si>
+  <si>
+    <t>服务</t>
+  </si>
+  <si>
+    <t>告警事件</t>
+  </si>
+  <si>
+    <t>发送</t>
+  </si>
+  <si>
+    <t>恢复</t>
+  </si>
+  <si>
+    <t>事件统计</t>
+  </si>
+  <si>
+    <t>租户日志管理</t>
+  </si>
+  <si>
+    <t>应用图标管理</t>
+  </si>
+  <si>
+    <t>查找设备</t>
+  </si>
+  <si>
+    <t>监控设置</t>
+  </si>
+  <si>
+    <t>短信通知管理</t>
+  </si>
+  <si>
+    <t>保存短信通知设置</t>
+  </si>
+  <si>
+    <t>下载限制设置</t>
+  </si>
+  <si>
+    <t>设备日志下载</t>
+  </si>
+  <si>
+    <t>网关调用日志</t>
+  </si>
+  <si>
+    <t>上传客户端</t>
+  </si>
+  <si>
+    <t>推送</t>
+  </si>
+  <si>
+    <t>BYOD客户端升级</t>
+  </si>
+  <si>
+    <t>IOS客户端升级</t>
+  </si>
+  <si>
+    <t>租户意见反馈</t>
+  </si>
+  <si>
+    <t>Android意见反馈</t>
+  </si>
+  <si>
+    <t>IOS意见反馈</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>send</t>
+  </si>
+  <si>
+    <t>restore</t>
+  </si>
+  <si>
+    <t>push</t>
+  </si>
+  <si>
+    <t>reply</t>
+  </si>
+  <si>
+    <t>ignore</t>
+  </si>
+  <si>
+    <t>Monitoring_management</t>
+  </si>
+  <si>
+    <t>The_server</t>
+  </si>
+  <si>
+    <t>Modify_the</t>
+  </si>
+  <si>
+    <t>The_alarm_event</t>
+  </si>
+  <si>
+    <t>Event_statistics</t>
+  </si>
+  <si>
+    <t>Tenant_Log_Management</t>
+  </si>
+  <si>
+    <t>Application_Icon_Management</t>
+  </si>
+  <si>
+    <t>Find_equipment</t>
+  </si>
+  <si>
+    <t>Monitor_setting</t>
+  </si>
+  <si>
+    <t>SMS_Notification_Management</t>
+  </si>
+  <si>
+    <t>Save_SMS_notification_Settings</t>
+  </si>
+  <si>
+    <t>Download_Limit_Settings</t>
+  </si>
+  <si>
+    <t>Downloading_Device_Logs</t>
+  </si>
+  <si>
+    <t>Gateway_Call_log</t>
+  </si>
+  <si>
+    <t>COPE_client_upgrade</t>
+  </si>
+  <si>
+    <t>Uploading_a_Client</t>
+  </si>
+  <si>
+    <t>Upgrade_the_BYOD_client</t>
+  </si>
+  <si>
+    <t>The_IOS_client_is_upgraded</t>
+  </si>
+  <si>
+    <t>Tenant_Feedback</t>
+  </si>
+  <si>
+    <t>Android_Feedback</t>
+  </si>
+  <si>
+    <t>IOS_Feedback</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>code</t>
   </si>
 </sst>
 </file>
@@ -4115,7 +4444,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5619,7 +5948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729CB04B-3595-F94F-8768-A7FA5DE90163}">
   <dimension ref="A1:E181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
@@ -5657,7 +5986,7 @@
         <v>412</v>
       </c>
       <c r="C2" t="str">
-        <f t="shared" ref="C2:C65" si="0">B2&amp;""&amp;A2&amp;D2&amp;A2&amp;E2</f>
+        <f t="shared" ref="C2:C47" si="0">B2&amp;""&amp;A2&amp;D2&amp;A2&amp;E2</f>
         <v>INSERT INTO `fine_auth_perm_relation` VALUES (363, '4', 'funcId',363);</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -7156,10 +7485,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B3B789-6212-894F-BA86-A23B372BEE33}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7173,21 +7502,24 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>90</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>231</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="B2" t="s">
-        <v>232</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -7198,7 +7530,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -7208,11 +7540,8 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>234</v>
-      </c>
       <c r="B4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -7223,10 +7552,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -7236,158 +7565,161 @@
       </c>
     </row>
     <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" t="s">
+        <v>235</v>
+      </c>
       <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>236</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>237</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>238</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
         <v>240</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>234</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="C8" t="s">
+    <row r="9" spans="1:7">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>76</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>241</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>242</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="B9" t="s">
+    <row r="10" spans="1:7">
+      <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="C10" t="s">
+    <row r="11" spans="1:7">
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="B11" t="s">
+    <row r="12" spans="1:7">
+      <c r="B12" t="s">
         <v>244</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="C12" t="s">
+    <row r="13" spans="1:7">
+      <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>245</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
         <v>247</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>248</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="C14" t="s">
+    <row r="15" spans="1:7">
+      <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>249</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>250</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="B15" t="s">
+    <row r="16" spans="1:7">
+      <c r="B16" t="s">
         <v>252</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>2</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="C16" t="s">
+    <row r="17" spans="1:6">
+      <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
         <v>104</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>99</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="B18" t="s">
-        <v>105</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -7397,30 +7729,30 @@
       </c>
     </row>
     <row r="19" spans="1:6">
+      <c r="B19" t="s">
+        <v>105</v>
+      </c>
       <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="C20" t="s">
         <v>8</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>253</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>254</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="B20" t="s">
-        <v>255</v>
-      </c>
-      <c r="C20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="B21" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -7430,16 +7762,27 @@
       </c>
     </row>
     <row r="22" spans="1:6">
+      <c r="B22" t="s">
+        <v>286</v>
+      </c>
       <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="C23" t="s">
         <v>8</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>287</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>289</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
         <v>288</v>
       </c>
     </row>
@@ -7451,11 +7794,956 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F9AB08-A3B8-514B-AD13-E0375A045A1B}">
-  <dimension ref="A1:G36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884E44BC-9319-B840-B499-063BCB3FAB83}">
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="B43" sqref="B43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" customWidth="1"/>
+    <col min="6" max="6" width="96" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" t="s">
+        <v>602</v>
+      </c>
+      <c r="D1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="str">
+        <f>D2</f>
+        <v>statistical_reports</v>
+      </c>
+      <c r="B2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C2" t="s">
+        <v>667</v>
+      </c>
+      <c r="D2" t="str">
+        <f>LOWER(C2)</f>
+        <v>statistical_reports</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"right."&amp;D2&amp;"="&amp;B2</f>
+        <v>right.statistical_reports=统计报表</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"right."&amp;D2&amp;"="&amp;D2</f>
+        <v>right.statistical_reports=statistical_reports</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="str">
+        <f>D3</f>
+        <v>platform_overview</v>
+      </c>
+      <c r="B3" t="s">
+        <v>690</v>
+      </c>
+      <c r="C3" t="s">
+        <v>716</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D39" si="0">LOWER(C3)</f>
+        <v>platform_overview</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E39" si="1">"right."&amp;D3&amp;"="&amp;B3</f>
+        <v>right.platform_overview=平台概况</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F39" si="2">"right."&amp;D3&amp;"="&amp;D3</f>
+        <v>right.platform_overview=platform_overview</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A39" si="3">D4</f>
+        <v>to_view</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>717</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>to_view</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>right.to_view=查看</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="2"/>
+        <v>right.to_view=to_view</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="str">
+        <f t="shared" si="3"/>
+        <v>platform_resources</v>
+      </c>
+      <c r="B5" t="s">
+        <v>691</v>
+      </c>
+      <c r="C5" t="s">
+        <v>718</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>platform_resources</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>right.platform_resources=平台资源</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="2"/>
+        <v>right.platform_resources=platform_resources</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="str">
+        <f t="shared" si="3"/>
+        <v>platform_operation</v>
+      </c>
+      <c r="B6" t="s">
+        <v>692</v>
+      </c>
+      <c r="C6" t="s">
+        <v>719</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>platform_operation</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>right.platform_operation=平台运营</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="2"/>
+        <v>right.platform_operation=platform_operation</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="str">
+        <f t="shared" si="3"/>
+        <v>tenant_management</v>
+      </c>
+      <c r="B7" t="s">
+        <v>693</v>
+      </c>
+      <c r="C7" t="s">
+        <v>720</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>tenant_management</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>right.tenant_management=租户管理</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="2"/>
+        <v>right.tenant_management=tenant_management</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="str">
+        <f t="shared" si="3"/>
+        <v>common_tenant_management</v>
+      </c>
+      <c r="B8" t="s">
+        <v>694</v>
+      </c>
+      <c r="C8" t="s">
+        <v>721</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>common_tenant_management</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>right.common_tenant_management=普通租户管理</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="2"/>
+        <v>right.common_tenant_management=common_tenant_management</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="str">
+        <f t="shared" si="3"/>
+        <v>the_editor</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>722</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>the_editor</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>right.the_editor=编辑</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_editor=the_editor</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="str">
+        <f t="shared" si="3"/>
+        <v>create_a_tenant</v>
+      </c>
+      <c r="B10" t="s">
+        <v>695</v>
+      </c>
+      <c r="C10" t="s">
+        <v>723</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>create_a_tenant</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>right.create_a_tenant=创建租户</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="2"/>
+        <v>right.create_a_tenant=create_a_tenant</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="str">
+        <f t="shared" si="3"/>
+        <v>stop_using_the_tenant</v>
+      </c>
+      <c r="B11" t="s">
+        <v>696</v>
+      </c>
+      <c r="C11" t="s">
+        <v>724</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>stop_using_the_tenant</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>right.stop_using_the_tenant=停用租户</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="2"/>
+        <v>right.stop_using_the_tenant=stop_using_the_tenant</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="str">
+        <f t="shared" si="3"/>
+        <v>edit_the_tenant</v>
+      </c>
+      <c r="B12" t="s">
+        <v>697</v>
+      </c>
+      <c r="C12" t="s">
+        <v>725</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>edit_the_tenant</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>right.edit_the_tenant=编辑租户</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="2"/>
+        <v>right.edit_the_tenant=edit_the_tenant</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="str">
+        <f t="shared" si="3"/>
+        <v>the_cancellation_of_the_tenant</v>
+      </c>
+      <c r="B13" t="s">
+        <v>698</v>
+      </c>
+      <c r="C13" t="s">
+        <v>726</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>the_cancellation_of_the_tenant</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>right.the_cancellation_of_the_tenant=注销租户</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_cancellation_of_the_tenant=the_cancellation_of_the_tenant</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="str">
+        <f t="shared" si="3"/>
+        <v>cb_tenant_management</v>
+      </c>
+      <c r="B14" t="s">
+        <v>240</v>
+      </c>
+      <c r="C14" t="s">
+        <v>727</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>cb_tenant_management</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>right.cb_tenant_management=CB租户管理</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="2"/>
+        <v>right.cb_tenant_management=cb_tenant_management</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="str">
+        <f t="shared" si="3"/>
+        <v>export</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>541</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>export</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>right.export=导出</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="2"/>
+        <v>right.export=export</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="str">
+        <f t="shared" si="3"/>
+        <v>open</v>
+      </c>
+      <c r="B16" t="s">
+        <v>527</v>
+      </c>
+      <c r="C16" t="s">
+        <v>542</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>open</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>right.open=开通</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="2"/>
+        <v>right.open=open</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="str">
+        <f t="shared" si="3"/>
+        <v>unsubscribe</v>
+      </c>
+      <c r="B17" t="s">
+        <v>529</v>
+      </c>
+      <c r="C17" t="s">
+        <v>543</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>unsubscribe</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>right.unsubscribe=退订</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="2"/>
+        <v>right.unsubscribe=unsubscribe</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="str">
+        <f t="shared" si="3"/>
+        <v>exporting_a_user_list</v>
+      </c>
+      <c r="B18" t="s">
+        <v>699</v>
+      </c>
+      <c r="C18" t="s">
+        <v>728</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>exporting_a_user_list</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>right.exporting_a_user_list=导出用户列表</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="2"/>
+        <v>right.exporting_a_user_list=exporting_a_user_list</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="str">
+        <f t="shared" si="3"/>
+        <v>user_management</v>
+      </c>
+      <c r="B19" t="s">
+        <v>292</v>
+      </c>
+      <c r="C19" t="s">
+        <v>729</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>user_management</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>right.user_management=用户管理</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="2"/>
+        <v>right.user_management=user_management</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="str">
+        <f t="shared" si="3"/>
+        <v>synchronous_log</v>
+      </c>
+      <c r="B20" t="s">
+        <v>700</v>
+      </c>
+      <c r="C20" t="s">
+        <v>730</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>synchronous_log</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>right.synchronous_log=同步日志</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="2"/>
+        <v>right.synchronous_log=synchronous_log</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="str">
+        <f t="shared" si="3"/>
+        <v>failed_to_export_vstore_records</v>
+      </c>
+      <c r="B21" t="s">
+        <v>701</v>
+      </c>
+      <c r="C21" t="s">
+        <v>731</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>failed_to_export_vstore_records</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>right.failed_to_export_vstore_records=导出租户失败记录</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="2"/>
+        <v>right.failed_to_export_vstore_records=failed_to_export_vstore_records</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="str">
+        <f t="shared" si="3"/>
+        <v>failed_to_export_user_logs</v>
+      </c>
+      <c r="B22" t="s">
+        <v>702</v>
+      </c>
+      <c r="C22" t="s">
+        <v>732</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>failed_to_export_user_logs</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>right.failed_to_export_user_logs=导出用户失败记录</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="2"/>
+        <v>right.failed_to_export_user_logs=failed_to_export_user_logs</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="str">
+        <f t="shared" si="3"/>
+        <v>service_management</v>
+      </c>
+      <c r="B23" t="s">
+        <v>703</v>
+      </c>
+      <c r="C23" t="s">
+        <v>733</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>service_management</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>right.service_management=服务管理</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="2"/>
+        <v>right.service_management=service_management</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="str">
+        <f t="shared" si="3"/>
+        <v>service_list</v>
+      </c>
+      <c r="B24" t="s">
+        <v>704</v>
+      </c>
+      <c r="C24" t="s">
+        <v>734</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>service_list</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>right.service_list=服务列表</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="2"/>
+        <v>right.service_list=service_list</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="str">
+        <f t="shared" si="3"/>
+        <v>add_the_service</v>
+      </c>
+      <c r="B25" t="s">
+        <v>705</v>
+      </c>
+      <c r="C25" t="s">
+        <v>735</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>add_the_service</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>right.add_the_service=添加服务</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="2"/>
+        <v>right.add_the_service=add_the_service</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="str">
+        <f t="shared" si="3"/>
+        <v>remove_the_service</v>
+      </c>
+      <c r="B26" t="s">
+        <v>706</v>
+      </c>
+      <c r="C26" t="s">
+        <v>736</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>remove_the_service</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>right.remove_the_service=删除服务</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="2"/>
+        <v>right.remove_the_service=remove_the_service</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="str">
+        <f t="shared" si="3"/>
+        <v>editing_service</v>
+      </c>
+      <c r="B27" t="s">
+        <v>707</v>
+      </c>
+      <c r="C27" t="s">
+        <v>737</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>editing_service</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>right.editing_service=编辑服务</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="2"/>
+        <v>right.editing_service=editing_service</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="str">
+        <f t="shared" si="3"/>
+        <v>application/sdk</v>
+      </c>
+      <c r="B28" t="s">
+        <v>252</v>
+      </c>
+      <c r="C28" t="s">
+        <v>715</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>application/sdk</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>right.application/sdk=应用/SDK</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="2"/>
+        <v>right.application/sdk=application/sdk</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="str">
+        <f t="shared" si="3"/>
+        <v>upgrade</v>
+      </c>
+      <c r="B29" t="s">
+        <v>626</v>
+      </c>
+      <c r="C29" t="s">
+        <v>649</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>upgrade</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>right.upgrade=升级</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="2"/>
+        <v>right.upgrade=upgrade</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="str">
+        <f t="shared" si="3"/>
+        <v>system_management</v>
+      </c>
+      <c r="B30" t="s">
+        <v>310</v>
+      </c>
+      <c r="C30" t="s">
+        <v>575</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>system_management</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>right.system_management=系统管理</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="2"/>
+        <v>right.system_management=system_management</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="str">
+        <f t="shared" si="3"/>
+        <v>administrator_operation_logs</v>
+      </c>
+      <c r="B31" t="s">
+        <v>387</v>
+      </c>
+      <c r="C31" t="s">
+        <v>574</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>administrator_operation_logs</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>right.administrator_operation_logs=管理员操作日志</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="2"/>
+        <v>right.administrator_operation_logs=administrator_operation_logs</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="str">
+        <f t="shared" si="3"/>
+        <v>system_settings</v>
+      </c>
+      <c r="B32" t="s">
+        <v>392</v>
+      </c>
+      <c r="C32" t="s">
+        <v>576</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>system_settings</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>right.system_settings=系统设置</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="2"/>
+        <v>right.system_settings=system_settings</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="str">
+        <f t="shared" si="3"/>
+        <v>edit_authorization_alert_settings</v>
+      </c>
+      <c r="B33" t="s">
+        <v>708</v>
+      </c>
+      <c r="C33" t="s">
+        <v>738</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>edit_authorization_alert_settings</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>right.edit_authorization_alert_settings=编辑授权提醒设置</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="2"/>
+        <v>right.edit_authorization_alert_settings=edit_authorization_alert_settings</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="str">
+        <f t="shared" si="3"/>
+        <v>edit_resource_usage_restrictions</v>
+      </c>
+      <c r="B34" t="s">
+        <v>709</v>
+      </c>
+      <c r="C34" t="s">
+        <v>739</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>edit_resource_usage_restrictions</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="1"/>
+        <v>right.edit_resource_usage_restrictions=编辑资源使用限制</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="2"/>
+        <v>right.edit_resource_usage_restrictions=edit_resource_usage_restrictions</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="str">
+        <f t="shared" si="3"/>
+        <v>platform_authorization_information</v>
+      </c>
+      <c r="B35" t="s">
+        <v>710</v>
+      </c>
+      <c r="C35" t="s">
+        <v>740</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>platform_authorization_information</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="1"/>
+        <v>right.platform_authorization_information=平台授权信息</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="2"/>
+        <v>right.platform_authorization_information=platform_authorization_information</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="str">
+        <f t="shared" si="3"/>
+        <v>two-factor_authentication_setting</v>
+      </c>
+      <c r="B36" t="s">
+        <v>711</v>
+      </c>
+      <c r="C36" t="s">
+        <v>741</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>two-factor_authentication_setting</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="1"/>
+        <v>right.two-factor_authentication_setting=双因素认证设置</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="2"/>
+        <v>right.two-factor_authentication_setting=two-factor_authentication_setting</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="str">
+        <f t="shared" si="3"/>
+        <v>edit_the_main_switch_of_sms_authentication</v>
+      </c>
+      <c r="B37" t="s">
+        <v>712</v>
+      </c>
+      <c r="C37" t="s">
+        <v>742</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>edit_the_main_switch_of_sms_authentication</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="1"/>
+        <v>right.edit_the_main_switch_of_sms_authentication=编辑短信认证总开关</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="2"/>
+        <v>right.edit_the_main_switch_of_sms_authentication=edit_the_main_switch_of_sms_authentication</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="str">
+        <f t="shared" si="3"/>
+        <v>configure_two-factor_authentication_in_batches</v>
+      </c>
+      <c r="B38" t="s">
+        <v>713</v>
+      </c>
+      <c r="C38" t="s">
+        <v>743</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>configure_two-factor_authentication_in_batches</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="1"/>
+        <v>right.configure_two-factor_authentication_in_batches=批量设置双因素认证</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="2"/>
+        <v>right.configure_two-factor_authentication_in_batches=configure_two-factor_authentication_in_batches</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="str">
+        <f t="shared" si="3"/>
+        <v>configure_two-factor_authentication</v>
+      </c>
+      <c r="B39" t="s">
+        <v>714</v>
+      </c>
+      <c r="C39" t="s">
+        <v>744</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>configure_two-factor_authentication</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="1"/>
+        <v>right.configure_two-factor_authentication=设置双因素认证</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="2"/>
+        <v>right.configure_two-factor_authentication=configure_two-factor_authentication</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F9AB08-A3B8-514B-AD13-E0375A045A1B}">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7467,24 +8755,24 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>795</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>796</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>797</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>798</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -7494,167 +8782,167 @@
       </c>
     </row>
     <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3" t="s">
+        <v>262</v>
+      </c>
       <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>110</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>263</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>264</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="B4" t="s">
+    <row r="5" spans="1:7">
+      <c r="B5" t="s">
         <v>265</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="C5" t="s">
+    <row r="6" spans="1:7">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>110</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>263</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>264</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="B6" t="s">
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
         <v>266</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="C7" t="s">
+    <row r="8" spans="1:7">
+      <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>76</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>267</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>268</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="B8" t="s">
+    <row r="9" spans="1:7">
+      <c r="B9" t="s">
         <v>269</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="C9" t="s">
+    <row r="10" spans="1:7">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
         <v>270</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>270</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>2</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="C11" t="s">
+    <row r="12" spans="1:7">
+      <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
         <v>271</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>271</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>2</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="C13" t="s">
+    <row r="14" spans="1:7">
+      <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>59</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>272</v>
-      </c>
-      <c r="B14" t="s">
-        <v>272</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>272</v>
       </c>
       <c r="B15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
@@ -7664,93 +8952,96 @@
       </c>
     </row>
     <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" t="s">
+        <v>273</v>
+      </c>
       <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>110</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>264</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>263</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
-      <c r="B17" t="s">
+    <row r="18" spans="2:7">
+      <c r="B18" t="s">
         <v>274</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
-      <c r="C18" t="s">
+    <row r="19" spans="2:7">
+      <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
-      <c r="B19" t="s">
+    <row r="20" spans="2:7">
+      <c r="B20" t="s">
         <v>105</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>2</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
-      <c r="C20" t="s">
+    <row r="21" spans="2:7">
+      <c r="C21" t="s">
         <v>8</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
-      <c r="B21" t="s">
+    <row r="22" spans="2:7">
+      <c r="B22" t="s">
         <v>277</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>2</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
-      <c r="C22" t="s">
+    <row r="23" spans="2:7">
+      <c r="C23" t="s">
         <v>8</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
-      <c r="B23" t="s">
+    <row r="24" spans="2:7">
+      <c r="B24" t="s">
         <v>99</v>
-      </c>
-      <c r="C23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" t="s">
-        <v>278</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -7759,9 +9050,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:7">
       <c r="B25" t="s">
-        <v>117</v>
+        <v>278</v>
       </c>
       <c r="C25" t="s">
         <v>2</v>
@@ -7770,124 +9061,135 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:7">
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
       <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="C27" t="s">
         <v>8</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>280</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="27" spans="2:5">
-      <c r="B27" t="s">
+    <row r="28" spans="2:7">
+      <c r="B28" t="s">
         <v>279</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>2</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:5">
-      <c r="C28" t="s">
+    <row r="29" spans="2:7">
+      <c r="C29" t="s">
         <v>8</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>280</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="29" spans="2:5">
-      <c r="B29" t="s">
+    <row r="30" spans="2:7">
+      <c r="B30" t="s">
         <v>282</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>2</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:5">
-      <c r="C30" t="s">
+    <row r="31" spans="2:7">
+      <c r="C31" t="s">
         <v>8</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>280</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="31" spans="2:5">
-      <c r="B31" t="s">
+    <row r="32" spans="2:7">
+      <c r="B32" t="s">
         <v>283</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>2</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:5">
-      <c r="C32" t="s">
+    <row r="33" spans="2:5">
+      <c r="C33" t="s">
         <v>8</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>114</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
-      <c r="B33" t="s">
+    <row r="34" spans="2:5">
+      <c r="B34" t="s">
         <v>284</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>2</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:5">
-      <c r="C34" t="s">
+    <row r="35" spans="2:5">
+      <c r="C35" t="s">
         <v>8</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>114</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="2:5">
-      <c r="B35" t="s">
+    <row r="36" spans="2:5">
+      <c r="B36" t="s">
         <v>285</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>2</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:5">
-      <c r="C36" t="s">
+    <row r="37" spans="2:5">
+      <c r="C37" t="s">
         <v>8</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>114</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>115</v>
       </c>
     </row>
@@ -7898,7 +9200,976 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A29DBD9-E94A-0143-B657-2C07F4BA4A49}">
+  <dimension ref="A1:F40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" customWidth="1"/>
+    <col min="6" max="6" width="96" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" t="s">
+        <v>602</v>
+      </c>
+      <c r="D1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="str">
+        <f>D2</f>
+        <v>monitoring_management</v>
+      </c>
+      <c r="B2" t="s">
+        <v>745</v>
+      </c>
+      <c r="C2" t="s">
+        <v>774</v>
+      </c>
+      <c r="D2" t="str">
+        <f>LOWER(C2)</f>
+        <v>monitoring_management</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"right."&amp;D2&amp;"="&amp;B2</f>
+        <v>right.monitoring_management=监控管理</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"right."&amp;D2&amp;"="&amp;D2</f>
+        <v>right.monitoring_management=monitoring_management</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="str">
+        <f>D3</f>
+        <v>the_server</v>
+      </c>
+      <c r="B3" t="s">
+        <v>746</v>
+      </c>
+      <c r="C3" t="s">
+        <v>775</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D40" si="0">LOWER(C3)</f>
+        <v>the_server</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E40" si="1">"right."&amp;D3&amp;"="&amp;B3</f>
+        <v>right.the_server=服务器</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F40" si="2">"right."&amp;D3&amp;"="&amp;D3</f>
+        <v>right.the_server=the_server</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A40" si="3">D4</f>
+        <v>to_view</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>717</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>to_view</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>right.to_view=查看</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="2"/>
+        <v>right.to_view=to_view</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="str">
+        <f t="shared" si="3"/>
+        <v>the_editor</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>722</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>the_editor</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>right.the_editor=编辑</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_editor=the_editor</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="str">
+        <f t="shared" si="3"/>
+        <v>increase</v>
+      </c>
+      <c r="B6" t="s">
+        <v>397</v>
+      </c>
+      <c r="C6" t="s">
+        <v>539</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>increase</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>right.increase=增加</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="2"/>
+        <v>right.increase=increase</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="str">
+        <f t="shared" si="3"/>
+        <v>copy</v>
+      </c>
+      <c r="B7" t="s">
+        <v>522</v>
+      </c>
+      <c r="C7" t="s">
+        <v>540</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>copy</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>right.copy=复制</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="2"/>
+        <v>right.copy=copy</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="str">
+        <f t="shared" si="3"/>
+        <v>modify_the</v>
+      </c>
+      <c r="B8" t="s">
+        <v>523</v>
+      </c>
+      <c r="C8" t="s">
+        <v>776</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>modify_the</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>right.modify_the=修改</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="2"/>
+        <v>right.modify_the=modify_the</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="str">
+        <f t="shared" si="3"/>
+        <v>delete</v>
+      </c>
+      <c r="B9" t="s">
+        <v>350</v>
+      </c>
+      <c r="C9" t="s">
+        <v>536</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>delete</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>right.delete=删除</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="2"/>
+        <v>right.delete=delete</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="str">
+        <f t="shared" si="3"/>
+        <v>service</v>
+      </c>
+      <c r="B10" t="s">
+        <v>747</v>
+      </c>
+      <c r="C10" t="s">
+        <v>768</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>service</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>right.service=服务</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="2"/>
+        <v>right.service=service</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="str">
+        <f t="shared" si="3"/>
+        <v>the_alarm_event</v>
+      </c>
+      <c r="B11" t="s">
+        <v>748</v>
+      </c>
+      <c r="C11" t="s">
+        <v>777</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>the_alarm_event</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>right.the_alarm_event=告警事件</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_alarm_event=the_alarm_event</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="str">
+        <f t="shared" si="3"/>
+        <v>export</v>
+      </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>541</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>export</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>right.export=导出</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="2"/>
+        <v>right.export=export</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="str">
+        <f t="shared" si="3"/>
+        <v>send</v>
+      </c>
+      <c r="B13" t="s">
+        <v>749</v>
+      </c>
+      <c r="C13" t="s">
+        <v>769</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>send</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>right.send=发送</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="2"/>
+        <v>right.send=send</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="str">
+        <f t="shared" si="3"/>
+        <v>restore</v>
+      </c>
+      <c r="B14" t="s">
+        <v>750</v>
+      </c>
+      <c r="C14" t="s">
+        <v>770</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>restore</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>right.restore=恢复</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="2"/>
+        <v>right.restore=restore</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="str">
+        <f t="shared" si="3"/>
+        <v>event_statistics</v>
+      </c>
+      <c r="B15" t="s">
+        <v>751</v>
+      </c>
+      <c r="C15" t="s">
+        <v>778</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>event_statistics</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>right.event_statistics=事件统计</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="2"/>
+        <v>right.event_statistics=event_statistics</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="str">
+        <f t="shared" si="3"/>
+        <v>tenant_log_management</v>
+      </c>
+      <c r="B16" t="s">
+        <v>752</v>
+      </c>
+      <c r="C16" t="s">
+        <v>779</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>tenant_log_management</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>right.tenant_log_management=租户日志管理</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="2"/>
+        <v>right.tenant_log_management=tenant_log_management</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="str">
+        <f t="shared" si="3"/>
+        <v>application_icon_management</v>
+      </c>
+      <c r="B17" t="s">
+        <v>753</v>
+      </c>
+      <c r="C17" t="s">
+        <v>780</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>application_icon_management</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>right.application_icon_management=应用图标管理</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="2"/>
+        <v>right.application_icon_management=application_icon_management</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="str">
+        <f t="shared" si="3"/>
+        <v>add</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>651</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>add</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>right.add=添加</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="2"/>
+        <v>right.add=add</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="str">
+        <f t="shared" si="3"/>
+        <v>find_equipment</v>
+      </c>
+      <c r="B19" t="s">
+        <v>754</v>
+      </c>
+      <c r="C19" t="s">
+        <v>781</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>find_equipment</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>right.find_equipment=查找设备</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="2"/>
+        <v>right.find_equipment=find_equipment</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="str">
+        <f t="shared" si="3"/>
+        <v>system_management</v>
+      </c>
+      <c r="B20" t="s">
+        <v>310</v>
+      </c>
+      <c r="C20" t="s">
+        <v>575</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>system_management</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>right.system_management=系统管理</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="2"/>
+        <v>right.system_management=system_management</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="str">
+        <f t="shared" si="3"/>
+        <v>monitor_setting</v>
+      </c>
+      <c r="B21" t="s">
+        <v>755</v>
+      </c>
+      <c r="C21" t="s">
+        <v>782</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>monitor_setting</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>right.monitor_setting=监控设置</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="2"/>
+        <v>right.monitor_setting=monitor_setting</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="str">
+        <f t="shared" si="3"/>
+        <v>sms_notification_management</v>
+      </c>
+      <c r="B22" t="s">
+        <v>756</v>
+      </c>
+      <c r="C22" t="s">
+        <v>783</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>sms_notification_management</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>right.sms_notification_management=短信通知管理</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="2"/>
+        <v>right.sms_notification_management=sms_notification_management</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="str">
+        <f t="shared" si="3"/>
+        <v>save_sms_notification_settings</v>
+      </c>
+      <c r="B23" t="s">
+        <v>757</v>
+      </c>
+      <c r="C23" t="s">
+        <v>784</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>save_sms_notification_settings</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>right.save_sms_notification_settings=保存短信通知设置</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="2"/>
+        <v>right.save_sms_notification_settings=save_sms_notification_settings</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="str">
+        <f t="shared" si="3"/>
+        <v>system_settings</v>
+      </c>
+      <c r="B24" t="s">
+        <v>392</v>
+      </c>
+      <c r="C24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>system_settings</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>right.system_settings=系统设置</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="2"/>
+        <v>right.system_settings=system_settings</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="str">
+        <f t="shared" si="3"/>
+        <v>download_limit_settings</v>
+      </c>
+      <c r="B25" t="s">
+        <v>758</v>
+      </c>
+      <c r="C25" t="s">
+        <v>785</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>download_limit_settings</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>right.download_limit_settings=下载限制设置</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="2"/>
+        <v>right.download_limit_settings=download_limit_settings</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="str">
+        <f t="shared" si="3"/>
+        <v>downloading_device_logs</v>
+      </c>
+      <c r="B26" t="s">
+        <v>759</v>
+      </c>
+      <c r="C26" t="s">
+        <v>786</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>downloading_device_logs</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>right.downloading_device_logs=设备日志下载</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="2"/>
+        <v>right.downloading_device_logs=downloading_device_logs</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="str">
+        <f t="shared" si="3"/>
+        <v>download</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>650</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>download</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>right.download=下载</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="2"/>
+        <v>right.download=download</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="str">
+        <f t="shared" si="3"/>
+        <v>administrator_operation_logs</v>
+      </c>
+      <c r="B28" t="s">
+        <v>387</v>
+      </c>
+      <c r="C28" t="s">
+        <v>574</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>administrator_operation_logs</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>right.administrator_operation_logs=管理员操作日志</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="2"/>
+        <v>right.administrator_operation_logs=administrator_operation_logs</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="str">
+        <f t="shared" si="3"/>
+        <v>gateway_call_log</v>
+      </c>
+      <c r="B29" t="s">
+        <v>760</v>
+      </c>
+      <c r="C29" t="s">
+        <v>787</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>gateway_call_log</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>right.gateway_call_log=网关调用日志</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="2"/>
+        <v>right.gateway_call_log=gateway_call_log</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="str">
+        <f t="shared" si="3"/>
+        <v>cope_client_upgrade</v>
+      </c>
+      <c r="B30" t="s">
+        <v>405</v>
+      </c>
+      <c r="C30" t="s">
+        <v>788</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>cope_client_upgrade</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>right.cope_client_upgrade=COPE客户端升级</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="2"/>
+        <v>right.cope_client_upgrade=cope_client_upgrade</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="str">
+        <f t="shared" si="3"/>
+        <v>uploading_a_client</v>
+      </c>
+      <c r="B31" t="s">
+        <v>761</v>
+      </c>
+      <c r="C31" t="s">
+        <v>789</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>uploading_a_client</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>right.uploading_a_client=上传客户端</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="2"/>
+        <v>right.uploading_a_client=uploading_a_client</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="str">
+        <f t="shared" si="3"/>
+        <v>push</v>
+      </c>
+      <c r="B32" t="s">
+        <v>762</v>
+      </c>
+      <c r="C32" t="s">
+        <v>771</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>push</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>right.push=推送</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="2"/>
+        <v>right.push=push</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="str">
+        <f t="shared" si="3"/>
+        <v>upgrade_the_byod_client</v>
+      </c>
+      <c r="B33" t="s">
+        <v>763</v>
+      </c>
+      <c r="C33" t="s">
+        <v>790</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>upgrade_the_byod_client</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>right.upgrade_the_byod_client=BYOD客户端升级</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="2"/>
+        <v>right.upgrade_the_byod_client=upgrade_the_byod_client</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="str">
+        <f t="shared" si="3"/>
+        <v>the_ios_client_is_upgraded</v>
+      </c>
+      <c r="B34" t="s">
+        <v>764</v>
+      </c>
+      <c r="C34" t="s">
+        <v>791</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>the_ios_client_is_upgraded</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="1"/>
+        <v>right.the_ios_client_is_upgraded=IOS客户端升级</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_ios_client_is_upgraded=the_ios_client_is_upgraded</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="str">
+        <f t="shared" si="3"/>
+        <v>tenant_feedback</v>
+      </c>
+      <c r="B35" t="s">
+        <v>765</v>
+      </c>
+      <c r="C35" t="s">
+        <v>792</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>tenant_feedback</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="1"/>
+        <v>right.tenant_feedback=租户意见反馈</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="2"/>
+        <v>right.tenant_feedback=tenant_feedback</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="str">
+        <f t="shared" si="3"/>
+        <v>reply</v>
+      </c>
+      <c r="B36" t="s">
+        <v>402</v>
+      </c>
+      <c r="C36" t="s">
+        <v>772</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>reply</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="1"/>
+        <v>right.reply=回复</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="2"/>
+        <v>right.reply=reply</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="str">
+        <f t="shared" si="3"/>
+        <v>ignore</v>
+      </c>
+      <c r="B37" t="s">
+        <v>403</v>
+      </c>
+      <c r="C37" t="s">
+        <v>773</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>ignore</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="1"/>
+        <v>right.ignore=忽略</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="2"/>
+        <v>right.ignore=ignore</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="str">
+        <f t="shared" si="3"/>
+        <v>android_feedback</v>
+      </c>
+      <c r="B38" t="s">
+        <v>766</v>
+      </c>
+      <c r="C38" t="s">
+        <v>793</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>android_feedback</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="1"/>
+        <v>right.android_feedback=Android意见反馈</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="2"/>
+        <v>right.android_feedback=android_feedback</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="str">
+        <f t="shared" si="3"/>
+        <v>ios_feedback</v>
+      </c>
+      <c r="B39" t="s">
+        <v>767</v>
+      </c>
+      <c r="C39" t="s">
+        <v>794</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>ios_feedback</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="1"/>
+        <v>right.ios_feedback=IOS意见反馈</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="2"/>
+        <v>right.ios_feedback=ios_feedback</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="str">
+        <f t="shared" si="3"/>
+        <v>the_front_panel</v>
+      </c>
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>425</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>the_front_panel</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="1"/>
+        <v>right.the_front_panel=首页面板</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_front_panel=the_front_panel</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89C31BD-9216-6A49-8C90-0ADAF2498DB4}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -11049,8 +13320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DFAFE7B-50A9-ED46-A4A9-43F085DA759E}">
   <dimension ref="A1:I185"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -16314,7 +18585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24903F80-53DC-C64D-9D85-89EE3AEF25C2}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
vault backup: 2022-01-07 11:33:46
Affected files:
.obsidian/plugins/recent-files-obsidian/data.json
.obsidian/plugins/rss-reader/data.json
.obsidian/workspace
14TODO/TODO.md
1附件/权限列表.xlsx
</commit_message>
<xml_diff>
--- a/1附件/权限列表.xlsx
+++ b/1附件/权限列表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0800894-4EA3-BF4E-97BB-30FEAD957A2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A7A570-2D2B-0644-B50A-E2869C3D2C28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="0" windowWidth="37500" windowHeight="21600" activeTab="15" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
+    <workbookView xWindow="900" yWindow="0" windowWidth="37500" windowHeight="21600" firstSheet="1" activeTab="16" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Mdm权限管理 (2)" sheetId="7" state="hidden" r:id="rId1"/>
@@ -29,7 +29,8 @@
     <sheet name="运营数据字典" sheetId="18" r:id="rId14"/>
     <sheet name="运维权限管理" sheetId="5" r:id="rId15"/>
     <sheet name="运维数据字典" sheetId="19" r:id="rId16"/>
-    <sheet name="安全审核权限管理" sheetId="6" r:id="rId17"/>
+    <sheet name="运维运营数据库脚本" sheetId="20" r:id="rId17"/>
+    <sheet name="安全审核权限管理" sheetId="6" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,139 +42,139 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3317" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3587" uniqueCount="803">
   <si>
     <t>首页面板</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>查看</t>
   </si>
   <si>
     <t>查看</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>下载</t>
   </si>
   <si>
     <t>下载</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>用户管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>组织机构</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑</t>
   </si>
   <si>
     <t>编辑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>发送消息</t>
   </si>
   <si>
     <t>发送消息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>分发文档</t>
   </si>
   <si>
     <t>分发文档</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>更改策略</t>
   </si>
   <si>
     <t>更改策略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>批量锁定设备</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>批量解锁设备</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>取消文档分发</t>
   </si>
   <si>
     <t>取消文档分发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>用户列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>用户分组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>设备管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>锁定设备</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>解锁设备</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>锁定沙箱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>解锁沙箱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>发警报音</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>擦除数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>恢复数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>丢失</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>完全擦除</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>注销设备</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>刷新设备信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>定位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>配置WLAN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>配置VPN</t>
@@ -192,105 +193,105 @@
   </si>
   <si>
     <t>提取日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>外出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>归队</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>重启设备</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>强制关机</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>验证证书</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>远程控制</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>解绑SIM卡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>获取实时运行数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>导出流量信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>删除应用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>注册审核</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>批量通过</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>批量拒绝</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>通过</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>拒绝</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>注册白名单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>批量导入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加</t>
   </si>
   <si>
     <t>添加</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>删除</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安全策略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>分发</t>
   </si>
   <si>
     <t>分发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>停用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>蓝牙白名单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加组</t>
@@ -303,893 +304,893 @@
   </si>
   <si>
     <t>批量导入蓝牙白名单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>批量删除蓝牙白名单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加蓝牙白名单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>删除蓝牙白名单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑蓝牙白名单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安全审计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>导出</t>
   </si>
   <si>
     <t>导出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>导出通话记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>导出通话录音</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>播放通话录音</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>下载通话录音</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>播放</t>
   </si>
   <si>
     <t>播放</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>导出会话</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>导出聊天记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>资源管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>应用分发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>文档管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>取消分发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>敏感词库</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>统计报表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>用户统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>流量统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>设备统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安全统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>应用统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>网络统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>敏感词统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>日志管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>管理员操作日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>用户登录日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>设备日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>门禁出入记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>电子围栏出入记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>系统管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>系统设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>保存注册设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>保存功能设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>保存SDK设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>移动门户设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>增加</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>预览</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>保存并推送</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>消息管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>回复</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>忽略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>报表下载</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>COPE客户端升级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>关于系统</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>下载二维码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>更改苹果规则</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓设备管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>苹果设备管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>批量删除</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓注册记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>苹果注册记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓设备策略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>苹果设备策略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>苹果规则</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓应用安装</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>苹果应用安装</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓应用使用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓上网行为</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓通话记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓短信记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓彩信记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓微信聊天</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓QQ聊天</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓敏感词</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓违规状态记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓意见反馈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>苹果意见反馈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>苹果客户端升级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>机构</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>导入组织机构</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>批量授权</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>应用授权</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加机构</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>删除机构</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>移动勾选用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>批量取消授权</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>取消授权</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑机构</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加单个用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>批量导入用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>标记</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>批量删除用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>授权</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>修改密码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>变更机构</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>离职</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>删除用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑标签</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>静态组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加静态组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑成员</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>移除分组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑分组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>动态组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加动态组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>移动应用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>授权记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>授权访问</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>单点登录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>数据字典</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>保存APP端认证设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加职级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑职级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加标签</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加职位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑职位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LDAP设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>同步</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>控制台</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>应用管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>创建应用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>下架应用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>升级应用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑安全策略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑发布策略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>删除应用评价</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>上架应用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑应用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>应用集市</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>上架</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>升级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>部署统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>活跃用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>运行统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓沙箱策略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加策略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>删除策略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑策略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>推荐管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加推荐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>修改推荐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>系统日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>类别管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加类别</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑类别</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>冻结类别</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>激活类别</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>标签管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>冻结</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>激活</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑默认签名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安全审核</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>消息推送审核</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>审核</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>试卷审核</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>问卷审核</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>应用审核</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>轮播图片审核</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>文档推送审核</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>审核日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>撤回</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>提醒</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>申请</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>平台概况</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>平台资源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>平台运营</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>租户管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>普通租户管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>创建租户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>停用租户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑租户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>注销租户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>CB租户管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>开通</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>退订</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>导出用户列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>同步日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>导出租户失败记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>导出用户失败记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>服务管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>服务列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>添加服务</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>删除服务</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑服务</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>应用/SDK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑授权提醒设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑资源使用限制</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>平台授权信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>开通退订管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>待开通用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>待退订用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>已退订用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>已开通用户</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>监控管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>服务器</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>复制</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>修改</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>服务</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>告警事件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>发送</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>恢复</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>事件统计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>租户日志管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>应用图标管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>查找设备</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>监控设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>短信通知管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>保存短信通知设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>下载限制设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>设备日志下载</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>网关调用日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>BYOD客户端升级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>上传客户端</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>推送</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>IOS客户端升级</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>租户意见反馈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Android意见反馈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>IOS意见反馈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>双因素认证设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑短信认证总开关</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>设置双因素认证</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>批量设置双因素认证</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>角色管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>管理员</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>用户管理</t>
@@ -1214,11 +1215,11 @@
   </si>
   <si>
     <t>统一认证</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安全管控</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>审核系统</t>
@@ -1252,26 +1253,26 @@
   </si>
   <si>
     <t>全部类别</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>子类别</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>读取</t>
   </si>
   <si>
     <t>读取</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>子菜单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>安卓设备管理</t>
@@ -1548,19 +1549,19 @@
   </si>
   <si>
     <t>category</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>menu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1593,7 +1594,7 @@
   </si>
   <si>
     <t>);</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1631,7 +1632,7 @@
       </rPr>
       <t>,</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -2184,67 +2185,67 @@
   </si>
   <si>
     <t>Single_sign_on</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Import_organization</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>organization</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>read</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Modify</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>data_dictionary</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Save_the_password_policy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>mobile_application</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>user</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>write</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>保存密码策略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>WEB应用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>编辑WEB应用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>WEB登录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>保存WEB端认证设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -2282,7 +2283,7 @@
       </rPr>
       <t>,</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -2575,7 +2576,7 @@
       </rPr>
       <t>,</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -2925,12 +2926,117 @@
   <si>
     <t>code</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>'0'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>'funcId'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>'0', 'funcId',</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>'0', 'funcId',</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>'0', 'funcId',</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3018,7 +3124,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4433,7 +4539,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -4777,7 +4883,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -5938,7 +6044,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -7477,7 +7583,7 @@
       <c r="D181" s="4"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -7787,7 +7893,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -8732,7 +8838,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -9194,7 +9300,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -9204,7 +9310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A29DBD9-E94A-0143-B657-2C07F4BA4A49}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -10163,13 +10269,2111 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DDFF0F-151D-2C4F-8ADA-466E373776C8}">
+  <dimension ref="A1:E181"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4">
+        <v>409</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C1" t="str">
+        <f>B1&amp;""&amp;A1&amp;D1&amp;A1&amp;E1</f>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (409, '0', 'funcId',409);</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>799</v>
+      </c>
+      <c r="E1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4">
+        <v>410</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C65" si="0">B2&amp;""&amp;A2&amp;D2&amp;A2&amp;E2</f>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (410, '0', 'funcId',410);</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>800</v>
+      </c>
+      <c r="E2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4">
+        <v>411</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (411, '0', 'funcId',411);</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4">
+        <v>412</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (412, '0', 'funcId',412);</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E4" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4">
+        <v>413</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (413, '0', 'funcId',413);</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4">
+        <v>414</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (414, '0', 'funcId',414);</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4">
+        <v>415</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (415, '0', 'funcId',415);</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E7" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4">
+        <v>416</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (416, '0', 'funcId',416);</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E8" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4">
+        <v>417</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (417, '0', 'funcId',417);</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E9" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4">
+        <v>418</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (418, '0', 'funcId',418);</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E10" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4">
+        <v>419</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (419, '0', 'funcId',419);</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E11" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4">
+        <v>420</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (420, '0', 'funcId',420);</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E12" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4">
+        <v>421</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (421, '0', 'funcId',421);</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E13" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4">
+        <v>422</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (422, '0', 'funcId',422);</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E14" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4">
+        <v>423</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (423, '0', 'funcId',423);</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E15" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4">
+        <v>424</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (424, '0', 'funcId',424);</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E16" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4">
+        <v>425</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (425, '0', 'funcId',425);</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E17" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4">
+        <v>426</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (426, '0', 'funcId',426);</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E18" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4">
+        <v>427</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (427, '0', 'funcId',427);</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E19" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4">
+        <v>428</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (428, '0', 'funcId',428);</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E20" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4">
+        <v>429</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (429, '0', 'funcId',429);</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E21" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4">
+        <v>430</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (430, '0', 'funcId',430);</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E22" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4">
+        <v>431</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (431, '0', 'funcId',431);</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E23" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4">
+        <v>432</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (432, '0', 'funcId',432);</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E24" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4">
+        <v>433</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (433, '0', 'funcId',433);</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E25" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="4">
+        <v>434</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (434, '0', 'funcId',434);</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E26" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4">
+        <v>435</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (435, '0', 'funcId',435);</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E27" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4">
+        <v>436</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (436, '0', 'funcId',436);</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E28" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="4">
+        <v>437</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (437, '0', 'funcId',437);</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E29" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="4">
+        <v>438</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (438, '0', 'funcId',438);</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E30" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4">
+        <v>439</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (439, '0', 'funcId',439);</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E31" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4">
+        <v>440</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (440, '0', 'funcId',440);</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E32" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4">
+        <v>441</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (441, '0', 'funcId',441);</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E33" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4">
+        <v>442</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (442, '0', 'funcId',442);</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E34" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="4">
+        <v>443</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (443, '0', 'funcId',443);</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E35" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4">
+        <v>444</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (444, '0', 'funcId',444);</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E36" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4">
+        <v>445</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (445, '0', 'funcId',445);</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E37" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4">
+        <v>446</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (446, '0', 'funcId',446);</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E38" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="4">
+        <v>447</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (447, '0', 'funcId',447);</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E39" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="4">
+        <v>448</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (448, '0', 'funcId',448);</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E40" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="4">
+        <v>449</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (449, '0', 'funcId',449);</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E41" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="4">
+        <v>450</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (450, '0', 'funcId',450);</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E42" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="4">
+        <v>451</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (451, '0', 'funcId',451);</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E43" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="4">
+        <v>452</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (452, '0', 'funcId',452);</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E44" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="4">
+        <v>453</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (453, '0', 'funcId',453);</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E45" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="4">
+        <v>454</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (454, '0', 'funcId',454);</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E46" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="4">
+        <v>455</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (455, '0', 'funcId',455);</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E47" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="4">
+        <v>456</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (456, '0', 'funcId',456);</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E48" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="4">
+        <v>457</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (457, '0', 'funcId',457);</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E49" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="4">
+        <v>458</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (458, '0', 'funcId',458);</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E50" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="4">
+        <v>459</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (459, '0', 'funcId',459);</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E51" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="4">
+        <v>460</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (460, '0', 'funcId',460);</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E52" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="4">
+        <v>461</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (461, '0', 'funcId',461);</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E53" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="4">
+        <v>462</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (462, '0', 'funcId',462);</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E54" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="4">
+        <v>463</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (463, '0', 'funcId',463);</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E55" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="4">
+        <v>464</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (464, '0', 'funcId',464);</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E56" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="4">
+        <v>465</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (465, '0', 'funcId',465);</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E57" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="4">
+        <v>466</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (466, '0', 'funcId',466);</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E58" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="4">
+        <v>467</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (467, '0', 'funcId',467);</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E59" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="4">
+        <v>468</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (468, '0', 'funcId',468);</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E60" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="4">
+        <v>469</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (469, '0', 'funcId',469);</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E61" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="4">
+        <v>470</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (470, '0', 'funcId',470);</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E62" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="4">
+        <v>471</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (471, '0', 'funcId',471);</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E63" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="4">
+        <v>472</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (472, '0', 'funcId',472);</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E64" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="4">
+        <v>473</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (473, '0', 'funcId',473);</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E65" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="4">
+        <v>474</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" ref="C66:C90" si="1">B66&amp;""&amp;A66&amp;D66&amp;A66&amp;E66</f>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (474, '0', 'funcId',474);</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E66" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="4">
+        <v>475</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (475, '0', 'funcId',475);</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E67" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="4">
+        <v>476</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (476, '0', 'funcId',476);</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E68" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="4">
+        <v>477</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (477, '0', 'funcId',477);</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E69" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="4">
+        <v>478</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (478, '0', 'funcId',478);</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E70" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="4">
+        <v>479</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (479, '0', 'funcId',479);</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E71" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="4">
+        <v>480</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (480, '0', 'funcId',480);</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E72" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="4">
+        <v>481</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (481, '0', 'funcId',481);</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E73" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="4">
+        <v>482</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (482, '0', 'funcId',482);</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E74" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="4">
+        <v>483</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (483, '0', 'funcId',483);</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E75" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="4">
+        <v>484</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (484, '0', 'funcId',484);</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E76" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="4">
+        <v>485</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (485, '0', 'funcId',485);</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E77" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="4">
+        <v>486</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (486, '0', 'funcId',486);</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E78" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="4">
+        <v>487</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (487, '0', 'funcId',487);</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E79" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="4">
+        <v>488</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (488, '0', 'funcId',488);</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E80" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="4">
+        <v>489</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (489, '0', 'funcId',489);</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E81" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="4">
+        <v>490</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (490, '0', 'funcId',490);</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E82" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="4">
+        <v>491</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (491, '0', 'funcId',491);</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E83" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="4">
+        <v>492</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (492, '0', 'funcId',492);</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E84" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="4">
+        <v>493</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (493, '0', 'funcId',493);</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E85" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="4">
+        <v>494</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (494, '0', 'funcId',494);</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E86" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="4">
+        <v>495</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (495, '0', 'funcId',495);</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E87" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="4">
+        <v>496</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (496, '0', 'funcId',496);</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E88" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="4">
+        <v>497</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (497, '0', 'funcId',497);</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>801</v>
+      </c>
+      <c r="E89" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="4">
+        <v>498</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (498, '0', 'funcId',498);</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>802</v>
+      </c>
+      <c r="E90" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="D91" s="4"/>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="D92" s="4"/>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="D93" s="4"/>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="D94" s="4"/>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="D95" s="4"/>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="D96" s="4"/>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="D97" s="4"/>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="D98" s="4"/>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="D99" s="4"/>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="D100" s="4"/>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="D101" s="4"/>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="D102" s="4"/>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="D103" s="4"/>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="4"/>
+      <c r="B104" s="4"/>
+      <c r="D104" s="4"/>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="4"/>
+      <c r="B105" s="4"/>
+      <c r="D105" s="4"/>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4"/>
+      <c r="D106" s="4"/>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="D107" s="4"/>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="D108" s="4"/>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="D109" s="4"/>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="4"/>
+      <c r="B110" s="4"/>
+      <c r="D110" s="4"/>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="4"/>
+      <c r="B111" s="4"/>
+      <c r="D111" s="4"/>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="D112" s="4"/>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="4"/>
+      <c r="B113" s="4"/>
+      <c r="D113" s="4"/>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="4"/>
+      <c r="B114" s="4"/>
+      <c r="D114" s="4"/>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="4"/>
+      <c r="B115" s="4"/>
+      <c r="D115" s="4"/>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="4"/>
+      <c r="B116" s="4"/>
+      <c r="D116" s="4"/>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="4"/>
+      <c r="B117" s="4"/>
+      <c r="D117" s="4"/>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="4"/>
+      <c r="B118" s="4"/>
+      <c r="D118" s="4"/>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+      <c r="D119" s="4"/>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="D120" s="4"/>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4"/>
+      <c r="D121" s="4"/>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="4"/>
+      <c r="B122" s="4"/>
+      <c r="D122" s="4"/>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="4"/>
+      <c r="B123" s="4"/>
+      <c r="D123" s="4"/>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="4"/>
+      <c r="B124" s="4"/>
+      <c r="D124" s="4"/>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="4"/>
+      <c r="B125" s="4"/>
+      <c r="D125" s="4"/>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="4"/>
+      <c r="B126" s="4"/>
+      <c r="D126" s="4"/>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="4"/>
+      <c r="B127" s="4"/>
+      <c r="D127" s="4"/>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="4"/>
+      <c r="B128" s="4"/>
+      <c r="D128" s="4"/>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="4"/>
+      <c r="B129" s="4"/>
+      <c r="D129" s="4"/>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="4"/>
+      <c r="B130" s="4"/>
+      <c r="D130" s="4"/>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="4"/>
+      <c r="B131" s="4"/>
+      <c r="D131" s="4"/>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="4"/>
+      <c r="B132" s="4"/>
+      <c r="D132" s="4"/>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="4"/>
+      <c r="B133" s="4"/>
+      <c r="D133" s="4"/>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="4"/>
+      <c r="B134" s="4"/>
+      <c r="D134" s="4"/>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="4"/>
+      <c r="B135" s="4"/>
+      <c r="D135" s="4"/>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="4"/>
+      <c r="B136" s="4"/>
+      <c r="D136" s="4"/>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="4"/>
+      <c r="B137" s="4"/>
+      <c r="D137" s="4"/>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="4"/>
+      <c r="B138" s="4"/>
+      <c r="D138" s="4"/>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="4"/>
+      <c r="B139" s="4"/>
+      <c r="D139" s="4"/>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="4"/>
+      <c r="B140" s="4"/>
+      <c r="D140" s="4"/>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="4"/>
+      <c r="B141" s="4"/>
+      <c r="D141" s="4"/>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="4"/>
+      <c r="B142" s="4"/>
+      <c r="D142" s="4"/>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="4"/>
+      <c r="B143" s="4"/>
+      <c r="D143" s="4"/>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="4"/>
+      <c r="B144" s="4"/>
+      <c r="D144" s="4"/>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="4"/>
+      <c r="B145" s="4"/>
+      <c r="D145" s="4"/>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="4"/>
+      <c r="B146" s="4"/>
+      <c r="D146" s="4"/>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="4"/>
+      <c r="B147" s="4"/>
+      <c r="D147" s="4"/>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="4"/>
+      <c r="B148" s="4"/>
+      <c r="D148" s="4"/>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="4"/>
+      <c r="B149" s="4"/>
+      <c r="D149" s="4"/>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" s="4"/>
+      <c r="B150" s="4"/>
+      <c r="D150" s="4"/>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" s="4"/>
+      <c r="B151" s="4"/>
+      <c r="D151" s="4"/>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" s="4"/>
+      <c r="B152" s="4"/>
+      <c r="D152" s="4"/>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" s="4"/>
+      <c r="B153" s="4"/>
+      <c r="D153" s="4"/>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="4"/>
+      <c r="B154" s="4"/>
+      <c r="D154" s="4"/>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="4"/>
+      <c r="B155" s="4"/>
+      <c r="D155" s="4"/>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="4"/>
+      <c r="B156" s="4"/>
+      <c r="D156" s="4"/>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="4"/>
+      <c r="B157" s="4"/>
+      <c r="D157" s="4"/>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="4"/>
+      <c r="B158" s="4"/>
+      <c r="D158" s="4"/>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="4"/>
+      <c r="B159" s="4"/>
+      <c r="D159" s="4"/>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" s="4"/>
+      <c r="B160" s="4"/>
+      <c r="D160" s="4"/>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="4"/>
+      <c r="B161" s="4"/>
+      <c r="D161" s="4"/>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="4"/>
+      <c r="B162" s="4"/>
+      <c r="D162" s="4"/>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="4"/>
+      <c r="B163" s="4"/>
+      <c r="D163" s="4"/>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" s="4"/>
+      <c r="B164" s="4"/>
+      <c r="D164" s="4"/>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="4"/>
+      <c r="B165" s="4"/>
+      <c r="D165" s="4"/>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="4"/>
+      <c r="B166" s="4"/>
+      <c r="D166" s="4"/>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="4"/>
+      <c r="B167" s="4"/>
+      <c r="D167" s="4"/>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" s="4"/>
+      <c r="B168" s="4"/>
+      <c r="D168" s="4"/>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" s="4"/>
+      <c r="B169" s="4"/>
+      <c r="D169" s="4"/>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" s="4"/>
+      <c r="B170" s="4"/>
+      <c r="D170" s="4"/>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" s="4"/>
+      <c r="B171" s="4"/>
+      <c r="D171" s="4"/>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" s="4"/>
+      <c r="B172" s="4"/>
+      <c r="D172" s="4"/>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" s="4"/>
+      <c r="B173" s="4"/>
+      <c r="D173" s="4"/>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" s="4"/>
+      <c r="B174" s="4"/>
+      <c r="D174" s="4"/>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" s="4"/>
+      <c r="B175" s="4"/>
+      <c r="D175" s="4"/>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="4"/>
+      <c r="B176" s="4"/>
+      <c r="D176" s="4"/>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" s="4"/>
+      <c r="B177" s="4"/>
+      <c r="D177" s="4"/>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" s="4"/>
+      <c r="B178" s="4"/>
+      <c r="D178" s="4"/>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" s="4"/>
+      <c r="B179" s="4"/>
+      <c r="D179" s="4"/>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" s="4"/>
+      <c r="B180" s="4"/>
+      <c r="D180" s="4"/>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" s="4"/>
+      <c r="B181" s="4"/>
+      <c r="D181" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89C31BD-9216-6A49-8C90-0ADAF2498DB4}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -10328,7 +12532,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -12082,7 +14286,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -12199,7 +14403,7 @@
     <row r="11" spans="1:10" collapsed="1"/>
   </sheetData>
   <dataConsolidate/>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -13310,7 +15514,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -14686,7 +16890,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A126">
     <sortCondition ref="A1:A126"/>
   </sortState>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -17967,7 +20171,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -18575,7 +20779,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -20288,7 +22492,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -23569,7 +25773,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
vault backup: 2022-01-10 15:33:24
Affected files:
.obsidian/plugins/recent-files-obsidian/data.json
.obsidian/workspace
1附件/权限列表.xlsx
</commit_message>
<xml_diff>
--- a/1附件/权限列表.xlsx
+++ b/1附件/权限列表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C2E72F-384C-7A4D-BC8F-6A2E2B0037FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24283C7-2F81-7F42-9801-661F9D8421F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="0" windowWidth="37460" windowHeight="21600" firstSheet="5" activeTab="16" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
+    <workbookView xWindow="940" yWindow="0" windowWidth="37460" windowHeight="21600" activeTab="10" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Mdm权限管理 (2)" sheetId="7" state="hidden" r:id="rId1"/>
@@ -22,18 +22,20 @@
     <sheet name="Mdm权限管理-补充" sheetId="21" r:id="rId7"/>
     <sheet name="Mdm数据字典-补充" sheetId="23" r:id="rId8"/>
     <sheet name="Mdm数据库脚本-补充" sheetId="24" r:id="rId9"/>
-    <sheet name="Uniauth权限管理" sheetId="2" r:id="rId10"/>
-    <sheet name="Uniauth数据字典" sheetId="13" r:id="rId11"/>
-    <sheet name="Uniauth数据库脚本" sheetId="14" r:id="rId12"/>
-    <sheet name="App权限管理" sheetId="3" r:id="rId13"/>
-    <sheet name="App数据字典" sheetId="15" r:id="rId14"/>
-    <sheet name="App数据库脚本" sheetId="16" r:id="rId15"/>
-    <sheet name="运营权限管理" sheetId="4" r:id="rId16"/>
-    <sheet name="运营数据字典" sheetId="18" r:id="rId17"/>
-    <sheet name="运维权限管理" sheetId="5" r:id="rId18"/>
-    <sheet name="运维数据字典" sheetId="19" r:id="rId19"/>
-    <sheet name="运维运营数据库脚本" sheetId="20" r:id="rId20"/>
-    <sheet name="安全审核权限管理" sheetId="6" r:id="rId21"/>
+    <sheet name="Uniauth权限管理-新" sheetId="25" r:id="rId10"/>
+    <sheet name="Uniauth数据字典-新" sheetId="26" r:id="rId11"/>
+    <sheet name="Uniauth权限管理" sheetId="2" r:id="rId12"/>
+    <sheet name="Uniauth数据字典" sheetId="13" r:id="rId13"/>
+    <sheet name="Uniauth数据库脚本" sheetId="14" r:id="rId14"/>
+    <sheet name="App权限管理" sheetId="3" r:id="rId15"/>
+    <sheet name="App数据字典" sheetId="15" r:id="rId16"/>
+    <sheet name="App数据库脚本" sheetId="16" r:id="rId17"/>
+    <sheet name="运营权限管理" sheetId="4" r:id="rId18"/>
+    <sheet name="运营数据字典" sheetId="18" r:id="rId19"/>
+    <sheet name="运维权限管理" sheetId="5" r:id="rId20"/>
+    <sheet name="运维数据字典" sheetId="19" r:id="rId21"/>
+    <sheet name="运维运营数据库脚本" sheetId="20" r:id="rId22"/>
+    <sheet name="安全审核权限管理" sheetId="6" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3713" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3769" uniqueCount="825">
   <si>
     <t>首页面板</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3088,6 +3090,12 @@
   <si>
     <t>Synchronization_tenant</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WEB应用</t>
+  </si>
+  <si>
+    <t>The_WEB_application</t>
   </si>
 </sst>
 </file>
@@ -4604,11 +4612,463 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A019302D-647A-2045-8CA6-471353C66534}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>524</v>
+      </c>
+      <c r="B2" t="s">
+        <v>524</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>397</v>
+      </c>
+      <c r="E3" t="s">
+        <v>523</v>
+      </c>
+      <c r="F3" t="s">
+        <v>350</v>
+      </c>
+      <c r="G3" t="s">
+        <v>487</v>
+      </c>
+      <c r="H3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4" t="s">
+        <v>521</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>397</v>
+      </c>
+      <c r="E5" t="s">
+        <v>522</v>
+      </c>
+      <c r="F5" t="s">
+        <v>523</v>
+      </c>
+      <c r="G5" t="s">
+        <v>350</v>
+      </c>
+      <c r="H5" t="s">
+        <v>487</v>
+      </c>
+      <c r="I5" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="B6" t="s">
+        <v>510</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7" t="s">
+        <v>823</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA1DC7ED-5AAB-3341-B08D-257D860CF2EB}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="96" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" t="s">
+        <v>602</v>
+      </c>
+      <c r="D1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="str">
+        <f>D2</f>
+        <v>the_administrator</v>
+      </c>
+      <c r="B2" t="s">
+        <v>524</v>
+      </c>
+      <c r="C2" t="s">
+        <v>586</v>
+      </c>
+      <c r="D2" t="str">
+        <f>LOWER(C2)</f>
+        <v>the_administrator</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"right."&amp;D2&amp;"="&amp;B2</f>
+        <v>right.the_administrator=管理员</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"right."&amp;D2&amp;"="&amp;D2</f>
+        <v>right.the_administrator=the_administrator</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A13" si="0">D3</f>
+        <v>to_view</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>717</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D13" si="1">LOWER(C3)</f>
+        <v>to_view</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E13" si="2">"right."&amp;D3&amp;"="&amp;B3</f>
+        <v>right.to_view=查看</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F13" si="3">"right."&amp;D3&amp;"="&amp;D3</f>
+        <v>right.to_view=to_view</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>the_editor</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>722</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>the_editor</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_editor=编辑</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="3"/>
+        <v>right.the_editor=the_editor</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>increase</v>
+      </c>
+      <c r="B5" t="s">
+        <v>397</v>
+      </c>
+      <c r="C5" t="s">
+        <v>539</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>increase</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="2"/>
+        <v>right.increase=增加</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="3"/>
+        <v>right.increase=increase</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>modify_the</v>
+      </c>
+      <c r="B6" t="s">
+        <v>523</v>
+      </c>
+      <c r="C6" t="s">
+        <v>776</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>modify_the</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="2"/>
+        <v>right.modify_the=修改</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="3"/>
+        <v>right.modify_the=modify_the</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>delete</v>
+      </c>
+      <c r="B7" t="s">
+        <v>350</v>
+      </c>
+      <c r="C7" t="s">
+        <v>536</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>delete</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="2"/>
+        <v>right.delete=删除</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="3"/>
+        <v>right.delete=delete</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>canceling_authorization_in_batches</v>
+      </c>
+      <c r="B8" t="s">
+        <v>487</v>
+      </c>
+      <c r="C8" t="s">
+        <v>549</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>canceling_authorization_in_batches</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="2"/>
+        <v>right.canceling_authorization_in_batches=批量取消授权</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="3"/>
+        <v>right.canceling_authorization_in_batches=canceling_authorization_in_batches</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>cancel_the_authorization</v>
+      </c>
+      <c r="B9" t="s">
+        <v>488</v>
+      </c>
+      <c r="C9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>cancel_the_authorization</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="2"/>
+        <v>right.cancel_the_authorization=取消授权</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="3"/>
+        <v>right.cancel_the_authorization=cancel_the_authorization</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>role_management</v>
+      </c>
+      <c r="B10" t="s">
+        <v>521</v>
+      </c>
+      <c r="C10" t="s">
+        <v>585</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>role_management</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="2"/>
+        <v>right.role_management=角色管理</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="3"/>
+        <v>right.role_management=role_management</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>copy</v>
+      </c>
+      <c r="B11" t="s">
+        <v>522</v>
+      </c>
+      <c r="C11" t="s">
+        <v>540</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>copy</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="2"/>
+        <v>right.copy=复制</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="3"/>
+        <v>right.copy=copy</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>authorization_records</v>
+      </c>
+      <c r="B12" t="s">
+        <v>510</v>
+      </c>
+      <c r="C12" t="s">
+        <v>570</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>authorization_records</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v>right.authorization_records=授权记录</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="3"/>
+        <v>right.authorization_records=authorization_records</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>the_web_application</v>
+      </c>
+      <c r="B13" t="s">
+        <v>823</v>
+      </c>
+      <c r="C13" t="s">
+        <v>824</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>the_web_application</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_web_application=WEB应用</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="3"/>
+        <v>right.the_web_application=the_web_application</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85160F0E-AAA4-2440-88EE-EDE07CD3F226}">
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A15" sqref="A15:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4870,34 +5330,34 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
-      <c r="B15" t="s">
+    <row r="15" spans="1:14" s="1" customFormat="1">
+      <c r="B15" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
-      <c r="C16" t="s">
+    <row r="16" spans="1:14" s="1" customFormat="1">
+      <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="1" t="s">
         <v>605</v>
       </c>
     </row>
@@ -5211,7 +5671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24903F80-53DC-C64D-9D85-89EE3AEF25C2}">
   <dimension ref="A1:F71"/>
   <sheetViews>
@@ -6924,7 +7384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8ED7B14-461E-2E4B-A00D-9153CAC1D1DD}">
   <dimension ref="A1:E181"/>
   <sheetViews>
@@ -10205,7 +10665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC44C7D-B5C9-8244-8110-B919A147507E}">
   <dimension ref="A1:I23"/>
   <sheetViews>
@@ -10549,7 +11009,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25078354-96F9-7844-A29A-36E43FC30F16}">
   <dimension ref="A1:F48"/>
   <sheetViews>
@@ -11710,7 +12170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729CB04B-3595-F94F-8768-A7FA5DE90163}">
   <dimension ref="A1:E181"/>
   <sheetViews>
@@ -13249,7 +13709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B3B789-6212-894F-BA86-A23B372BEE33}">
   <dimension ref="A1:H23"/>
   <sheetViews>
@@ -13562,12 +14022,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884E44BC-9319-B840-B499-063BCB3FAB83}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14522,1437 +14982,6 @@
       <c r="F40" t="str">
         <f t="shared" si="2"/>
         <v>right.synchronization_tenant=synchronization_tenant</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F9AB08-A3B8-514B-AD13-E0375A045A1B}">
-  <dimension ref="A1:G37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>795</v>
-      </c>
-      <c r="B1" t="s">
-        <v>796</v>
-      </c>
-      <c r="C1" t="s">
-        <v>797</v>
-      </c>
-      <c r="D1" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>261</v>
-      </c>
-      <c r="B3" t="s">
-        <v>262</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" t="s">
-        <v>263</v>
-      </c>
-      <c r="F4" t="s">
-        <v>264</v>
-      </c>
-      <c r="G4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="B5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E6" t="s">
-        <v>263</v>
-      </c>
-      <c r="F6" t="s">
-        <v>264</v>
-      </c>
-      <c r="G6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="B7" t="s">
-        <v>266</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" t="s">
-        <v>267</v>
-      </c>
-      <c r="F8" t="s">
-        <v>268</v>
-      </c>
-      <c r="G8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" t="s">
-        <v>269</v>
-      </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>270</v>
-      </c>
-      <c r="B11" t="s">
-        <v>270</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>271</v>
-      </c>
-      <c r="B13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>272</v>
-      </c>
-      <c r="B15" t="s">
-        <v>272</v>
-      </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B16" t="s">
-        <v>273</v>
-      </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>110</v>
-      </c>
-      <c r="E17" t="s">
-        <v>264</v>
-      </c>
-      <c r="F17" t="s">
-        <v>263</v>
-      </c>
-      <c r="G17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" t="s">
-        <v>274</v>
-      </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" t="s">
-        <v>105</v>
-      </c>
-      <c r="C20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" t="s">
-        <v>277</v>
-      </c>
-      <c r="C22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" t="s">
-        <v>278</v>
-      </c>
-      <c r="C25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" t="s">
-        <v>117</v>
-      </c>
-      <c r="C26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" t="s">
-        <v>280</v>
-      </c>
-      <c r="E27" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="B28" t="s">
-        <v>279</v>
-      </c>
-      <c r="C28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
-        <v>280</v>
-      </c>
-      <c r="E29" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7">
-      <c r="B30" t="s">
-        <v>282</v>
-      </c>
-      <c r="C30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="C31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" t="s">
-        <v>280</v>
-      </c>
-      <c r="E31" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7">
-      <c r="B32" t="s">
-        <v>283</v>
-      </c>
-      <c r="C32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5">
-      <c r="C33" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" t="s">
-        <v>114</v>
-      </c>
-      <c r="E33" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" t="s">
-        <v>284</v>
-      </c>
-      <c r="C34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="C35" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" t="s">
-        <v>114</v>
-      </c>
-      <c r="E35" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" t="s">
-        <v>285</v>
-      </c>
-      <c r="C36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5">
-      <c r="C37" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" t="s">
-        <v>114</v>
-      </c>
-      <c r="E37" t="s">
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A29DBD9-E94A-0143-B657-2C07F4BA4A49}">
-  <dimension ref="A1:F40"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" customWidth="1"/>
-    <col min="6" max="6" width="96" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="B1" t="s">
-        <v>602</v>
-      </c>
-      <c r="D1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="str">
-        <f>D2</f>
-        <v>monitoring_management</v>
-      </c>
-      <c r="B2" t="s">
-        <v>745</v>
-      </c>
-      <c r="C2" t="s">
-        <v>774</v>
-      </c>
-      <c r="D2" t="str">
-        <f>LOWER(C2)</f>
-        <v>monitoring_management</v>
-      </c>
-      <c r="E2" t="str">
-        <f>"right."&amp;D2&amp;"="&amp;B2</f>
-        <v>right.monitoring_management=监控管理</v>
-      </c>
-      <c r="F2" t="str">
-        <f>"right."&amp;D2&amp;"="&amp;D2</f>
-        <v>right.monitoring_management=monitoring_management</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="str">
-        <f>D3</f>
-        <v>the_server</v>
-      </c>
-      <c r="B3" t="s">
-        <v>746</v>
-      </c>
-      <c r="C3" t="s">
-        <v>775</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" ref="D3:D40" si="0">LOWER(C3)</f>
-        <v>the_server</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E40" si="1">"right."&amp;D3&amp;"="&amp;B3</f>
-        <v>right.the_server=服务器</v>
-      </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F40" si="2">"right."&amp;D3&amp;"="&amp;D3</f>
-        <v>right.the_server=the_server</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="str">
-        <f t="shared" ref="A4:A40" si="3">D4</f>
-        <v>to_view</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>717</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v>to_view</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" si="1"/>
-        <v>right.to_view=查看</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" si="2"/>
-        <v>right.to_view=to_view</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="str">
-        <f t="shared" si="3"/>
-        <v>the_editor</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>722</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>the_editor</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" si="1"/>
-        <v>right.the_editor=编辑</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="2"/>
-        <v>right.the_editor=the_editor</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="str">
-        <f t="shared" si="3"/>
-        <v>increase</v>
-      </c>
-      <c r="B6" t="s">
-        <v>397</v>
-      </c>
-      <c r="C6" t="s">
-        <v>539</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>increase</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="1"/>
-        <v>right.increase=增加</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="2"/>
-        <v>right.increase=increase</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="str">
-        <f t="shared" si="3"/>
-        <v>copy</v>
-      </c>
-      <c r="B7" t="s">
-        <v>522</v>
-      </c>
-      <c r="C7" t="s">
-        <v>540</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>copy</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="1"/>
-        <v>right.copy=复制</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="2"/>
-        <v>right.copy=copy</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="str">
-        <f t="shared" si="3"/>
-        <v>modify_the</v>
-      </c>
-      <c r="B8" t="s">
-        <v>523</v>
-      </c>
-      <c r="C8" t="s">
-        <v>776</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>modify_the</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" si="1"/>
-        <v>right.modify_the=修改</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="2"/>
-        <v>right.modify_the=modify_the</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="str">
-        <f t="shared" si="3"/>
-        <v>delete</v>
-      </c>
-      <c r="B9" t="s">
-        <v>350</v>
-      </c>
-      <c r="C9" t="s">
-        <v>536</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>delete</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="1"/>
-        <v>right.delete=删除</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="2"/>
-        <v>right.delete=delete</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="str">
-        <f t="shared" si="3"/>
-        <v>service</v>
-      </c>
-      <c r="B10" t="s">
-        <v>747</v>
-      </c>
-      <c r="C10" t="s">
-        <v>768</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>service</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="1"/>
-        <v>right.service=服务</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="2"/>
-        <v>right.service=service</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="str">
-        <f t="shared" si="3"/>
-        <v>the_alarm_event</v>
-      </c>
-      <c r="B11" t="s">
-        <v>748</v>
-      </c>
-      <c r="C11" t="s">
-        <v>777</v>
-      </c>
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v>the_alarm_event</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="1"/>
-        <v>right.the_alarm_event=告警事件</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="2"/>
-        <v>right.the_alarm_event=the_alarm_event</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="str">
-        <f t="shared" si="3"/>
-        <v>export</v>
-      </c>
-      <c r="B12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" t="s">
-        <v>541</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>export</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="1"/>
-        <v>right.export=导出</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="2"/>
-        <v>right.export=export</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="str">
-        <f t="shared" si="3"/>
-        <v>send</v>
-      </c>
-      <c r="B13" t="s">
-        <v>749</v>
-      </c>
-      <c r="C13" t="s">
-        <v>769</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v>send</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="1"/>
-        <v>right.send=发送</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="2"/>
-        <v>right.send=send</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="str">
-        <f t="shared" si="3"/>
-        <v>restore</v>
-      </c>
-      <c r="B14" t="s">
-        <v>750</v>
-      </c>
-      <c r="C14" t="s">
-        <v>770</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>restore</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="1"/>
-        <v>right.restore=恢复</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="2"/>
-        <v>right.restore=restore</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="str">
-        <f t="shared" si="3"/>
-        <v>event_statistics</v>
-      </c>
-      <c r="B15" t="s">
-        <v>751</v>
-      </c>
-      <c r="C15" t="s">
-        <v>778</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v>event_statistics</v>
-      </c>
-      <c r="E15" t="str">
-        <f t="shared" si="1"/>
-        <v>right.event_statistics=事件统计</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="2"/>
-        <v>right.event_statistics=event_statistics</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="str">
-        <f t="shared" si="3"/>
-        <v>tenant_log_management</v>
-      </c>
-      <c r="B16" t="s">
-        <v>752</v>
-      </c>
-      <c r="C16" t="s">
-        <v>779</v>
-      </c>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>tenant_log_management</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="shared" si="1"/>
-        <v>right.tenant_log_management=租户日志管理</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="2"/>
-        <v>right.tenant_log_management=tenant_log_management</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="str">
-        <f t="shared" si="3"/>
-        <v>application_icon_management</v>
-      </c>
-      <c r="B17" t="s">
-        <v>753</v>
-      </c>
-      <c r="C17" t="s">
-        <v>780</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v>application_icon_management</v>
-      </c>
-      <c r="E17" t="str">
-        <f t="shared" si="1"/>
-        <v>right.application_icon_management=应用图标管理</v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" si="2"/>
-        <v>right.application_icon_management=application_icon_management</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="str">
-        <f t="shared" si="3"/>
-        <v>add</v>
-      </c>
-      <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" t="s">
-        <v>651</v>
-      </c>
-      <c r="D18" t="str">
-        <f t="shared" si="0"/>
-        <v>add</v>
-      </c>
-      <c r="E18" t="str">
-        <f t="shared" si="1"/>
-        <v>right.add=添加</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="2"/>
-        <v>right.add=add</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="str">
-        <f t="shared" si="3"/>
-        <v>find_equipment</v>
-      </c>
-      <c r="B19" t="s">
-        <v>754</v>
-      </c>
-      <c r="C19" t="s">
-        <v>781</v>
-      </c>
-      <c r="D19" t="str">
-        <f t="shared" si="0"/>
-        <v>find_equipment</v>
-      </c>
-      <c r="E19" t="str">
-        <f t="shared" si="1"/>
-        <v>right.find_equipment=查找设备</v>
-      </c>
-      <c r="F19" t="str">
-        <f t="shared" si="2"/>
-        <v>right.find_equipment=find_equipment</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="str">
-        <f t="shared" si="3"/>
-        <v>system_management</v>
-      </c>
-      <c r="B20" t="s">
-        <v>310</v>
-      </c>
-      <c r="C20" t="s">
-        <v>575</v>
-      </c>
-      <c r="D20" t="str">
-        <f t="shared" si="0"/>
-        <v>system_management</v>
-      </c>
-      <c r="E20" t="str">
-        <f t="shared" si="1"/>
-        <v>right.system_management=系统管理</v>
-      </c>
-      <c r="F20" t="str">
-        <f t="shared" si="2"/>
-        <v>right.system_management=system_management</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="str">
-        <f t="shared" si="3"/>
-        <v>monitor_setting</v>
-      </c>
-      <c r="B21" t="s">
-        <v>755</v>
-      </c>
-      <c r="C21" t="s">
-        <v>782</v>
-      </c>
-      <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v>monitor_setting</v>
-      </c>
-      <c r="E21" t="str">
-        <f t="shared" si="1"/>
-        <v>right.monitor_setting=监控设置</v>
-      </c>
-      <c r="F21" t="str">
-        <f t="shared" si="2"/>
-        <v>right.monitor_setting=monitor_setting</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="str">
-        <f t="shared" si="3"/>
-        <v>sms_notification_management</v>
-      </c>
-      <c r="B22" t="s">
-        <v>756</v>
-      </c>
-      <c r="C22" t="s">
-        <v>783</v>
-      </c>
-      <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v>sms_notification_management</v>
-      </c>
-      <c r="E22" t="str">
-        <f t="shared" si="1"/>
-        <v>right.sms_notification_management=短信通知管理</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" si="2"/>
-        <v>right.sms_notification_management=sms_notification_management</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="str">
-        <f t="shared" si="3"/>
-        <v>save_sms_notification_settings</v>
-      </c>
-      <c r="B23" t="s">
-        <v>757</v>
-      </c>
-      <c r="C23" t="s">
-        <v>784</v>
-      </c>
-      <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v>save_sms_notification_settings</v>
-      </c>
-      <c r="E23" t="str">
-        <f t="shared" si="1"/>
-        <v>right.save_sms_notification_settings=保存短信通知设置</v>
-      </c>
-      <c r="F23" t="str">
-        <f t="shared" si="2"/>
-        <v>right.save_sms_notification_settings=save_sms_notification_settings</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="str">
-        <f t="shared" si="3"/>
-        <v>system_settings</v>
-      </c>
-      <c r="B24" t="s">
-        <v>392</v>
-      </c>
-      <c r="C24" t="s">
-        <v>576</v>
-      </c>
-      <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v>system_settings</v>
-      </c>
-      <c r="E24" t="str">
-        <f t="shared" si="1"/>
-        <v>right.system_settings=系统设置</v>
-      </c>
-      <c r="F24" t="str">
-        <f t="shared" si="2"/>
-        <v>right.system_settings=system_settings</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="str">
-        <f t="shared" si="3"/>
-        <v>download_limit_settings</v>
-      </c>
-      <c r="B25" t="s">
-        <v>758</v>
-      </c>
-      <c r="C25" t="s">
-        <v>785</v>
-      </c>
-      <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>download_limit_settings</v>
-      </c>
-      <c r="E25" t="str">
-        <f t="shared" si="1"/>
-        <v>right.download_limit_settings=下载限制设置</v>
-      </c>
-      <c r="F25" t="str">
-        <f t="shared" si="2"/>
-        <v>right.download_limit_settings=download_limit_settings</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="str">
-        <f t="shared" si="3"/>
-        <v>downloading_device_logs</v>
-      </c>
-      <c r="B26" t="s">
-        <v>759</v>
-      </c>
-      <c r="C26" t="s">
-        <v>786</v>
-      </c>
-      <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v>downloading_device_logs</v>
-      </c>
-      <c r="E26" t="str">
-        <f t="shared" si="1"/>
-        <v>right.downloading_device_logs=设备日志下载</v>
-      </c>
-      <c r="F26" t="str">
-        <f t="shared" si="2"/>
-        <v>right.downloading_device_logs=downloading_device_logs</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="str">
-        <f t="shared" si="3"/>
-        <v>download</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>650</v>
-      </c>
-      <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>download</v>
-      </c>
-      <c r="E27" t="str">
-        <f t="shared" si="1"/>
-        <v>right.download=下载</v>
-      </c>
-      <c r="F27" t="str">
-        <f t="shared" si="2"/>
-        <v>right.download=download</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="str">
-        <f t="shared" si="3"/>
-        <v>administrator_operation_logs</v>
-      </c>
-      <c r="B28" t="s">
-        <v>387</v>
-      </c>
-      <c r="C28" t="s">
-        <v>574</v>
-      </c>
-      <c r="D28" t="str">
-        <f t="shared" si="0"/>
-        <v>administrator_operation_logs</v>
-      </c>
-      <c r="E28" t="str">
-        <f t="shared" si="1"/>
-        <v>right.administrator_operation_logs=管理员操作日志</v>
-      </c>
-      <c r="F28" t="str">
-        <f t="shared" si="2"/>
-        <v>right.administrator_operation_logs=administrator_operation_logs</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="str">
-        <f t="shared" si="3"/>
-        <v>gateway_call_log</v>
-      </c>
-      <c r="B29" t="s">
-        <v>760</v>
-      </c>
-      <c r="C29" t="s">
-        <v>787</v>
-      </c>
-      <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>gateway_call_log</v>
-      </c>
-      <c r="E29" t="str">
-        <f t="shared" si="1"/>
-        <v>right.gateway_call_log=网关调用日志</v>
-      </c>
-      <c r="F29" t="str">
-        <f t="shared" si="2"/>
-        <v>right.gateway_call_log=gateway_call_log</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="str">
-        <f t="shared" si="3"/>
-        <v>cope_client_upgrade</v>
-      </c>
-      <c r="B30" t="s">
-        <v>405</v>
-      </c>
-      <c r="C30" t="s">
-        <v>788</v>
-      </c>
-      <c r="D30" t="str">
-        <f t="shared" si="0"/>
-        <v>cope_client_upgrade</v>
-      </c>
-      <c r="E30" t="str">
-        <f t="shared" si="1"/>
-        <v>right.cope_client_upgrade=COPE客户端升级</v>
-      </c>
-      <c r="F30" t="str">
-        <f t="shared" si="2"/>
-        <v>right.cope_client_upgrade=cope_client_upgrade</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="str">
-        <f t="shared" si="3"/>
-        <v>uploading_a_client</v>
-      </c>
-      <c r="B31" t="s">
-        <v>761</v>
-      </c>
-      <c r="C31" t="s">
-        <v>789</v>
-      </c>
-      <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v>uploading_a_client</v>
-      </c>
-      <c r="E31" t="str">
-        <f t="shared" si="1"/>
-        <v>right.uploading_a_client=上传客户端</v>
-      </c>
-      <c r="F31" t="str">
-        <f t="shared" si="2"/>
-        <v>right.uploading_a_client=uploading_a_client</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="str">
-        <f t="shared" si="3"/>
-        <v>push</v>
-      </c>
-      <c r="B32" t="s">
-        <v>762</v>
-      </c>
-      <c r="C32" t="s">
-        <v>771</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>push</v>
-      </c>
-      <c r="E32" t="str">
-        <f t="shared" si="1"/>
-        <v>right.push=推送</v>
-      </c>
-      <c r="F32" t="str">
-        <f t="shared" si="2"/>
-        <v>right.push=push</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="str">
-        <f t="shared" si="3"/>
-        <v>upgrade_the_byod_client</v>
-      </c>
-      <c r="B33" t="s">
-        <v>763</v>
-      </c>
-      <c r="C33" t="s">
-        <v>790</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>upgrade_the_byod_client</v>
-      </c>
-      <c r="E33" t="str">
-        <f t="shared" si="1"/>
-        <v>right.upgrade_the_byod_client=BYOD客户端升级</v>
-      </c>
-      <c r="F33" t="str">
-        <f t="shared" si="2"/>
-        <v>right.upgrade_the_byod_client=upgrade_the_byod_client</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="str">
-        <f t="shared" si="3"/>
-        <v>the_ios_client_is_upgraded</v>
-      </c>
-      <c r="B34" t="s">
-        <v>764</v>
-      </c>
-      <c r="C34" t="s">
-        <v>791</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" si="0"/>
-        <v>the_ios_client_is_upgraded</v>
-      </c>
-      <c r="E34" t="str">
-        <f t="shared" si="1"/>
-        <v>right.the_ios_client_is_upgraded=IOS客户端升级</v>
-      </c>
-      <c r="F34" t="str">
-        <f t="shared" si="2"/>
-        <v>right.the_ios_client_is_upgraded=the_ios_client_is_upgraded</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="str">
-        <f t="shared" si="3"/>
-        <v>tenant_feedback</v>
-      </c>
-      <c r="B35" t="s">
-        <v>765</v>
-      </c>
-      <c r="C35" t="s">
-        <v>792</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v>tenant_feedback</v>
-      </c>
-      <c r="E35" t="str">
-        <f t="shared" si="1"/>
-        <v>right.tenant_feedback=租户意见反馈</v>
-      </c>
-      <c r="F35" t="str">
-        <f t="shared" si="2"/>
-        <v>right.tenant_feedback=tenant_feedback</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" t="str">
-        <f t="shared" si="3"/>
-        <v>reply</v>
-      </c>
-      <c r="B36" t="s">
-        <v>402</v>
-      </c>
-      <c r="C36" t="s">
-        <v>772</v>
-      </c>
-      <c r="D36" t="str">
-        <f t="shared" si="0"/>
-        <v>reply</v>
-      </c>
-      <c r="E36" t="str">
-        <f t="shared" si="1"/>
-        <v>right.reply=回复</v>
-      </c>
-      <c r="F36" t="str">
-        <f t="shared" si="2"/>
-        <v>right.reply=reply</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="str">
-        <f t="shared" si="3"/>
-        <v>ignore</v>
-      </c>
-      <c r="B37" t="s">
-        <v>403</v>
-      </c>
-      <c r="C37" t="s">
-        <v>773</v>
-      </c>
-      <c r="D37" t="str">
-        <f t="shared" si="0"/>
-        <v>ignore</v>
-      </c>
-      <c r="E37" t="str">
-        <f t="shared" si="1"/>
-        <v>right.ignore=忽略</v>
-      </c>
-      <c r="F37" t="str">
-        <f t="shared" si="2"/>
-        <v>right.ignore=ignore</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" t="str">
-        <f t="shared" si="3"/>
-        <v>android_feedback</v>
-      </c>
-      <c r="B38" t="s">
-        <v>766</v>
-      </c>
-      <c r="C38" t="s">
-        <v>793</v>
-      </c>
-      <c r="D38" t="str">
-        <f t="shared" si="0"/>
-        <v>android_feedback</v>
-      </c>
-      <c r="E38" t="str">
-        <f t="shared" si="1"/>
-        <v>right.android_feedback=Android意见反馈</v>
-      </c>
-      <c r="F38" t="str">
-        <f t="shared" si="2"/>
-        <v>right.android_feedback=android_feedback</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" t="str">
-        <f t="shared" si="3"/>
-        <v>ios_feedback</v>
-      </c>
-      <c r="B39" t="s">
-        <v>767</v>
-      </c>
-      <c r="C39" t="s">
-        <v>794</v>
-      </c>
-      <c r="D39" t="str">
-        <f t="shared" si="0"/>
-        <v>ios_feedback</v>
-      </c>
-      <c r="E39" t="str">
-        <f t="shared" si="1"/>
-        <v>right.ios_feedback=IOS意见反馈</v>
-      </c>
-      <c r="F39" t="str">
-        <f t="shared" si="2"/>
-        <v>right.ios_feedback=ios_feedback</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="str">
-        <f t="shared" si="3"/>
-        <v>the_front_panel</v>
-      </c>
-      <c r="B40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" t="s">
-        <v>425</v>
-      </c>
-      <c r="D40" t="str">
-        <f t="shared" si="0"/>
-        <v>the_front_panel</v>
-      </c>
-      <c r="E40" t="str">
-        <f t="shared" si="1"/>
-        <v>right.the_front_panel=首页面板</v>
-      </c>
-      <c r="F40" t="str">
-        <f t="shared" si="2"/>
-        <v>right.the_front_panel=the_front_panel</v>
       </c>
     </row>
   </sheetData>
@@ -19244,6 +18273,1437 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73F9AB08-A3B8-514B-AD13-E0375A045A1B}">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B1" t="s">
+        <v>796</v>
+      </c>
+      <c r="C1" t="s">
+        <v>797</v>
+      </c>
+      <c r="D1" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" t="s">
+        <v>263</v>
+      </c>
+      <c r="F4" t="s">
+        <v>264</v>
+      </c>
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" t="s">
+        <v>263</v>
+      </c>
+      <c r="F6" t="s">
+        <v>264</v>
+      </c>
+      <c r="G6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" t="s">
+        <v>267</v>
+      </c>
+      <c r="F8" t="s">
+        <v>268</v>
+      </c>
+      <c r="G8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>270</v>
+      </c>
+      <c r="B11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>271</v>
+      </c>
+      <c r="B13" t="s">
+        <v>271</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>272</v>
+      </c>
+      <c r="B15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" t="s">
+        <v>273</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" t="s">
+        <v>264</v>
+      </c>
+      <c r="F17" t="s">
+        <v>263</v>
+      </c>
+      <c r="G17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" t="s">
+        <v>274</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" t="s">
+        <v>277</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" t="s">
+        <v>278</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>280</v>
+      </c>
+      <c r="E27" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" t="s">
+        <v>279</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>280</v>
+      </c>
+      <c r="E29" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" t="s">
+        <v>282</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>280</v>
+      </c>
+      <c r="E31" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" t="s">
+        <v>283</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>114</v>
+      </c>
+      <c r="E33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" t="s">
+        <v>284</v>
+      </c>
+      <c r="C34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" t="s">
+        <v>285</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A29DBD9-E94A-0143-B657-2C07F4BA4A49}">
+  <dimension ref="A1:F40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="46" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" customWidth="1"/>
+    <col min="6" max="6" width="96" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" t="s">
+        <v>602</v>
+      </c>
+      <c r="D1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="str">
+        <f>D2</f>
+        <v>monitoring_management</v>
+      </c>
+      <c r="B2" t="s">
+        <v>745</v>
+      </c>
+      <c r="C2" t="s">
+        <v>774</v>
+      </c>
+      <c r="D2" t="str">
+        <f>LOWER(C2)</f>
+        <v>monitoring_management</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"right."&amp;D2&amp;"="&amp;B2</f>
+        <v>right.monitoring_management=监控管理</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"right."&amp;D2&amp;"="&amp;D2</f>
+        <v>right.monitoring_management=monitoring_management</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="str">
+        <f>D3</f>
+        <v>the_server</v>
+      </c>
+      <c r="B3" t="s">
+        <v>746</v>
+      </c>
+      <c r="C3" t="s">
+        <v>775</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D40" si="0">LOWER(C3)</f>
+        <v>the_server</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E40" si="1">"right."&amp;D3&amp;"="&amp;B3</f>
+        <v>right.the_server=服务器</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F40" si="2">"right."&amp;D3&amp;"="&amp;D3</f>
+        <v>right.the_server=the_server</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A40" si="3">D4</f>
+        <v>to_view</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>717</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>to_view</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>right.to_view=查看</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="2"/>
+        <v>right.to_view=to_view</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="str">
+        <f t="shared" si="3"/>
+        <v>the_editor</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>722</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>the_editor</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>right.the_editor=编辑</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_editor=the_editor</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="str">
+        <f t="shared" si="3"/>
+        <v>increase</v>
+      </c>
+      <c r="B6" t="s">
+        <v>397</v>
+      </c>
+      <c r="C6" t="s">
+        <v>539</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>increase</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>right.increase=增加</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="2"/>
+        <v>right.increase=increase</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="str">
+        <f t="shared" si="3"/>
+        <v>copy</v>
+      </c>
+      <c r="B7" t="s">
+        <v>522</v>
+      </c>
+      <c r="C7" t="s">
+        <v>540</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>copy</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>right.copy=复制</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="2"/>
+        <v>right.copy=copy</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="str">
+        <f t="shared" si="3"/>
+        <v>modify_the</v>
+      </c>
+      <c r="B8" t="s">
+        <v>523</v>
+      </c>
+      <c r="C8" t="s">
+        <v>776</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>modify_the</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>right.modify_the=修改</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="2"/>
+        <v>right.modify_the=modify_the</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="str">
+        <f t="shared" si="3"/>
+        <v>delete</v>
+      </c>
+      <c r="B9" t="s">
+        <v>350</v>
+      </c>
+      <c r="C9" t="s">
+        <v>536</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>delete</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>right.delete=删除</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="2"/>
+        <v>right.delete=delete</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="str">
+        <f t="shared" si="3"/>
+        <v>service</v>
+      </c>
+      <c r="B10" t="s">
+        <v>747</v>
+      </c>
+      <c r="C10" t="s">
+        <v>768</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>service</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>right.service=服务</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="2"/>
+        <v>right.service=service</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="str">
+        <f t="shared" si="3"/>
+        <v>the_alarm_event</v>
+      </c>
+      <c r="B11" t="s">
+        <v>748</v>
+      </c>
+      <c r="C11" t="s">
+        <v>777</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>the_alarm_event</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>right.the_alarm_event=告警事件</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_alarm_event=the_alarm_event</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="str">
+        <f t="shared" si="3"/>
+        <v>export</v>
+      </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>541</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>export</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>right.export=导出</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="2"/>
+        <v>right.export=export</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="str">
+        <f t="shared" si="3"/>
+        <v>send</v>
+      </c>
+      <c r="B13" t="s">
+        <v>749</v>
+      </c>
+      <c r="C13" t="s">
+        <v>769</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>send</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>right.send=发送</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="2"/>
+        <v>right.send=send</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="str">
+        <f t="shared" si="3"/>
+        <v>restore</v>
+      </c>
+      <c r="B14" t="s">
+        <v>750</v>
+      </c>
+      <c r="C14" t="s">
+        <v>770</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>restore</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>right.restore=恢复</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="2"/>
+        <v>right.restore=restore</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="str">
+        <f t="shared" si="3"/>
+        <v>event_statistics</v>
+      </c>
+      <c r="B15" t="s">
+        <v>751</v>
+      </c>
+      <c r="C15" t="s">
+        <v>778</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>event_statistics</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>right.event_statistics=事件统计</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="2"/>
+        <v>right.event_statistics=event_statistics</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="str">
+        <f t="shared" si="3"/>
+        <v>tenant_log_management</v>
+      </c>
+      <c r="B16" t="s">
+        <v>752</v>
+      </c>
+      <c r="C16" t="s">
+        <v>779</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>tenant_log_management</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>right.tenant_log_management=租户日志管理</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="2"/>
+        <v>right.tenant_log_management=tenant_log_management</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="str">
+        <f t="shared" si="3"/>
+        <v>application_icon_management</v>
+      </c>
+      <c r="B17" t="s">
+        <v>753</v>
+      </c>
+      <c r="C17" t="s">
+        <v>780</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>application_icon_management</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>right.application_icon_management=应用图标管理</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="2"/>
+        <v>right.application_icon_management=application_icon_management</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="str">
+        <f t="shared" si="3"/>
+        <v>add</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>651</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>add</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>right.add=添加</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="2"/>
+        <v>right.add=add</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="str">
+        <f t="shared" si="3"/>
+        <v>find_equipment</v>
+      </c>
+      <c r="B19" t="s">
+        <v>754</v>
+      </c>
+      <c r="C19" t="s">
+        <v>781</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>find_equipment</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>right.find_equipment=查找设备</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="2"/>
+        <v>right.find_equipment=find_equipment</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="str">
+        <f t="shared" si="3"/>
+        <v>system_management</v>
+      </c>
+      <c r="B20" t="s">
+        <v>310</v>
+      </c>
+      <c r="C20" t="s">
+        <v>575</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>system_management</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>right.system_management=系统管理</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="2"/>
+        <v>right.system_management=system_management</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="str">
+        <f t="shared" si="3"/>
+        <v>monitor_setting</v>
+      </c>
+      <c r="B21" t="s">
+        <v>755</v>
+      </c>
+      <c r="C21" t="s">
+        <v>782</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>monitor_setting</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>right.monitor_setting=监控设置</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="2"/>
+        <v>right.monitor_setting=monitor_setting</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="str">
+        <f t="shared" si="3"/>
+        <v>sms_notification_management</v>
+      </c>
+      <c r="B22" t="s">
+        <v>756</v>
+      </c>
+      <c r="C22" t="s">
+        <v>783</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>sms_notification_management</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>right.sms_notification_management=短信通知管理</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="2"/>
+        <v>right.sms_notification_management=sms_notification_management</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="str">
+        <f t="shared" si="3"/>
+        <v>save_sms_notification_settings</v>
+      </c>
+      <c r="B23" t="s">
+        <v>757</v>
+      </c>
+      <c r="C23" t="s">
+        <v>784</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>save_sms_notification_settings</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>right.save_sms_notification_settings=保存短信通知设置</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="2"/>
+        <v>right.save_sms_notification_settings=save_sms_notification_settings</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="str">
+        <f t="shared" si="3"/>
+        <v>system_settings</v>
+      </c>
+      <c r="B24" t="s">
+        <v>392</v>
+      </c>
+      <c r="C24" t="s">
+        <v>576</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>system_settings</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>right.system_settings=系统设置</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="2"/>
+        <v>right.system_settings=system_settings</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="str">
+        <f t="shared" si="3"/>
+        <v>download_limit_settings</v>
+      </c>
+      <c r="B25" t="s">
+        <v>758</v>
+      </c>
+      <c r="C25" t="s">
+        <v>785</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>download_limit_settings</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>right.download_limit_settings=下载限制设置</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="2"/>
+        <v>right.download_limit_settings=download_limit_settings</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="str">
+        <f t="shared" si="3"/>
+        <v>downloading_device_logs</v>
+      </c>
+      <c r="B26" t="s">
+        <v>759</v>
+      </c>
+      <c r="C26" t="s">
+        <v>786</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>downloading_device_logs</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>right.downloading_device_logs=设备日志下载</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="2"/>
+        <v>right.downloading_device_logs=downloading_device_logs</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="str">
+        <f t="shared" si="3"/>
+        <v>download</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>650</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>download</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>right.download=下载</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="2"/>
+        <v>right.download=download</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="str">
+        <f t="shared" si="3"/>
+        <v>administrator_operation_logs</v>
+      </c>
+      <c r="B28" t="s">
+        <v>387</v>
+      </c>
+      <c r="C28" t="s">
+        <v>574</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>administrator_operation_logs</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>right.administrator_operation_logs=管理员操作日志</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="2"/>
+        <v>right.administrator_operation_logs=administrator_operation_logs</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="str">
+        <f t="shared" si="3"/>
+        <v>gateway_call_log</v>
+      </c>
+      <c r="B29" t="s">
+        <v>760</v>
+      </c>
+      <c r="C29" t="s">
+        <v>787</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>gateway_call_log</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>right.gateway_call_log=网关调用日志</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="2"/>
+        <v>right.gateway_call_log=gateway_call_log</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="str">
+        <f t="shared" si="3"/>
+        <v>cope_client_upgrade</v>
+      </c>
+      <c r="B30" t="s">
+        <v>405</v>
+      </c>
+      <c r="C30" t="s">
+        <v>788</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>cope_client_upgrade</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>right.cope_client_upgrade=COPE客户端升级</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="2"/>
+        <v>right.cope_client_upgrade=cope_client_upgrade</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="str">
+        <f t="shared" si="3"/>
+        <v>uploading_a_client</v>
+      </c>
+      <c r="B31" t="s">
+        <v>761</v>
+      </c>
+      <c r="C31" t="s">
+        <v>789</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>uploading_a_client</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>right.uploading_a_client=上传客户端</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="2"/>
+        <v>right.uploading_a_client=uploading_a_client</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="str">
+        <f t="shared" si="3"/>
+        <v>push</v>
+      </c>
+      <c r="B32" t="s">
+        <v>762</v>
+      </c>
+      <c r="C32" t="s">
+        <v>771</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>push</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>right.push=推送</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="2"/>
+        <v>right.push=push</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="str">
+        <f t="shared" si="3"/>
+        <v>upgrade_the_byod_client</v>
+      </c>
+      <c r="B33" t="s">
+        <v>763</v>
+      </c>
+      <c r="C33" t="s">
+        <v>790</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>upgrade_the_byod_client</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>right.upgrade_the_byod_client=BYOD客户端升级</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="2"/>
+        <v>right.upgrade_the_byod_client=upgrade_the_byod_client</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="str">
+        <f t="shared" si="3"/>
+        <v>the_ios_client_is_upgraded</v>
+      </c>
+      <c r="B34" t="s">
+        <v>764</v>
+      </c>
+      <c r="C34" t="s">
+        <v>791</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>the_ios_client_is_upgraded</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="1"/>
+        <v>right.the_ios_client_is_upgraded=IOS客户端升级</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_ios_client_is_upgraded=the_ios_client_is_upgraded</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="str">
+        <f t="shared" si="3"/>
+        <v>tenant_feedback</v>
+      </c>
+      <c r="B35" t="s">
+        <v>765</v>
+      </c>
+      <c r="C35" t="s">
+        <v>792</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>tenant_feedback</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="1"/>
+        <v>right.tenant_feedback=租户意见反馈</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="2"/>
+        <v>right.tenant_feedback=tenant_feedback</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="str">
+        <f t="shared" si="3"/>
+        <v>reply</v>
+      </c>
+      <c r="B36" t="s">
+        <v>402</v>
+      </c>
+      <c r="C36" t="s">
+        <v>772</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>reply</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="1"/>
+        <v>right.reply=回复</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="2"/>
+        <v>right.reply=reply</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="str">
+        <f t="shared" si="3"/>
+        <v>ignore</v>
+      </c>
+      <c r="B37" t="s">
+        <v>403</v>
+      </c>
+      <c r="C37" t="s">
+        <v>773</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>ignore</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="1"/>
+        <v>right.ignore=忽略</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="2"/>
+        <v>right.ignore=ignore</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="str">
+        <f t="shared" si="3"/>
+        <v>android_feedback</v>
+      </c>
+      <c r="B38" t="s">
+        <v>766</v>
+      </c>
+      <c r="C38" t="s">
+        <v>793</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>android_feedback</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="1"/>
+        <v>right.android_feedback=Android意见反馈</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="2"/>
+        <v>right.android_feedback=android_feedback</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="str">
+        <f t="shared" si="3"/>
+        <v>ios_feedback</v>
+      </c>
+      <c r="B39" t="s">
+        <v>767</v>
+      </c>
+      <c r="C39" t="s">
+        <v>794</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>ios_feedback</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="1"/>
+        <v>right.ios_feedback=IOS意见反馈</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="2"/>
+        <v>right.ios_feedback=ios_feedback</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="str">
+        <f t="shared" si="3"/>
+        <v>the_front_panel</v>
+      </c>
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>425</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>the_front_panel</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="1"/>
+        <v>right.the_front_panel=首页面板</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_front_panel=the_front_panel</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DDFF0F-151D-2C4F-8ADA-466E373776C8}">
   <dimension ref="A1:E181"/>
   <sheetViews>
@@ -21341,7 +21801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89C31BD-9216-6A49-8C90-0ADAF2498DB4}">
   <dimension ref="A1:D14"/>
   <sheetViews>

</xml_diff>

<commit_message>
vault backup: 2022-01-24 13:05:20
Affected files:
1附件/权限列表.xlsx
</commit_message>
<xml_diff>
--- a/1附件/权限列表.xlsx
+++ b/1附件/权限列表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2BF31D-9AB5-C248-92D4-277E10F4CC0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E6D818-6F1A-7648-982E-B10A41DB6AEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="7" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
@@ -28923,7 +28923,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -28970,7 +28970,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A21" si="0">D3</f>
+        <f t="shared" ref="A3:A27" si="0">D3</f>
         <v>apple_device_management</v>
       </c>
       <c r="B3" t="s">
@@ -28980,15 +28980,15 @@
         <v>857</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D21" si="1">LOWER(C3)</f>
+        <f t="shared" ref="D3:D27" si="1">LOWER(C3)</f>
         <v>apple_device_management</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E21" si="2">"right."&amp;D3&amp;"="&amp;B3</f>
+        <f t="shared" ref="E3:E27" si="2">"right."&amp;D3&amp;"="&amp;B3</f>
         <v>right.apple_device_management=苹果设备管理</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F21" si="3">"right."&amp;D3&amp;"="&amp;D3</f>
+        <f t="shared" ref="F3:F27" si="3">"right."&amp;D3&amp;"="&amp;D3</f>
         <v>right.apple_device_management=apple_device_management</v>
       </c>
     </row>
@@ -29425,51 +29425,147 @@
       </c>
     </row>
     <row r="22" spans="1:6">
+      <c r="A22" t="str">
+        <f>D22</f>
+        <v>disable</v>
+      </c>
       <c r="B22" t="s">
         <v>353</v>
       </c>
       <c r="C22" t="s">
         <v>534</v>
       </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>disable</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="2"/>
+        <v>right.disable=停用</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="3"/>
+        <v>right.disable=disable</v>
+      </c>
     </row>
     <row r="23" spans="1:6">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>to_enable_the</v>
+      </c>
       <c r="B23" t="s">
         <v>851</v>
       </c>
       <c r="C23" t="s">
         <v>872</v>
       </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>to_enable_the</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="2"/>
+        <v>right.to_enable_the=启用</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="3"/>
+        <v>right.to_enable_the=to_enable_the</v>
+      </c>
     </row>
     <row r="24" spans="1:6">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>distribution</v>
+      </c>
       <c r="B24" t="s">
         <v>62</v>
       </c>
       <c r="C24" t="s">
         <v>856</v>
       </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>distribution</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="2"/>
+        <v>right.distribution=分发</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="3"/>
+        <v>right.distribution=distribution</v>
+      </c>
     </row>
     <row r="25" spans="1:6">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>user_management</v>
+      </c>
       <c r="B25" t="s">
         <v>292</v>
       </c>
       <c r="C25" t="s">
         <v>729</v>
       </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>user_management</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="2"/>
+        <v>right.user_management=用户管理</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="3"/>
+        <v>right.user_management=user_management</v>
+      </c>
     </row>
     <row r="26" spans="1:6">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>the_user_group</v>
+      </c>
       <c r="B26" t="s">
         <v>298</v>
       </c>
       <c r="C26" t="s">
         <v>814</v>
       </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>the_user_group</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="2"/>
+        <v>right.the_user_group=用户分组</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="3"/>
+        <v>right.the_user_group=the_user_group</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v>remove_the_group</v>
+      </c>
       <c r="B27" t="s">
         <v>505</v>
       </c>
       <c r="C27" t="s">
         <v>564</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>remove_the_group</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="2"/>
+        <v>right.remove_the_group=移除分组</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="3"/>
+        <v>right.remove_the_group=remove_the_group</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2022-01-24 14:05:23
Affected files:
.obsidian/plugins/rss-reader/data.json
14TODO/TODO.md
1附件/~$权限列表.xlsx
1附件/权限列表.xlsx
</commit_message>
<xml_diff>
--- a/1附件/权限列表.xlsx
+++ b/1附件/权限列表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E6D818-6F1A-7648-982E-B10A41DB6AEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889F7AC5-352F-5D44-96BE-43665B3BF041}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="7" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3945" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3945" uniqueCount="874">
   <si>
     <t>首页面板</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3257,6 +3257,44 @@
   </si>
   <si>
     <t>To_enable_the</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>'function_ios_dev_management'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF6A8759"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>'func'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FFCC7832"/>
+        <rFont val="JetBrains Mono"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -15247,31 +15285,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A421E20D-3F20-FF4A-A250-792992ED1A42}">
   <dimension ref="A1:E181"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="L84" sqref="L84"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4">
-        <v>0</v>
+        <v>546</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C1" t="str">
         <f>B1&amp;""&amp;A1&amp;D1&amp;A1&amp;E1</f>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (0, '2', 'funcId',0);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (546, 'function_ios_dev_management', 'func',546);</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>414</v>
+        <v>873</v>
       </c>
       <c r="E1" t="s">
         <v>413</v>
@@ -15279,17 +15317,17 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4">
-        <v>1</v>
+        <v>547</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C65" si="0">B2&amp;""&amp;A2&amp;D2&amp;A2&amp;E2</f>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (1, '2', 'funcId',1);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (547, 'function_ios_dev_management', 'func',547);</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>414</v>
+        <v>873</v>
       </c>
       <c r="E2" t="s">
         <v>413</v>
@@ -15297,17 +15335,17 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4">
-        <v>2</v>
+        <v>548</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (2, '2', 'funcId',2);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (548, 'function_ios_dev_management', 'func',548);</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>415</v>
+        <v>873</v>
       </c>
       <c r="E3" t="s">
         <v>413</v>
@@ -15315,17 +15353,17 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4">
-        <v>3</v>
+        <v>549</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (3, '2', 'funcId',3);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (549, 'function_ios_dev_management', 'func',549);</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>415</v>
+        <v>873</v>
       </c>
       <c r="E4" t="s">
         <v>413</v>
@@ -15333,17 +15371,17 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4">
-        <v>4</v>
+        <v>550</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (4, '2', 'funcId',4);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (550, 'function_ios_dev_management', 'func',550);</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>415</v>
+        <v>873</v>
       </c>
       <c r="E5" t="s">
         <v>413</v>
@@ -15351,17 +15389,17 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4">
-        <v>5</v>
+        <v>551</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (5, '2', 'funcId',5);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (551, 'function_ios_dev_management', 'func',551);</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>415</v>
+        <v>873</v>
       </c>
       <c r="E6" t="s">
         <v>413</v>
@@ -15369,17 +15407,17 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4">
-        <v>6</v>
+        <v>552</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (6, '2', 'funcId',6);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (552, 'function_ios_dev_management', 'func',552);</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>415</v>
+        <v>873</v>
       </c>
       <c r="E7" t="s">
         <v>413</v>
@@ -15387,17 +15425,17 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4">
-        <v>7</v>
+        <v>553</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (7, '2', 'funcId',7);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (553, 'function_ios_dev_management', 'func',553);</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>415</v>
+        <v>873</v>
       </c>
       <c r="E8" t="s">
         <v>413</v>
@@ -15405,17 +15443,17 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4">
-        <v>8</v>
+        <v>554</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (8, '2', 'funcId',8);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (554, 'function_ios_dev_management', 'func',554);</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>415</v>
+        <v>873</v>
       </c>
       <c r="E9" t="s">
         <v>413</v>
@@ -15423,17 +15461,17 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="4">
-        <v>9</v>
+        <v>555</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (9, '2', 'funcId',9);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (555, 'function_ios_dev_management', 'func',555);</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>415</v>
+        <v>873</v>
       </c>
       <c r="E10" t="s">
         <v>413</v>
@@ -15441,17 +15479,17 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="4">
-        <v>10</v>
+        <v>556</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (10, '2', 'funcId',10);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (556, 'function_ios_dev_management', 'func',556);</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>415</v>
+        <v>873</v>
       </c>
       <c r="E11" t="s">
         <v>413</v>
@@ -15459,17 +15497,17 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4">
-        <v>11</v>
+        <v>557</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (11, '2', 'funcId',11);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (557, 'function_ios_dev_management', 'func',557);</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>415</v>
+        <v>873</v>
       </c>
       <c r="E12" t="s">
         <v>413</v>
@@ -15477,14 +15515,14 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4">
-        <v>12</v>
+        <v>558</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (12, '2', 'funcId',12);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (558, '2', 'funcId',558);</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>415</v>
@@ -15495,14 +15533,14 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="4">
-        <v>13</v>
+        <v>559</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (13, '2', 'funcId',13);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (559, '2', 'funcId',559);</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>415</v>
@@ -15513,14 +15551,14 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="4">
-        <v>14</v>
+        <v>560</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (14, '2', 'funcId',14);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (560, '2', 'funcId',560);</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>415</v>
@@ -15531,14 +15569,14 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4">
-        <v>15</v>
+        <v>561</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (15, '2', 'funcId',15);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (561, '2', 'funcId',561);</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>415</v>
@@ -15549,14 +15587,14 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="4">
-        <v>16</v>
+        <v>562</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (16, '2', 'funcId',16);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (562, '2', 'funcId',562);</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>415</v>
@@ -15567,14 +15605,14 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="4">
-        <v>17</v>
+        <v>563</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (17, '2', 'funcId',17);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (563, '2', 'funcId',563);</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>415</v>
@@ -15585,14 +15623,14 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="4">
-        <v>18</v>
+        <v>564</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (18, '2', 'funcId',18);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (564, '2', 'funcId',564);</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>415</v>
@@ -15603,14 +15641,14 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="4">
-        <v>19</v>
+        <v>565</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (19, '2', 'funcId',19);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (565, '2', 'funcId',565);</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>415</v>
@@ -15621,14 +15659,14 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="4">
-        <v>20</v>
+        <v>566</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (20, '2', 'funcId',20);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (566, '2', 'funcId',566);</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>415</v>
@@ -15639,14 +15677,14 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="4">
-        <v>21</v>
+        <v>567</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (21, '2', 'funcId',21);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (567, '2', 'funcId',567);</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>415</v>
@@ -15657,14 +15695,14 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="4">
-        <v>22</v>
+        <v>568</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (22, '2', 'funcId',22);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (568, '2', 'funcId',568);</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>415</v>
@@ -15675,14 +15713,14 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="4">
-        <v>23</v>
+        <v>569</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (23, '2', 'funcId',23);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (569, '2', 'funcId',569);</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>415</v>
@@ -15693,14 +15731,14 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="4">
-        <v>24</v>
+        <v>570</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (24, '2', 'funcId',24);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (570, '2', 'funcId',570);</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>415</v>
@@ -15711,14 +15749,14 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="4">
-        <v>25</v>
+        <v>571</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (25, '2', 'funcId',25);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (571, '2', 'funcId',571);</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>415</v>
@@ -15729,14 +15767,14 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="4">
-        <v>26</v>
+        <v>572</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (26, '2', 'funcId',26);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (572, '2', 'funcId',572);</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>415</v>
@@ -15747,14 +15785,14 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="4">
-        <v>27</v>
+        <v>573</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (27, '2', 'funcId',27);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (573, '2', 'funcId',573);</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>415</v>
@@ -15765,14 +15803,14 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="4">
-        <v>28</v>
+        <v>574</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (28, '2', 'funcId',28);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (574, '2', 'funcId',574);</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>415</v>
@@ -15783,14 +15821,14 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="4">
-        <v>29</v>
+        <v>575</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (29, '2', 'funcId',29);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (575, '2', 'funcId',575);</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>415</v>
@@ -15801,14 +15839,14 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="4">
-        <v>30</v>
+        <v>576</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (30, '2', 'funcId',30);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (576, '2', 'funcId',576);</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>415</v>
@@ -15819,14 +15857,14 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="4">
-        <v>31</v>
+        <v>577</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (31, '2', 'funcId',31);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (577, '2', 'funcId',577);</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>415</v>
@@ -15837,14 +15875,14 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="4">
-        <v>32</v>
+        <v>578</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (32, '2', 'funcId',32);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (578, '2', 'funcId',578);</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>415</v>
@@ -15855,14 +15893,14 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="4">
-        <v>33</v>
+        <v>579</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (33, '2', 'funcId',33);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (579, '2', 'funcId',579);</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>415</v>
@@ -15873,14 +15911,14 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="4">
-        <v>34</v>
+        <v>580</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (34, '2', 'funcId',34);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (580, '2', 'funcId',580);</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>415</v>
@@ -15891,14 +15929,14 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="4">
-        <v>35</v>
+        <v>581</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (35, '2', 'funcId',35);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (581, '2', 'funcId',581);</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>415</v>
@@ -15909,14 +15947,14 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="4">
-        <v>36</v>
+        <v>582</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (36, '2', 'funcId',36);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (582, '2', 'funcId',582);</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>415</v>
@@ -15927,14 +15965,14 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="4">
-        <v>37</v>
+        <v>583</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (37, '2', 'funcId',37);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (583, '2', 'funcId',583);</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>415</v>
@@ -15945,14 +15983,14 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="4">
-        <v>38</v>
+        <v>584</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (38, '2', 'funcId',38);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (584, '2', 'funcId',584);</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>415</v>
@@ -15963,14 +16001,14 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="4">
-        <v>39</v>
+        <v>585</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (39, '2', 'funcId',39);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (585, '2', 'funcId',585);</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>415</v>
@@ -15981,14 +16019,14 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="4">
-        <v>40</v>
+        <v>586</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (40, '2', 'funcId',40);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (586, '2', 'funcId',586);</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>415</v>
@@ -15999,14 +16037,14 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="4">
-        <v>41</v>
+        <v>587</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (41, '2', 'funcId',41);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (587, '2', 'funcId',587);</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>415</v>
@@ -16017,14 +16055,14 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="4">
-        <v>42</v>
+        <v>588</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (42, '2', 'funcId',42);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (588, '2', 'funcId',588);</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>415</v>
@@ -16035,14 +16073,14 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="4">
-        <v>43</v>
+        <v>589</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (43, '2', 'funcId',43);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (589, '2', 'funcId',589);</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>415</v>
@@ -16053,14 +16091,14 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="4">
-        <v>44</v>
+        <v>590</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (44, '2', 'funcId',44);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (590, '2', 'funcId',590);</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>415</v>
@@ -16071,14 +16109,14 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="4">
-        <v>45</v>
+        <v>591</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (45, '2', 'funcId',45);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (591, '2', 'funcId',591);</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>415</v>
@@ -16089,14 +16127,14 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="4">
-        <v>46</v>
+        <v>592</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (46, '2', 'funcId',46);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (592, '2', 'funcId',592);</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>415</v>
@@ -16107,14 +16145,14 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="4">
-        <v>47</v>
+        <v>593</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (47, '2', 'funcId',47);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (593, '2', 'funcId',593);</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>415</v>
@@ -16125,14 +16163,14 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="4">
-        <v>48</v>
+        <v>594</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (48, '2', 'funcId',48);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (594, '2', 'funcId',594);</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>415</v>
@@ -16143,14 +16181,14 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="4">
-        <v>49</v>
+        <v>595</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (49, '2', 'funcId',49);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (595, '2', 'funcId',595);</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>415</v>
@@ -16161,14 +16199,14 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="4">
-        <v>50</v>
+        <v>596</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (50, '2', 'funcId',50);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (596, '2', 'funcId',596);</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>415</v>
@@ -16179,14 +16217,14 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="4">
-        <v>51</v>
+        <v>597</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (51, '2', 'funcId',51);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (597, '2', 'funcId',597);</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>415</v>
@@ -16197,14 +16235,14 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="4">
-        <v>52</v>
+        <v>598</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (52, '2', 'funcId',52);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (598, '2', 'funcId',598);</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>415</v>
@@ -16215,14 +16253,14 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="4">
-        <v>53</v>
+        <v>599</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (53, '2', 'funcId',53);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (599, '2', 'funcId',599);</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>415</v>
@@ -16233,14 +16271,14 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="4">
-        <v>54</v>
+        <v>600</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (54, '2', 'funcId',54);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (600, '2', 'funcId',600);</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>415</v>
@@ -16251,14 +16289,14 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="4">
-        <v>55</v>
+        <v>601</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (55, '2', 'funcId',55);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (601, '2', 'funcId',601);</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>415</v>
@@ -16269,14 +16307,14 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="4">
-        <v>56</v>
+        <v>602</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (56, '2', 'funcId',56);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (602, '2', 'funcId',602);</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>415</v>
@@ -16287,14 +16325,14 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="4">
-        <v>57</v>
+        <v>603</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (57, '2', 'funcId',57);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (603, '2', 'funcId',603);</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>415</v>
@@ -16305,14 +16343,14 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="4">
-        <v>58</v>
+        <v>604</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (58, '2', 'funcId',58);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (604, '2', 'funcId',604);</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>415</v>
@@ -16323,14 +16361,14 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="4">
-        <v>59</v>
+        <v>605</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (59, '2', 'funcId',59);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (605, '2', 'funcId',605);</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>415</v>
@@ -16341,14 +16379,14 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="4">
-        <v>60</v>
+        <v>606</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (60, '2', 'funcId',60);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (606, '2', 'funcId',606);</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>415</v>
@@ -16359,14 +16397,14 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="4">
-        <v>61</v>
+        <v>607</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (61, '2', 'funcId',61);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (607, '2', 'funcId',607);</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>415</v>
@@ -16377,14 +16415,14 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="4">
-        <v>62</v>
+        <v>608</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (62, '2', 'funcId',62);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (608, '2', 'funcId',608);</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>415</v>
@@ -16395,14 +16433,14 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="4">
-        <v>63</v>
+        <v>609</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (63, '2', 'funcId',63);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (609, '2', 'funcId',609);</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>415</v>
@@ -16413,14 +16451,14 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="4">
-        <v>64</v>
+        <v>610</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (64, '2', 'funcId',64);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (610, '2', 'funcId',610);</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>415</v>
@@ -16431,14 +16469,14 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="4">
-        <v>65</v>
+        <v>611</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" ref="C66:C129" si="1">B66&amp;""&amp;A66&amp;D66&amp;A66&amp;E66</f>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (65, '2', 'funcId',65);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (611, '2', 'funcId',611);</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>415</v>
@@ -16449,14 +16487,14 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="4">
-        <v>66</v>
+        <v>612</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (66, '2', 'funcId',66);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (612, '2', 'funcId',612);</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>415</v>
@@ -16467,14 +16505,14 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="4">
-        <v>67</v>
+        <v>613</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (67, '2', 'funcId',67);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (613, '2', 'funcId',613);</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>415</v>
@@ -16485,14 +16523,14 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="4">
-        <v>68</v>
+        <v>614</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (68, '2', 'funcId',68);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (614, '2', 'funcId',614);</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>415</v>
@@ -16503,14 +16541,14 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="4">
-        <v>69</v>
+        <v>615</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (69, '2', 'funcId',69);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (615, '2', 'funcId',615);</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>415</v>
@@ -16521,14 +16559,14 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="4">
-        <v>70</v>
+        <v>616</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (70, '2', 'funcId',70);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (616, '2', 'funcId',616);</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>415</v>
@@ -16539,14 +16577,14 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="4">
-        <v>71</v>
+        <v>617</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (71, '2', 'funcId',71);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (617, '2', 'funcId',617);</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>415</v>
@@ -16557,14 +16595,14 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="4">
-        <v>72</v>
+        <v>618</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (72, '2', 'funcId',72);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (618, '2', 'funcId',618);</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>415</v>
@@ -16575,14 +16613,14 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="4">
-        <v>73</v>
+        <v>619</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (73, '2', 'funcId',73);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (619, '2', 'funcId',619);</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>415</v>
@@ -16593,14 +16631,14 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="4">
-        <v>74</v>
+        <v>620</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (74, '2', 'funcId',74);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (620, '2', 'funcId',620);</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>415</v>
@@ -16611,14 +16649,14 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="4">
-        <v>75</v>
+        <v>621</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (75, '2', 'funcId',75);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (621, '2', 'funcId',621);</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>415</v>
@@ -16629,14 +16667,14 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="4">
-        <v>76</v>
+        <v>622</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (76, '2', 'funcId',76);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (622, '2', 'funcId',622);</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>415</v>
@@ -16647,14 +16685,14 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="4">
-        <v>77</v>
+        <v>623</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (77, '2', 'funcId',77);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (623, '2', 'funcId',623);</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>415</v>
@@ -16665,14 +16703,14 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="4">
-        <v>78</v>
+        <v>624</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (78, '2', 'funcId',78);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (624, '2', 'funcId',624);</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>415</v>
@@ -16683,14 +16721,14 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="4">
-        <v>79</v>
+        <v>625</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (79, '2', 'funcId',79);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (625, '2', 'funcId',625);</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>415</v>
@@ -16701,14 +16739,14 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="4">
-        <v>80</v>
+        <v>626</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (80, '2', 'funcId',80);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (626, '2', 'funcId',626);</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>415</v>
@@ -16719,14 +16757,14 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="4">
-        <v>81</v>
+        <v>627</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (81, '2', 'funcId',81);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (627, '2', 'funcId',627);</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>415</v>
@@ -16737,14 +16775,14 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="4">
-        <v>82</v>
+        <v>628</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (82, '2', 'funcId',82);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (628, '2', 'funcId',628);</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>415</v>
@@ -16755,14 +16793,14 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="4">
-        <v>83</v>
+        <v>629</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (83, '2', 'funcId',83);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (629, '2', 'funcId',629);</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>415</v>
@@ -16773,14 +16811,14 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="4">
-        <v>84</v>
+        <v>630</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (84, '2', 'funcId',84);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (630, '2', 'funcId',630);</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>415</v>
@@ -16791,14 +16829,14 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="4">
-        <v>85</v>
+        <v>631</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (85, '2', 'funcId',85);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (631, '2', 'funcId',631);</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>415</v>
@@ -16809,14 +16847,14 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="4">
-        <v>86</v>
+        <v>632</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (86, '2', 'funcId',86);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (632, '2', 'funcId',632);</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>415</v>
@@ -16827,14 +16865,14 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="4">
-        <v>87</v>
+        <v>633</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C88" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (87, '2', 'funcId',87);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (633, '2', 'funcId',633);</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>415</v>
@@ -16845,14 +16883,14 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="4">
-        <v>88</v>
+        <v>634</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (88, '2', 'funcId',88);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (634, '2', 'funcId',634);</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>415</v>
@@ -16863,14 +16901,14 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="4">
-        <v>89</v>
+        <v>635</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (89, '2', 'funcId',89);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (635, '2', 'funcId',635);</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>415</v>
@@ -16881,14 +16919,14 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="4">
-        <v>90</v>
+        <v>636</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (90, '2', 'funcId',90);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (636, '2', 'funcId',636);</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>415</v>
@@ -16899,14 +16937,14 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="4">
-        <v>91</v>
+        <v>637</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (91, '2', 'funcId',91);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (637, '2', 'funcId',637);</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>415</v>
@@ -16917,14 +16955,14 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="4">
-        <v>92</v>
+        <v>638</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (92, '2', 'funcId',92);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (638, '2', 'funcId',638);</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>415</v>
@@ -16935,14 +16973,14 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="4">
-        <v>93</v>
+        <v>639</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (93, '2', 'funcId',93);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (639, '2', 'funcId',639);</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>415</v>
@@ -16953,14 +16991,14 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="4">
-        <v>94</v>
+        <v>640</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (94, '2', 'funcId',94);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (640, '2', 'funcId',640);</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>415</v>
@@ -16971,14 +17009,14 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="4">
-        <v>95</v>
+        <v>641</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (95, '2', 'funcId',95);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (641, '2', 'funcId',641);</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>415</v>
@@ -16989,14 +17027,14 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="4">
-        <v>96</v>
+        <v>642</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (96, '2', 'funcId',96);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (642, '2', 'funcId',642);</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>415</v>
@@ -17007,14 +17045,14 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="4">
-        <v>97</v>
+        <v>643</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (97, '2', 'funcId',97);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (643, '2', 'funcId',643);</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>415</v>
@@ -17025,14 +17063,14 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4">
-        <v>98</v>
+        <v>644</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (98, '2', 'funcId',98);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (644, '2', 'funcId',644);</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>415</v>
@@ -17043,14 +17081,14 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="4">
-        <v>99</v>
+        <v>645</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (99, '2', 'funcId',99);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (645, '2', 'funcId',645);</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>415</v>
@@ -17061,14 +17099,14 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="4">
-        <v>100</v>
+        <v>646</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (100, '2', 'funcId',100);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (646, '2', 'funcId',646);</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>415</v>
@@ -17079,14 +17117,14 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="4">
-        <v>101</v>
+        <v>647</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (101, '2', 'funcId',101);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (647, '2', 'funcId',647);</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>415</v>
@@ -17097,14 +17135,14 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="4">
-        <v>102</v>
+        <v>648</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (102, '2', 'funcId',102);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (648, '2', 'funcId',648);</v>
       </c>
       <c r="D103" s="4" t="s">
         <v>415</v>
@@ -17115,14 +17153,14 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="4">
-        <v>103</v>
+        <v>649</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (103, '2', 'funcId',103);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (649, '2', 'funcId',649);</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>415</v>
@@ -17133,14 +17171,14 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="4">
-        <v>104</v>
+        <v>650</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (104, '2', 'funcId',104);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (650, '2', 'funcId',650);</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>415</v>
@@ -17151,14 +17189,14 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="4">
-        <v>105</v>
+        <v>651</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (105, '2', 'funcId',105);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (651, '2', 'funcId',651);</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>415</v>
@@ -17169,14 +17207,14 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="4">
-        <v>106</v>
+        <v>652</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (106, '2', 'funcId',106);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (652, '2', 'funcId',652);</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>415</v>
@@ -17187,14 +17225,14 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4">
-        <v>107</v>
+        <v>653</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C108" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (107, '2', 'funcId',107);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (653, '2', 'funcId',653);</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>415</v>
@@ -17205,14 +17243,14 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="4">
-        <v>108</v>
+        <v>654</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C109" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (108, '2', 'funcId',108);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (654, '2', 'funcId',654);</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>415</v>
@@ -17223,14 +17261,14 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="4">
-        <v>109</v>
+        <v>655</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C110" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (109, '2', 'funcId',109);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (655, '2', 'funcId',655);</v>
       </c>
       <c r="D110" s="4" t="s">
         <v>415</v>
@@ -17241,14 +17279,14 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="4">
-        <v>110</v>
+        <v>656</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C111" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (110, '2', 'funcId',110);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (656, '2', 'funcId',656);</v>
       </c>
       <c r="D111" s="4" t="s">
         <v>415</v>
@@ -17259,14 +17297,14 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="4">
-        <v>111</v>
+        <v>657</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C112" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (111, '2', 'funcId',111);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (657, '2', 'funcId',657);</v>
       </c>
       <c r="D112" s="4" t="s">
         <v>415</v>
@@ -17277,14 +17315,14 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4">
-        <v>112</v>
+        <v>658</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C113" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (112, '2', 'funcId',112);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (658, '2', 'funcId',658);</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>415</v>
@@ -17295,14 +17333,14 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="4">
-        <v>113</v>
+        <v>659</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C114" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (113, '2', 'funcId',113);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (659, '2', 'funcId',659);</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>415</v>
@@ -17313,14 +17351,14 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="4">
-        <v>114</v>
+        <v>660</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C115" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (114, '2', 'funcId',114);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (660, '2', 'funcId',660);</v>
       </c>
       <c r="D115" s="4" t="s">
         <v>415</v>
@@ -17331,14 +17369,14 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="4">
-        <v>115</v>
+        <v>661</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C116" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (115, '2', 'funcId',115);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (661, '2', 'funcId',661);</v>
       </c>
       <c r="D116" s="4" t="s">
         <v>415</v>
@@ -17349,14 +17387,14 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="4">
-        <v>116</v>
+        <v>662</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C117" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (116, '2', 'funcId',116);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (662, '2', 'funcId',662);</v>
       </c>
       <c r="D117" s="4" t="s">
         <v>415</v>
@@ -17367,14 +17405,14 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="4">
-        <v>117</v>
+        <v>663</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C118" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (117, '2', 'funcId',117);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (663, '2', 'funcId',663);</v>
       </c>
       <c r="D118" s="4" t="s">
         <v>415</v>
@@ -17385,14 +17423,14 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="4">
-        <v>118</v>
+        <v>664</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C119" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (118, '2', 'funcId',118);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (664, '2', 'funcId',664);</v>
       </c>
       <c r="D119" s="4" t="s">
         <v>415</v>
@@ -17403,14 +17441,14 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="4">
-        <v>119</v>
+        <v>665</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C120" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (119, '2', 'funcId',119);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (665, '2', 'funcId',665);</v>
       </c>
       <c r="D120" s="4" t="s">
         <v>415</v>
@@ -17421,14 +17459,14 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="4">
-        <v>120</v>
+        <v>666</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C121" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (120, '2', 'funcId',120);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (666, '2', 'funcId',666);</v>
       </c>
       <c r="D121" s="4" t="s">
         <v>415</v>
@@ -17439,14 +17477,14 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4">
-        <v>121</v>
+        <v>667</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C122" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (121, '2', 'funcId',121);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (667, '2', 'funcId',667);</v>
       </c>
       <c r="D122" s="4" t="s">
         <v>415</v>
@@ -17457,14 +17495,14 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="4">
-        <v>122</v>
+        <v>668</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C123" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (122, '2', 'funcId',122);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (668, '2', 'funcId',668);</v>
       </c>
       <c r="D123" s="4" t="s">
         <v>415</v>
@@ -17475,14 +17513,14 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="4">
-        <v>123</v>
+        <v>669</v>
       </c>
       <c r="B124" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C124" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (123, '2', 'funcId',123);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (669, '2', 'funcId',669);</v>
       </c>
       <c r="D124" s="4" t="s">
         <v>415</v>
@@ -17493,14 +17531,14 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="4">
-        <v>124</v>
+        <v>670</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C125" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (124, '2', 'funcId',124);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (670, '2', 'funcId',670);</v>
       </c>
       <c r="D125" s="4" t="s">
         <v>415</v>
@@ -17511,14 +17549,14 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="4">
-        <v>125</v>
+        <v>671</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C126" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (125, '2', 'funcId',125);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (671, '2', 'funcId',671);</v>
       </c>
       <c r="D126" s="4" t="s">
         <v>415</v>
@@ -17529,14 +17567,14 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="4">
-        <v>126</v>
+        <v>672</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C127" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (126, '2', 'funcId',126);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (672, '2', 'funcId',672);</v>
       </c>
       <c r="D127" s="4" t="s">
         <v>415</v>
@@ -17547,14 +17585,14 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="4">
-        <v>127</v>
+        <v>673</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C128" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (127, '2', 'funcId',127);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (673, '2', 'funcId',673);</v>
       </c>
       <c r="D128" s="4" t="s">
         <v>415</v>
@@ -17565,14 +17603,14 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="4">
-        <v>128</v>
+        <v>674</v>
       </c>
       <c r="B129" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C129" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (128, '2', 'funcId',128);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (674, '2', 'funcId',674);</v>
       </c>
       <c r="D129" s="4" t="s">
         <v>415</v>
@@ -17583,14 +17621,14 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4">
-        <v>129</v>
+        <v>675</v>
       </c>
       <c r="B130" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C130" t="str">
         <f t="shared" ref="C130:C181" si="2">B130&amp;""&amp;A130&amp;D130&amp;A130&amp;E130</f>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (129, '2', 'funcId',129);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (675, '2', 'funcId',675);</v>
       </c>
       <c r="D130" s="4" t="s">
         <v>415</v>
@@ -17601,14 +17639,14 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="4">
-        <v>130</v>
+        <v>676</v>
       </c>
       <c r="B131" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C131" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (130, '2', 'funcId',130);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (676, '2', 'funcId',676);</v>
       </c>
       <c r="D131" s="4" t="s">
         <v>415</v>
@@ -17619,14 +17657,14 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="4">
-        <v>131</v>
+        <v>677</v>
       </c>
       <c r="B132" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C132" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (131, '2', 'funcId',131);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (677, '2', 'funcId',677);</v>
       </c>
       <c r="D132" s="4" t="s">
         <v>415</v>
@@ -17637,14 +17675,14 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="4">
-        <v>132</v>
+        <v>678</v>
       </c>
       <c r="B133" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C133" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (132, '2', 'funcId',132);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (678, '2', 'funcId',678);</v>
       </c>
       <c r="D133" s="4" t="s">
         <v>415</v>
@@ -17655,14 +17693,14 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="4">
-        <v>133</v>
+        <v>679</v>
       </c>
       <c r="B134" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C134" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (133, '2', 'funcId',133);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (679, '2', 'funcId',679);</v>
       </c>
       <c r="D134" s="4" t="s">
         <v>415</v>
@@ -17673,14 +17711,14 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="4">
-        <v>134</v>
+        <v>680</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C135" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (134, '2', 'funcId',134);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (680, '2', 'funcId',680);</v>
       </c>
       <c r="D135" s="4" t="s">
         <v>415</v>
@@ -17691,14 +17729,14 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="4">
-        <v>135</v>
+        <v>681</v>
       </c>
       <c r="B136" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C136" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (135, '2', 'funcId',135);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (681, '2', 'funcId',681);</v>
       </c>
       <c r="D136" s="4" t="s">
         <v>415</v>
@@ -17709,14 +17747,14 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="4">
-        <v>136</v>
+        <v>682</v>
       </c>
       <c r="B137" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C137" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (136, '2', 'funcId',136);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (682, '2', 'funcId',682);</v>
       </c>
       <c r="D137" s="4" t="s">
         <v>415</v>
@@ -17727,14 +17765,14 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="4">
-        <v>137</v>
+        <v>683</v>
       </c>
       <c r="B138" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C138" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (137, '2', 'funcId',137);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (683, '2', 'funcId',683);</v>
       </c>
       <c r="D138" s="4" t="s">
         <v>415</v>
@@ -17745,14 +17783,14 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="4">
-        <v>138</v>
+        <v>684</v>
       </c>
       <c r="B139" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C139" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (138, '2', 'funcId',138);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (684, '2', 'funcId',684);</v>
       </c>
       <c r="D139" s="4" t="s">
         <v>415</v>
@@ -17763,14 +17801,14 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="4">
-        <v>139</v>
+        <v>685</v>
       </c>
       <c r="B140" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C140" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (139, '2', 'funcId',139);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (685, '2', 'funcId',685);</v>
       </c>
       <c r="D140" s="4" t="s">
         <v>415</v>
@@ -17781,14 +17819,14 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="4">
-        <v>140</v>
+        <v>686</v>
       </c>
       <c r="B141" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C141" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (140, '2', 'funcId',140);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (686, '2', 'funcId',686);</v>
       </c>
       <c r="D141" s="4" t="s">
         <v>415</v>
@@ -17799,14 +17837,14 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="4">
-        <v>141</v>
+        <v>687</v>
       </c>
       <c r="B142" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C142" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (141, '2', 'funcId',141);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (687, '2', 'funcId',687);</v>
       </c>
       <c r="D142" s="4" t="s">
         <v>415</v>
@@ -17817,14 +17855,14 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="4">
-        <v>142</v>
+        <v>688</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C143" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (142, '2', 'funcId',142);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (688, '2', 'funcId',688);</v>
       </c>
       <c r="D143" s="4" t="s">
         <v>415</v>
@@ -17835,14 +17873,14 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4">
-        <v>143</v>
+        <v>689</v>
       </c>
       <c r="B144" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C144" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (143, '2', 'funcId',143);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (689, '2', 'funcId',689);</v>
       </c>
       <c r="D144" s="4" t="s">
         <v>415</v>
@@ -17853,14 +17891,14 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="4">
-        <v>144</v>
+        <v>690</v>
       </c>
       <c r="B145" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C145" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (144, '2', 'funcId',144);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (690, '2', 'funcId',690);</v>
       </c>
       <c r="D145" s="4" t="s">
         <v>415</v>
@@ -17871,14 +17909,14 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="4">
-        <v>145</v>
+        <v>691</v>
       </c>
       <c r="B146" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C146" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (145, '2', 'funcId',145);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (691, '2', 'funcId',691);</v>
       </c>
       <c r="D146" s="4" t="s">
         <v>415</v>
@@ -17889,14 +17927,14 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="4">
-        <v>146</v>
+        <v>692</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C147" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (146, '2', 'funcId',146);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (692, '2', 'funcId',692);</v>
       </c>
       <c r="D147" s="4" t="s">
         <v>415</v>
@@ -17907,14 +17945,14 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="4">
-        <v>147</v>
+        <v>693</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C148" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (147, '2', 'funcId',147);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (693, '2', 'funcId',693);</v>
       </c>
       <c r="D148" s="4" t="s">
         <v>415</v>
@@ -17925,14 +17963,14 @@
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="4">
-        <v>148</v>
+        <v>694</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C149" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (148, '2', 'funcId',148);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (694, '2', 'funcId',694);</v>
       </c>
       <c r="D149" s="4" t="s">
         <v>415</v>
@@ -17943,14 +17981,14 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="4">
-        <v>149</v>
+        <v>695</v>
       </c>
       <c r="B150" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C150" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (149, '2', 'funcId',149);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (695, '2', 'funcId',695);</v>
       </c>
       <c r="D150" s="4" t="s">
         <v>415</v>
@@ -17961,14 +17999,14 @@
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="4">
-        <v>150</v>
+        <v>696</v>
       </c>
       <c r="B151" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C151" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (150, '2', 'funcId',150);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (696, '2', 'funcId',696);</v>
       </c>
       <c r="D151" s="4" t="s">
         <v>415</v>
@@ -17979,14 +18017,14 @@
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="4">
-        <v>151</v>
+        <v>697</v>
       </c>
       <c r="B152" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C152" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (151, '2', 'funcId',151);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (697, '2', 'funcId',697);</v>
       </c>
       <c r="D152" s="4" t="s">
         <v>415</v>
@@ -17997,14 +18035,14 @@
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="4">
-        <v>152</v>
+        <v>698</v>
       </c>
       <c r="B153" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C153" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (152, '2', 'funcId',152);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (698, '2', 'funcId',698);</v>
       </c>
       <c r="D153" s="4" t="s">
         <v>415</v>
@@ -18015,14 +18053,14 @@
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="4">
-        <v>153</v>
+        <v>699</v>
       </c>
       <c r="B154" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C154" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (153, '2', 'funcId',153);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (699, '2', 'funcId',699);</v>
       </c>
       <c r="D154" s="4" t="s">
         <v>415</v>
@@ -18033,14 +18071,14 @@
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="4">
-        <v>154</v>
+        <v>700</v>
       </c>
       <c r="B155" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C155" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (154, '2', 'funcId',154);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (700, '2', 'funcId',700);</v>
       </c>
       <c r="D155" s="4" t="s">
         <v>415</v>
@@ -18051,14 +18089,14 @@
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="4">
-        <v>155</v>
+        <v>701</v>
       </c>
       <c r="B156" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C156" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (155, '2', 'funcId',155);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (701, '2', 'funcId',701);</v>
       </c>
       <c r="D156" s="4" t="s">
         <v>415</v>
@@ -18069,14 +18107,14 @@
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="4">
-        <v>156</v>
+        <v>702</v>
       </c>
       <c r="B157" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C157" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (156, '2', 'funcId',156);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (702, '2', 'funcId',702);</v>
       </c>
       <c r="D157" s="4" t="s">
         <v>415</v>
@@ -18087,14 +18125,14 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="4">
-        <v>157</v>
+        <v>703</v>
       </c>
       <c r="B158" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C158" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (157, '2', 'funcId',157);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (703, '2', 'funcId',703);</v>
       </c>
       <c r="D158" s="4" t="s">
         <v>415</v>
@@ -18105,14 +18143,14 @@
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="4">
-        <v>158</v>
+        <v>704</v>
       </c>
       <c r="B159" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C159" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (158, '2', 'funcId',158);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (704, '2', 'funcId',704);</v>
       </c>
       <c r="D159" s="4" t="s">
         <v>415</v>
@@ -18123,14 +18161,14 @@
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="4">
-        <v>159</v>
+        <v>705</v>
       </c>
       <c r="B160" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C160" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (159, '2', 'funcId',159);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (705, '2', 'funcId',705);</v>
       </c>
       <c r="D160" s="4" t="s">
         <v>415</v>
@@ -18141,14 +18179,14 @@
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="4">
-        <v>160</v>
+        <v>706</v>
       </c>
       <c r="B161" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C161" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (160, '2', 'funcId',160);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (706, '2', 'funcId',706);</v>
       </c>
       <c r="D161" s="4" t="s">
         <v>415</v>
@@ -18159,14 +18197,14 @@
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="4">
-        <v>161</v>
+        <v>707</v>
       </c>
       <c r="B162" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C162" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (161, '2', 'funcId',161);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (707, '2', 'funcId',707);</v>
       </c>
       <c r="D162" s="4" t="s">
         <v>415</v>
@@ -18177,14 +18215,14 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="4">
-        <v>162</v>
+        <v>708</v>
       </c>
       <c r="B163" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C163" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (162, '2', 'funcId',162);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (708, '2', 'funcId',708);</v>
       </c>
       <c r="D163" s="4" t="s">
         <v>415</v>
@@ -18195,14 +18233,14 @@
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="4">
-        <v>163</v>
+        <v>709</v>
       </c>
       <c r="B164" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C164" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (163, '2', 'funcId',163);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (709, '2', 'funcId',709);</v>
       </c>
       <c r="D164" s="4" t="s">
         <v>415</v>
@@ -18213,14 +18251,14 @@
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="4">
-        <v>164</v>
+        <v>710</v>
       </c>
       <c r="B165" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C165" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (164, '2', 'funcId',164);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (710, '2', 'funcId',710);</v>
       </c>
       <c r="D165" s="4" t="s">
         <v>415</v>
@@ -18231,14 +18269,14 @@
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="4">
-        <v>165</v>
+        <v>711</v>
       </c>
       <c r="B166" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C166" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (165, '2', 'funcId',165);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (711, '2', 'funcId',711);</v>
       </c>
       <c r="D166" s="4" t="s">
         <v>415</v>
@@ -18249,14 +18287,14 @@
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="4">
-        <v>166</v>
+        <v>712</v>
       </c>
       <c r="B167" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C167" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (166, '2', 'funcId',166);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (712, '2', 'funcId',712);</v>
       </c>
       <c r="D167" s="4" t="s">
         <v>415</v>
@@ -18267,14 +18305,14 @@
     </row>
     <row r="168" spans="1:5">
       <c r="A168" s="4">
-        <v>167</v>
+        <v>713</v>
       </c>
       <c r="B168" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C168" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (167, '2', 'funcId',167);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (713, '2', 'funcId',713);</v>
       </c>
       <c r="D168" s="4" t="s">
         <v>415</v>
@@ -18285,14 +18323,14 @@
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="4">
-        <v>168</v>
+        <v>714</v>
       </c>
       <c r="B169" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C169" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (168, '2', 'funcId',168);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (714, '2', 'funcId',714);</v>
       </c>
       <c r="D169" s="4" t="s">
         <v>415</v>
@@ -18303,14 +18341,14 @@
     </row>
     <row r="170" spans="1:5">
       <c r="A170" s="4">
-        <v>169</v>
+        <v>715</v>
       </c>
       <c r="B170" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C170" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (169, '2', 'funcId',169);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (715, '2', 'funcId',715);</v>
       </c>
       <c r="D170" s="4" t="s">
         <v>415</v>
@@ -18321,14 +18359,14 @@
     </row>
     <row r="171" spans="1:5">
       <c r="A171" s="4">
-        <v>170</v>
+        <v>716</v>
       </c>
       <c r="B171" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C171" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (170, '2', 'funcId',170);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (716, '2', 'funcId',716);</v>
       </c>
       <c r="D171" s="4" t="s">
         <v>415</v>
@@ -18339,14 +18377,14 @@
     </row>
     <row r="172" spans="1:5">
       <c r="A172" s="4">
-        <v>171</v>
+        <v>717</v>
       </c>
       <c r="B172" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C172" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (171, '2', 'funcId',171);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (717, '2', 'funcId',717);</v>
       </c>
       <c r="D172" s="4" t="s">
         <v>415</v>
@@ -18357,14 +18395,14 @@
     </row>
     <row r="173" spans="1:5">
       <c r="A173" s="4">
-        <v>172</v>
+        <v>718</v>
       </c>
       <c r="B173" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C173" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (172, '2', 'funcId',172);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (718, '2', 'funcId',718);</v>
       </c>
       <c r="D173" s="4" t="s">
         <v>415</v>
@@ -18375,14 +18413,14 @@
     </row>
     <row r="174" spans="1:5">
       <c r="A174" s="4">
-        <v>173</v>
+        <v>719</v>
       </c>
       <c r="B174" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C174" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (173, '2', 'funcId',173);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (719, '2', 'funcId',719);</v>
       </c>
       <c r="D174" s="4" t="s">
         <v>415</v>
@@ -18393,14 +18431,14 @@
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="4">
-        <v>174</v>
+        <v>720</v>
       </c>
       <c r="B175" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C175" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (174, '2', 'funcId',174);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (720, '2', 'funcId',720);</v>
       </c>
       <c r="D175" s="4" t="s">
         <v>415</v>
@@ -18411,14 +18449,14 @@
     </row>
     <row r="176" spans="1:5">
       <c r="A176" s="4">
-        <v>175</v>
+        <v>721</v>
       </c>
       <c r="B176" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C176" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (175, '2', 'funcId',175);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (721, '2', 'funcId',721);</v>
       </c>
       <c r="D176" s="4" t="s">
         <v>415</v>
@@ -18429,14 +18467,14 @@
     </row>
     <row r="177" spans="1:5">
       <c r="A177" s="4">
-        <v>176</v>
+        <v>722</v>
       </c>
       <c r="B177" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C177" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (176, '2', 'funcId',176);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (722, '2', 'funcId',722);</v>
       </c>
       <c r="D177" s="4" t="s">
         <v>415</v>
@@ -18447,14 +18485,14 @@
     </row>
     <row r="178" spans="1:5">
       <c r="A178" s="4">
-        <v>177</v>
+        <v>723</v>
       </c>
       <c r="B178" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C178" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (177, '2', 'funcId',177);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (723, '2', 'funcId',723);</v>
       </c>
       <c r="D178" s="4" t="s">
         <v>415</v>
@@ -18465,14 +18503,14 @@
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="4">
-        <v>178</v>
+        <v>724</v>
       </c>
       <c r="B179" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C179" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (178, '2', 'funcId',178);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (724, '2', 'funcId',724);</v>
       </c>
       <c r="D179" s="4" t="s">
         <v>415</v>
@@ -18483,14 +18521,14 @@
     </row>
     <row r="180" spans="1:5">
       <c r="A180" s="4">
-        <v>179</v>
+        <v>725</v>
       </c>
       <c r="B180" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C180" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (179, '2', 'funcId',179);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (725, '2', 'funcId',725);</v>
       </c>
       <c r="D180" s="4" t="s">
         <v>415</v>
@@ -18501,14 +18539,14 @@
     </row>
     <row r="181" spans="1:5">
       <c r="A181" s="4">
-        <v>180</v>
+        <v>726</v>
       </c>
       <c r="B181" s="4" t="s">
         <v>412</v>
       </c>
       <c r="C181" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO `fine_auth_perm_relation` VALUES (180, '2', 'funcId',180);</v>
+        <v>INSERT INTO `fine_auth_perm_relation` VALUES (726, '2', 'funcId',726);</v>
       </c>
       <c r="D181" s="4" t="s">
         <v>415</v>
@@ -18873,7 +18911,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -28518,7 +28556,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -28923,7 +28961,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -29580,7 +29618,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N28" sqref="A14:N28"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
vault backup: 2022-02-07 12:06:34
Affected files:
.obsidian/plugins/recent-files-obsidian/data.json
.obsidian/workspace
1附件/~$权限列表.xlsx
1附件/权限列表.xlsx
</commit_message>
<xml_diff>
--- a/1附件/权限列表.xlsx
+++ b/1附件/权限列表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanglidong/git/learn/1附件/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B39E204-5899-9D4F-9E6A-A89C64FB44C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FC380C-7881-BD48-9ABF-7215EE519FF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="0" windowWidth="37460" windowHeight="21600" activeTab="4" xr2:uid="{A24D0D43-9B7D-E446-B31E-E18A468734D4}"/>
   </bookViews>
@@ -28644,7 +28644,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -28732,7 +28732,7 @@
         <v>879</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="0"/>
+        <f>LOWER(F4)</f>
         <v>call_the_roll</v>
       </c>
       <c r="H4" t="str">

</xml_diff>